<commit_message>
notas de credito - modelo actualizado
</commit_message>
<xml_diff>
--- a/data/NC_semanal.xlsx
+++ b/data/NC_semanal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Desktop\MetrovaloresApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AE68E3-3261-42F6-A2F3-39BFFC3FC2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B000E28-FFE8-44DA-B6A3-090A2DC2301C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{9E78C8B1-ED59-4A81-8FF9-F1A88ED1C1A0}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,8 +167,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,6 +351,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -465,7 +476,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -508,13 +519,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="18" fillId="33" borderId="0" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -533,6 +545,7 @@
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="ANCLAS,REZONES Y SUS PARTES,DE FUNDICION,DE HIERRO O DE ACERO" xfId="42" xr:uid="{ACDCAF54-3D8B-4FE3-AD59-AA47A11913E9}"/>
     <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
@@ -891,16 +904,16 @@
   <dimension ref="A1:B282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B2" sqref="B2:B282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -908,2251 +921,2251 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1140.92</v>
       </c>
-      <c r="B2" s="1">
-        <v>992000</v>
+      <c r="B2" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>135.96</v>
       </c>
-      <c r="B3" s="1">
-        <v>930000</v>
+      <c r="B3" s="2">
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>128516.33</v>
       </c>
-      <c r="B4" s="1">
-        <v>997600</v>
+      <c r="B4" s="2">
+        <v>99.76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>19510.89</v>
       </c>
-      <c r="B5" s="1">
-        <v>996000</v>
+      <c r="B5" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>19872.64</v>
       </c>
-      <c r="B6" s="1">
-        <v>995500</v>
+      <c r="B6" s="2">
+        <v>99.55</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>196370.73</v>
       </c>
-      <c r="B7" s="1">
-        <v>997600</v>
+      <c r="B7" s="2">
+        <v>99.76</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>220718.91</v>
       </c>
-      <c r="B8" s="1">
-        <v>998000</v>
+      <c r="B8" s="2">
+        <v>99.8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>15970.77</v>
       </c>
-      <c r="B9" s="1">
-        <v>993000</v>
+      <c r="B9" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>143503.24</v>
       </c>
-      <c r="B10" s="1">
-        <v>997600</v>
+      <c r="B10" s="2">
+        <v>99.76</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>37838.129999999997</v>
       </c>
-      <c r="B11" s="1">
-        <v>996500</v>
+      <c r="B11" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>2159.81</v>
       </c>
-      <c r="B12" s="1">
-        <v>993700</v>
+      <c r="B12" s="2">
+        <v>99.37</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>1092.1199999999999</v>
       </c>
-      <c r="B13" s="1">
-        <v>992000</v>
+      <c r="B13" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>2030.94</v>
       </c>
-      <c r="B14" s="1">
-        <v>994000</v>
+      <c r="B14" s="2">
+        <v>99.4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>407.92</v>
       </c>
-      <c r="B15" s="1">
-        <v>960000</v>
+      <c r="B15" s="2">
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>4203.99</v>
       </c>
-      <c r="B16" s="1">
-        <v>994500</v>
+      <c r="B16" s="2">
+        <v>99.45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>1582.39</v>
       </c>
-      <c r="B17" s="1">
-        <v>992000</v>
+      <c r="B17" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>729.88</v>
       </c>
-      <c r="B18" s="1">
-        <v>990000</v>
+      <c r="B18" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>1208.1500000000001</v>
       </c>
-      <c r="B19" s="1">
-        <v>992500</v>
+      <c r="B19" s="2">
+        <v>99.25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>121071.23</v>
       </c>
-      <c r="B20" s="1">
-        <v>997700</v>
+      <c r="B20" s="2">
+        <v>99.77</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>1838.43</v>
       </c>
-      <c r="B21" s="1">
-        <v>992000</v>
+      <c r="B21" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>21138.55</v>
       </c>
-      <c r="B22" s="1">
-        <v>993500</v>
+      <c r="B22" s="2">
+        <v>99.35</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>1678.31</v>
       </c>
-      <c r="B23" s="1">
-        <v>993500</v>
+      <c r="B23" s="2">
+        <v>99.35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>746.67</v>
       </c>
-      <c r="B24" s="1">
-        <v>990000</v>
+      <c r="B24" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>1633</v>
       </c>
-      <c r="B25" s="1">
-        <v>993600</v>
+      <c r="B25" s="2">
+        <v>99.36</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>92712.45</v>
       </c>
-      <c r="B26" s="1">
-        <v>997601</v>
+      <c r="B26" s="2">
+        <v>99.76</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>2826.47</v>
       </c>
-      <c r="B27" s="1">
-        <v>994701</v>
+      <c r="B27" s="2">
+        <v>99.47</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>2604.63</v>
       </c>
-      <c r="B28" s="1">
-        <v>990500</v>
+      <c r="B28" s="2">
+        <v>99.05</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>17874.7</v>
       </c>
-      <c r="B29" s="1">
-        <v>996500</v>
+      <c r="B29" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>7158.8</v>
       </c>
-      <c r="B30" s="1">
-        <v>995650</v>
+      <c r="B30" s="2">
+        <v>99.56</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>23212.28</v>
       </c>
-      <c r="B31" s="1">
-        <v>996500</v>
+      <c r="B31" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>102698.4</v>
       </c>
-      <c r="B32" s="1">
-        <v>997900</v>
+      <c r="B32" s="2">
+        <v>99.79</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>26435.4</v>
       </c>
-      <c r="B33" s="1">
-        <v>992000</v>
+      <c r="B33" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>4501.6899999999996</v>
       </c>
-      <c r="B34" s="1">
-        <v>994000</v>
+      <c r="B34" s="2">
+        <v>99.4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>9254.33</v>
       </c>
-      <c r="B35" s="1">
-        <v>995750</v>
+      <c r="B35" s="2">
+        <v>99.57</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>1730.63</v>
       </c>
-      <c r="B36" s="1">
-        <v>993500</v>
+      <c r="B36" s="2">
+        <v>99.35</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>7198.93</v>
       </c>
-      <c r="B37" s="1">
-        <v>994000</v>
+      <c r="B37" s="2">
+        <v>99.4</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>908.93</v>
       </c>
-      <c r="B38" s="1">
-        <v>992000</v>
+      <c r="B38" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <v>10344.200000000001</v>
       </c>
-      <c r="B39" s="1">
-        <v>996800</v>
+      <c r="B39" s="2">
+        <v>99.68</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>15154.55</v>
       </c>
-      <c r="B40" s="1">
-        <v>995000</v>
+      <c r="B40" s="2">
+        <v>99.5</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="A41" s="1">
         <v>1599.49</v>
       </c>
-      <c r="B41" s="1">
-        <v>993000</v>
+      <c r="B41" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>468343.59</v>
       </c>
-      <c r="B42" s="1">
-        <v>998000</v>
+      <c r="B42" s="2">
+        <v>99.8</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="A43" s="1">
         <v>13339.09</v>
       </c>
-      <c r="B43" s="1">
-        <v>995500</v>
+      <c r="B43" s="2">
+        <v>99.55</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>12118.39</v>
       </c>
-      <c r="B44" s="1">
-        <v>995500</v>
+      <c r="B44" s="2">
+        <v>99.55</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>28384.13</v>
       </c>
-      <c r="B45" s="1">
-        <v>996500</v>
+      <c r="B45" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+      <c r="A46" s="1">
         <v>10996.8</v>
       </c>
-      <c r="B46" s="1">
-        <v>996500</v>
+      <c r="B46" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="A47" s="1">
         <v>400.21</v>
       </c>
-      <c r="B47" s="1">
-        <v>970000</v>
+      <c r="B47" s="2">
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>1614.57</v>
       </c>
-      <c r="B48" s="1">
-        <v>991000</v>
+      <c r="B48" s="2">
+        <v>99.1</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>8290.57</v>
       </c>
-      <c r="B49" s="1">
-        <v>990500</v>
+      <c r="B49" s="2">
+        <v>99.05</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>1977.79</v>
       </c>
-      <c r="B50" s="1">
-        <v>990000</v>
+      <c r="B50" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="A51" s="1">
         <v>669.01</v>
       </c>
-      <c r="B51" s="1">
-        <v>985000</v>
+      <c r="B51" s="2">
+        <v>98.5</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="A52" s="1">
         <v>21656.03</v>
       </c>
-      <c r="B52" s="1">
-        <v>997500</v>
+      <c r="B52" s="2">
+        <v>99.75</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="A53" s="1">
         <v>93116.6</v>
       </c>
-      <c r="B53" s="1">
-        <v>997600</v>
+      <c r="B53" s="2">
+        <v>99.76</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+      <c r="A54" s="1">
         <v>1957.17</v>
       </c>
-      <c r="B54" s="1">
-        <v>992500</v>
+      <c r="B54" s="2">
+        <v>99.25</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+      <c r="A55" s="1">
         <v>12524.24</v>
       </c>
-      <c r="B55" s="1">
-        <v>995000</v>
+      <c r="B55" s="2">
+        <v>99.5</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="A56" s="1">
         <v>10000</v>
       </c>
-      <c r="B56" s="1">
-        <v>996000</v>
+      <c r="B56" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="A57" s="1">
         <v>39527.01</v>
       </c>
-      <c r="B57" s="1">
-        <v>996700</v>
+      <c r="B57" s="2">
+        <v>99.67</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+      <c r="A58" s="1">
         <v>3136.98</v>
       </c>
-      <c r="B58" s="1">
-        <v>993500</v>
+      <c r="B58" s="2">
+        <v>99.35</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
+      <c r="A59" s="1">
         <v>969.95</v>
       </c>
-      <c r="B59" s="1">
-        <v>992000</v>
+      <c r="B59" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
+      <c r="A60" s="1">
         <v>1172.46</v>
       </c>
-      <c r="B60" s="1">
-        <v>992500</v>
+      <c r="B60" s="2">
+        <v>99.25</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
+      <c r="A61" s="1">
         <v>3232.92</v>
       </c>
-      <c r="B61" s="1">
-        <v>993500</v>
+      <c r="B61" s="2">
+        <v>99.35</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
+      <c r="A62" s="1">
         <v>6070.04</v>
       </c>
-      <c r="B62" s="1">
-        <v>994000</v>
+      <c r="B62" s="2">
+        <v>99.4</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+      <c r="A63" s="1">
         <v>10586.42</v>
       </c>
-      <c r="B63" s="1">
-        <v>994000</v>
+      <c r="B63" s="2">
+        <v>99.4</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+      <c r="A64" s="1">
         <v>7921.52</v>
       </c>
-      <c r="B64" s="1">
-        <v>994500</v>
+      <c r="B64" s="2">
+        <v>99.45</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+      <c r="A65" s="1">
         <v>3298.82</v>
       </c>
-      <c r="B65" s="1">
-        <v>992000</v>
+      <c r="B65" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+      <c r="A66" s="1">
         <v>310950.89</v>
       </c>
-      <c r="B66" s="1">
-        <v>997700</v>
+      <c r="B66" s="2">
+        <v>99.77</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="A67" s="1">
         <v>10680.91</v>
       </c>
-      <c r="B67" s="1">
-        <v>995000</v>
+      <c r="B67" s="2">
+        <v>99.5</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+      <c r="A68" s="1">
         <v>289559.96000000002</v>
       </c>
-      <c r="B68" s="1">
-        <v>997200</v>
+      <c r="B68" s="2">
+        <v>99.72</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+      <c r="A69" s="1">
         <v>6653.77</v>
       </c>
-      <c r="B69" s="1">
-        <v>994000</v>
+      <c r="B69" s="2">
+        <v>99.4</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
+      <c r="A70" s="1">
         <v>1559.85</v>
       </c>
-      <c r="B70" s="1">
-        <v>991000</v>
+      <c r="B70" s="2">
+        <v>99.1</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
+      <c r="A71" s="1">
         <v>7988.39</v>
       </c>
-      <c r="B71" s="1">
-        <v>995000</v>
+      <c r="B71" s="2">
+        <v>99.5</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
+      <c r="A72" s="1">
         <v>44956.800000000003</v>
       </c>
-      <c r="B72" s="1">
-        <v>996500</v>
+      <c r="B72" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
+      <c r="A73" s="1">
         <v>361851.73</v>
       </c>
-      <c r="B73" s="1">
-        <v>998100</v>
+      <c r="B73" s="2">
+        <v>99.81</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
+      <c r="A74" s="1">
         <v>39886.6</v>
       </c>
-      <c r="B74" s="1">
-        <v>996750</v>
+      <c r="B74" s="2">
+        <v>99.67</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
+      <c r="A75" s="1">
         <v>93715.28</v>
       </c>
-      <c r="B75" s="1">
-        <v>997600</v>
+      <c r="B75" s="2">
+        <v>99.76</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
+      <c r="A76" s="1">
         <v>9111.18</v>
       </c>
-      <c r="B76" s="1">
-        <v>996000</v>
+      <c r="B76" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+      <c r="A77" s="1">
         <v>3295.46</v>
       </c>
-      <c r="B77" s="1">
-        <v>993000</v>
+      <c r="B77" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
+      <c r="A78" s="1">
         <v>100703.09</v>
       </c>
-      <c r="B78" s="1">
-        <v>997600</v>
+      <c r="B78" s="2">
+        <v>99.76</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+      <c r="A79" s="1">
         <v>153194.67000000001</v>
       </c>
-      <c r="B79" s="1">
-        <v>997600</v>
+      <c r="B79" s="2">
+        <v>99.76</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+      <c r="A80" s="1">
         <v>44552.76</v>
       </c>
-      <c r="B80" s="1">
-        <v>996700</v>
+      <c r="B80" s="2">
+        <v>99.67</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
+      <c r="A81" s="1">
         <v>1139.22</v>
       </c>
-      <c r="B81" s="1">
-        <v>993000</v>
+      <c r="B81" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+      <c r="A82" s="1">
         <v>9354.5499999999993</v>
       </c>
-      <c r="B82" s="1">
-        <v>995900</v>
+      <c r="B82" s="2">
+        <v>99.59</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
+      <c r="A83" s="1">
         <v>30542.51</v>
       </c>
-      <c r="B83" s="1">
-        <v>996000</v>
+      <c r="B83" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+      <c r="A84" s="1">
         <v>1342.4</v>
       </c>
-      <c r="B84" s="1">
-        <v>992500</v>
+      <c r="B84" s="2">
+        <v>99.25</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
+      <c r="A85" s="1">
         <v>106916.71</v>
       </c>
-      <c r="B85" s="1">
-        <v>997500</v>
+      <c r="B85" s="2">
+        <v>99.75</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
+      <c r="A86" s="1">
         <v>36148.730000000003</v>
       </c>
-      <c r="B86" s="1">
-        <v>997000</v>
+      <c r="B86" s="2">
+        <v>99.7</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+      <c r="A87" s="1">
         <v>1548.59</v>
       </c>
-      <c r="B87" s="1">
-        <v>992200</v>
+      <c r="B87" s="2">
+        <v>99.22</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
+      <c r="A88" s="1">
         <v>1097.1500000000001</v>
       </c>
-      <c r="B88" s="1">
-        <v>990000</v>
+      <c r="B88" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
+      <c r="A89" s="1">
         <v>1210.3900000000001</v>
       </c>
-      <c r="B89" s="1">
-        <v>990000</v>
+      <c r="B89" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
+      <c r="A90" s="1">
         <v>1392.34</v>
       </c>
-      <c r="B90" s="1">
-        <v>990000</v>
+      <c r="B90" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
+      <c r="A91" s="1">
         <v>265636.02</v>
       </c>
-      <c r="B91" s="1">
-        <v>997700</v>
+      <c r="B91" s="2">
+        <v>99.77</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+      <c r="A92" s="1">
         <v>2330.15</v>
       </c>
-      <c r="B92" s="1">
-        <v>990000</v>
+      <c r="B92" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
+      <c r="A93" s="1">
         <v>1136.31</v>
       </c>
-      <c r="B93" s="1">
-        <v>993000</v>
+      <c r="B93" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
+      <c r="A94" s="1">
         <v>3209.98</v>
       </c>
-      <c r="B94" s="1">
-        <v>990000</v>
+      <c r="B94" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
+      <c r="A95" s="1">
         <v>3997.6</v>
       </c>
-      <c r="B95" s="1">
-        <v>990000</v>
+      <c r="B95" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+      <c r="A96" s="1">
         <v>15960.72</v>
       </c>
-      <c r="B96" s="1">
-        <v>996210</v>
+      <c r="B96" s="2">
+        <v>99.62</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
+      <c r="A97" s="1">
         <v>12958.81</v>
       </c>
-      <c r="B97" s="1">
-        <v>996350</v>
+      <c r="B97" s="2">
+        <v>99.63</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
+      <c r="A98" s="1">
         <v>381487.86</v>
       </c>
-      <c r="B98" s="1">
-        <v>998000</v>
+      <c r="B98" s="2">
+        <v>99.8</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
+      <c r="A99" s="1">
         <v>1934.71</v>
       </c>
-      <c r="B99" s="1">
-        <v>993010</v>
+      <c r="B99" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
+      <c r="A100" s="1">
         <v>2751.03</v>
       </c>
-      <c r="B100" s="1">
-        <v>993000</v>
+      <c r="B100" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
+      <c r="A101" s="1">
         <v>1001.55</v>
       </c>
-      <c r="B101" s="1">
-        <v>992000</v>
+      <c r="B101" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="2">
+      <c r="A102" s="1">
         <v>536.4</v>
       </c>
-      <c r="B102" s="1">
-        <v>987500</v>
+      <c r="B102" s="2">
+        <v>98.75</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
+      <c r="A103" s="1">
         <v>1991.16</v>
       </c>
-      <c r="B103" s="1">
-        <v>992500</v>
+      <c r="B103" s="2">
+        <v>99.25</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="2">
+      <c r="A104" s="1">
         <v>22200.26</v>
       </c>
-      <c r="B104" s="1">
-        <v>996500</v>
+      <c r="B104" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="2">
+      <c r="A105" s="1">
         <v>1388.76</v>
       </c>
-      <c r="B105" s="1">
-        <v>993000</v>
+      <c r="B105" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="2">
+      <c r="A106" s="1">
         <v>60014.19</v>
       </c>
-      <c r="B106" s="1">
-        <v>997500</v>
+      <c r="B106" s="2">
+        <v>99.75</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="2">
+      <c r="A107" s="1">
         <v>66630.89</v>
       </c>
-      <c r="B107" s="1">
-        <v>997500</v>
+      <c r="B107" s="2">
+        <v>99.75</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="2">
+      <c r="A108" s="1">
         <v>2998.65</v>
       </c>
-      <c r="B108" s="1">
-        <v>993000</v>
+      <c r="B108" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="2">
+      <c r="A109" s="1">
         <v>116823.47</v>
       </c>
-      <c r="B109" s="1">
-        <v>997600</v>
+      <c r="B109" s="2">
+        <v>99.76</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="2">
+      <c r="A110" s="1">
         <v>1361935.73</v>
       </c>
-      <c r="B110" s="1">
-        <v>998250</v>
+      <c r="B110" s="2">
+        <v>99.82</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="2">
+      <c r="A111" s="1">
         <v>25696.49</v>
       </c>
-      <c r="B111" s="1">
-        <v>996500</v>
+      <c r="B111" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="2">
+      <c r="A112" s="1">
         <v>6890.48</v>
       </c>
-      <c r="B112" s="1">
-        <v>994000</v>
+      <c r="B112" s="2">
+        <v>99.4</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="2">
+      <c r="A113" s="1">
         <v>525381.06000000006</v>
       </c>
-      <c r="B113" s="1">
-        <v>998000</v>
+      <c r="B113" s="2">
+        <v>99.8</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="2">
+      <c r="A114" s="1">
         <v>42513.11</v>
       </c>
-      <c r="B114" s="1">
-        <v>996500</v>
+      <c r="B114" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="2">
+      <c r="A115" s="1">
         <v>1294.99</v>
       </c>
-      <c r="B115" s="1">
-        <v>993000</v>
+      <c r="B115" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="2">
+      <c r="A116" s="1">
         <v>27015.42</v>
       </c>
-      <c r="B116" s="1">
-        <v>996600</v>
+      <c r="B116" s="2">
+        <v>99.66</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="2">
+      <c r="A117" s="1">
         <v>300.18</v>
       </c>
-      <c r="B117" s="1">
-        <v>970000</v>
+      <c r="B117" s="2">
+        <v>97</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="2">
+      <c r="A118" s="1">
         <v>5951.24</v>
       </c>
-      <c r="B118" s="1">
-        <v>995000</v>
+      <c r="B118" s="2">
+        <v>99.5</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="2">
+      <c r="A119" s="1">
         <v>2399354.2799999998</v>
       </c>
-      <c r="B119" s="1">
-        <v>998350</v>
+      <c r="B119" s="2">
+        <v>99.83</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="2">
+      <c r="A120" s="1">
         <v>118299.66</v>
       </c>
-      <c r="B120" s="1">
-        <v>997600</v>
+      <c r="B120" s="2">
+        <v>99.76</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="2">
+      <c r="A121" s="1">
         <v>349.1</v>
       </c>
-      <c r="B121" s="1">
-        <v>950000</v>
+      <c r="B121" s="2">
+        <v>95</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="2">
+      <c r="A122" s="1">
         <v>9684.14</v>
       </c>
-      <c r="B122" s="1">
-        <v>996000</v>
+      <c r="B122" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="2">
+      <c r="A123" s="1">
         <v>1370.05</v>
       </c>
-      <c r="B123" s="1">
-        <v>992000</v>
+      <c r="B123" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="2">
+      <c r="A124" s="1">
         <v>220506.75</v>
       </c>
-      <c r="B124" s="1">
-        <v>997800</v>
+      <c r="B124" s="2">
+        <v>99.78</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="2">
+      <c r="A125" s="1">
         <v>7094.43</v>
       </c>
-      <c r="B125" s="1">
-        <v>995500</v>
+      <c r="B125" s="2">
+        <v>99.55</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="2">
+      <c r="A126" s="1">
         <v>1258.3599999999999</v>
       </c>
-      <c r="B126" s="1">
-        <v>991000</v>
+      <c r="B126" s="2">
+        <v>99.1</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="2">
+      <c r="A127" s="1">
         <v>218266.96</v>
       </c>
-      <c r="B127" s="1">
-        <v>997702</v>
+      <c r="B127" s="2">
+        <v>99.77</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="2">
+      <c r="A128" s="1">
         <v>655.82</v>
       </c>
-      <c r="B128" s="1">
-        <v>987500</v>
+      <c r="B128" s="2">
+        <v>98.75</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="2">
+      <c r="A129" s="1">
         <v>5159</v>
       </c>
-      <c r="B129" s="1">
-        <v>995000</v>
+      <c r="B129" s="2">
+        <v>99.5</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="2">
+      <c r="A130" s="1">
         <v>26359.83</v>
       </c>
-      <c r="B130" s="1">
-        <v>996500</v>
+      <c r="B130" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="2">
+      <c r="A131" s="1">
         <v>564.86</v>
       </c>
-      <c r="B131" s="1">
-        <v>990000</v>
+      <c r="B131" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="2">
+      <c r="A132" s="1">
         <v>171135.24</v>
       </c>
-      <c r="B132" s="1">
-        <v>997800</v>
+      <c r="B132" s="2">
+        <v>99.78</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="2">
+      <c r="A133" s="1">
         <v>8763.2000000000007</v>
       </c>
-      <c r="B133" s="1">
-        <v>995500</v>
+      <c r="B133" s="2">
+        <v>99.55</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="2">
+      <c r="A134" s="1">
         <v>19134.32</v>
       </c>
-      <c r="B134" s="1">
-        <v>996000</v>
+      <c r="B134" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="2">
+      <c r="A135" s="1">
         <v>2130.34</v>
       </c>
-      <c r="B135" s="1">
-        <v>990500</v>
+      <c r="B135" s="2">
+        <v>99.05</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="2">
+      <c r="A136" s="1">
         <v>520.66999999999996</v>
       </c>
-      <c r="B136" s="1">
-        <v>990500</v>
+      <c r="B136" s="2">
+        <v>99.05</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="2">
+      <c r="A137" s="1">
         <v>4054.47</v>
       </c>
-      <c r="B137" s="1">
-        <v>990000</v>
+      <c r="B137" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="2">
+      <c r="A138" s="1">
         <v>58048.63</v>
       </c>
-      <c r="B138" s="1">
-        <v>997000</v>
+      <c r="B138" s="2">
+        <v>99.7</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="2">
+      <c r="A139" s="1">
         <v>85567.3</v>
       </c>
-      <c r="B139" s="1">
-        <v>997500</v>
+      <c r="B139" s="2">
+        <v>99.75</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="2">
+      <c r="A140" s="1">
         <v>235968.46</v>
       </c>
-      <c r="B140" s="1">
-        <v>997800</v>
+      <c r="B140" s="2">
+        <v>99.78</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="2">
+      <c r="A141" s="1">
         <v>95305.7</v>
       </c>
-      <c r="B141" s="1">
-        <v>997500</v>
+      <c r="B141" s="2">
+        <v>99.75</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="2">
+      <c r="A142" s="1">
         <v>865.58</v>
       </c>
-      <c r="B142" s="1">
-        <v>987501</v>
+      <c r="B142" s="2">
+        <v>98.75</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="2">
+      <c r="A143" s="1">
         <v>333.64</v>
       </c>
-      <c r="B143" s="1">
-        <v>970000</v>
+      <c r="B143" s="2">
+        <v>97</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="2">
+      <c r="A144" s="1">
         <v>1263.5999999999999</v>
       </c>
-      <c r="B144" s="1">
-        <v>991000</v>
+      <c r="B144" s="2">
+        <v>99.1</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="2">
+      <c r="A145" s="1">
         <v>17026.400000000001</v>
       </c>
-      <c r="B145" s="1">
-        <v>995600</v>
+      <c r="B145" s="2">
+        <v>99.56</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="2">
+      <c r="A146" s="1">
         <v>339478.68</v>
       </c>
-      <c r="B146" s="1">
-        <v>997901</v>
+      <c r="B146" s="2">
+        <v>99.79</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="2">
+      <c r="A147" s="1">
         <v>14985.34</v>
       </c>
-      <c r="B147" s="1">
-        <v>996500</v>
+      <c r="B147" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="2">
+      <c r="A148" s="1">
         <v>32350.02</v>
       </c>
-      <c r="B148" s="1">
-        <v>997000</v>
+      <c r="B148" s="2">
+        <v>99.7</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="2">
+      <c r="A149" s="1">
         <v>30858.43</v>
       </c>
-      <c r="B149" s="1">
-        <v>996500</v>
+      <c r="B149" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="2">
+      <c r="A150" s="1">
         <v>63977.85</v>
       </c>
-      <c r="B150" s="1">
-        <v>997000</v>
+      <c r="B150" s="2">
+        <v>99.7</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="2">
+      <c r="A151" s="1">
         <v>4342.51</v>
       </c>
-      <c r="B151" s="1">
-        <v>994500</v>
+      <c r="B151" s="2">
+        <v>99.45</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="2">
+      <c r="A152" s="1">
         <v>78509.600000000006</v>
       </c>
-      <c r="B152" s="1">
-        <v>997000</v>
+      <c r="B152" s="2">
+        <v>99.7</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="2">
+      <c r="A153" s="1">
         <v>1065.17</v>
       </c>
-      <c r="B153" s="1">
-        <v>992500</v>
+      <c r="B153" s="2">
+        <v>99.25</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="2">
+      <c r="A154" s="1">
         <v>4474.4799999999996</v>
       </c>
-      <c r="B154" s="1">
-        <v>994500</v>
+      <c r="B154" s="2">
+        <v>99.45</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="2">
+      <c r="A155" s="1">
         <v>1168.03</v>
       </c>
-      <c r="B155" s="1">
-        <v>993400</v>
+      <c r="B155" s="2">
+        <v>99.34</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="2">
+      <c r="A156" s="1">
         <v>11072.98</v>
       </c>
-      <c r="B156" s="1">
-        <v>995000</v>
+      <c r="B156" s="2">
+        <v>99.5</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="2">
+      <c r="A157" s="1">
         <v>49722.58</v>
       </c>
-      <c r="B157" s="1">
-        <v>996600</v>
+      <c r="B157" s="2">
+        <v>99.66</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="2">
+      <c r="A158" s="1">
         <v>31729.22</v>
       </c>
-      <c r="B158" s="1">
-        <v>993500</v>
+      <c r="B158" s="2">
+        <v>99.35</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="2">
+      <c r="A159" s="1">
         <v>841.46</v>
       </c>
-      <c r="B159" s="1">
-        <v>990000</v>
+      <c r="B159" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="2">
+      <c r="A160" s="1">
         <v>526.89</v>
       </c>
-      <c r="B160" s="1">
-        <v>990000</v>
+      <c r="B160" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="2">
+      <c r="A161" s="1">
         <v>1751.05</v>
       </c>
-      <c r="B161" s="1">
-        <v>990000</v>
+      <c r="B161" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="2">
+      <c r="A162" s="1">
         <v>25541.19</v>
       </c>
-      <c r="B162" s="1">
-        <v>992500</v>
+      <c r="B162" s="2">
+        <v>99.25</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="2">
+      <c r="A163" s="1">
         <v>563.03</v>
       </c>
-      <c r="B163" s="1">
-        <v>960000</v>
+      <c r="B163" s="2">
+        <v>96</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="2">
+      <c r="A164" s="1">
         <v>1001.53</v>
       </c>
-      <c r="B164" s="1">
-        <v>992500</v>
+      <c r="B164" s="2">
+        <v>99.25</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="2">
+      <c r="A165" s="1">
         <v>1640.67</v>
       </c>
-      <c r="B165" s="1">
-        <v>992500</v>
+      <c r="B165" s="2">
+        <v>99.25</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="2">
+      <c r="A166" s="1">
         <v>9780.32</v>
       </c>
-      <c r="B166" s="1">
-        <v>995000</v>
+      <c r="B166" s="2">
+        <v>99.5</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="2">
+      <c r="A167" s="1">
         <v>2153.3200000000002</v>
       </c>
-      <c r="B167" s="1">
-        <v>992500</v>
+      <c r="B167" s="2">
+        <v>99.25</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="2">
+      <c r="A168" s="1">
         <v>791.16</v>
       </c>
-      <c r="B168" s="1">
-        <v>990000</v>
+      <c r="B168" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="2">
+      <c r="A169" s="1">
         <v>373.09</v>
       </c>
-      <c r="B169" s="1">
-        <v>970000</v>
+      <c r="B169" s="2">
+        <v>97</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="2">
+      <c r="A170" s="1">
         <v>957</v>
       </c>
-      <c r="B170" s="1">
-        <v>991000</v>
+      <c r="B170" s="2">
+        <v>99.1</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="2">
+      <c r="A171" s="1">
         <v>3434.39</v>
       </c>
-      <c r="B171" s="1">
-        <v>994000</v>
+      <c r="B171" s="2">
+        <v>99.4</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="2">
+      <c r="A172" s="1">
         <v>183322.32</v>
       </c>
-      <c r="B172" s="1">
-        <v>997850</v>
+      <c r="B172" s="2">
+        <v>99.78</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="2">
+      <c r="A173" s="1">
         <v>312453.14</v>
       </c>
-      <c r="B173" s="1">
-        <v>997800</v>
+      <c r="B173" s="2">
+        <v>99.78</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="2">
+      <c r="A174" s="1">
         <v>2404.66</v>
       </c>
-      <c r="B174" s="1">
-        <v>993500</v>
+      <c r="B174" s="2">
+        <v>99.35</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="2">
+      <c r="A175" s="1">
         <v>2149.46</v>
       </c>
-      <c r="B175" s="1">
-        <v>994000</v>
+      <c r="B175" s="2">
+        <v>99.4</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="2">
+      <c r="A176" s="1">
         <v>1515167.74</v>
       </c>
-      <c r="B176" s="1">
-        <v>998150</v>
+      <c r="B176" s="2">
+        <v>99.81</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="2">
+      <c r="A177" s="1">
         <v>1093.83</v>
       </c>
-      <c r="B177" s="1">
-        <v>991000</v>
+      <c r="B177" s="2">
+        <v>99.1</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="2">
+      <c r="A178" s="1">
         <v>199646.2</v>
       </c>
-      <c r="B178" s="1">
-        <v>997900</v>
+      <c r="B178" s="2">
+        <v>99.79</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="2">
+      <c r="A179" s="1">
         <v>6871.39</v>
       </c>
-      <c r="B179" s="1">
-        <v>994500</v>
+      <c r="B179" s="2">
+        <v>99.45</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="2">
+      <c r="A180" s="1">
         <v>403.24</v>
       </c>
-      <c r="B180" s="1">
-        <v>987500</v>
+      <c r="B180" s="2">
+        <v>98.75</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="2">
+      <c r="A181" s="1">
         <v>3152853.96</v>
       </c>
-      <c r="B181" s="1">
-        <v>998300</v>
+      <c r="B181" s="2">
+        <v>99.83</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="2">
+      <c r="A182" s="1">
         <v>16598.689999999999</v>
       </c>
-      <c r="B182" s="1">
-        <v>993900</v>
+      <c r="B182" s="2">
+        <v>99.39</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="2">
+      <c r="A183" s="1">
         <v>907.86</v>
       </c>
-      <c r="B183" s="1">
-        <v>991000</v>
+      <c r="B183" s="2">
+        <v>99.1</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="2">
+      <c r="A184" s="1">
         <v>11602.88</v>
       </c>
-      <c r="B184" s="1">
-        <v>995000</v>
+      <c r="B184" s="2">
+        <v>99.5</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="2">
+      <c r="A185" s="1">
         <v>1578.78</v>
       </c>
-      <c r="B185" s="1">
-        <v>991000</v>
+      <c r="B185" s="2">
+        <v>99.1</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="2">
+      <c r="A186" s="1">
         <v>20943.599999999999</v>
       </c>
-      <c r="B186" s="1">
-        <v>995500</v>
+      <c r="B186" s="2">
+        <v>99.55</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="2">
+      <c r="A187" s="1">
         <v>139.08000000000001</v>
       </c>
-      <c r="B187" s="1">
-        <v>930000</v>
+      <c r="B187" s="2">
+        <v>93</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="2">
+      <c r="A188" s="1">
         <v>36426.89</v>
       </c>
-      <c r="B188" s="1">
-        <v>996500</v>
+      <c r="B188" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="2">
+      <c r="A189" s="1">
         <v>3500</v>
       </c>
-      <c r="B189" s="1">
-        <v>991000</v>
+      <c r="B189" s="2">
+        <v>99.1</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="2">
+      <c r="A190" s="1">
         <v>28564.28</v>
       </c>
-      <c r="B190" s="1">
-        <v>996500</v>
+      <c r="B190" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="2">
+      <c r="A191" s="1">
         <v>13749.05</v>
       </c>
-      <c r="B191" s="1">
-        <v>996000</v>
+      <c r="B191" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="2">
+      <c r="A192" s="1">
         <v>29344.15</v>
       </c>
-      <c r="B192" s="1">
-        <v>992500</v>
+      <c r="B192" s="2">
+        <v>99.25</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="2">
+      <c r="A193" s="1">
         <v>33034.29</v>
       </c>
-      <c r="B193" s="1">
-        <v>996000</v>
+      <c r="B193" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="2">
+      <c r="A194" s="1">
         <v>36391.839999999997</v>
       </c>
-      <c r="B194" s="1">
-        <v>997000</v>
+      <c r="B194" s="2">
+        <v>99.7</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="2">
+      <c r="A195" s="1">
         <v>3210.66</v>
       </c>
-      <c r="B195" s="1">
-        <v>993000</v>
+      <c r="B195" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="2">
+      <c r="A196" s="1">
         <v>23583.74</v>
       </c>
-      <c r="B196" s="1">
-        <v>993000</v>
+      <c r="B196" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="2">
+      <c r="A197" s="1">
         <v>873.38</v>
       </c>
-      <c r="B197" s="1">
-        <v>980000</v>
+      <c r="B197" s="2">
+        <v>98</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="2">
+      <c r="A198" s="1">
         <v>10802</v>
       </c>
-      <c r="B198" s="1">
-        <v>995000</v>
+      <c r="B198" s="2">
+        <v>99.5</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="2">
+      <c r="A199" s="1">
         <v>61553.73</v>
       </c>
-      <c r="B199" s="1">
-        <v>997200</v>
+      <c r="B199" s="2">
+        <v>99.72</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="2">
+      <c r="A200" s="1">
         <v>10510.02</v>
       </c>
-      <c r="B200" s="1">
-        <v>996000</v>
+      <c r="B200" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="2">
+      <c r="A201" s="1">
         <v>4789.8999999999996</v>
       </c>
-      <c r="B201" s="1">
-        <v>993000</v>
+      <c r="B201" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="2">
+      <c r="A202" s="1">
         <v>1048.1099999999999</v>
       </c>
-      <c r="B202" s="1">
-        <v>992000</v>
+      <c r="B202" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="2">
+      <c r="A203" s="1">
         <v>1856.87</v>
       </c>
-      <c r="B203" s="1">
-        <v>993000</v>
+      <c r="B203" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="2">
+      <c r="A204" s="1">
         <v>313.66000000000003</v>
       </c>
-      <c r="B204" s="1">
-        <v>975000</v>
+      <c r="B204" s="2">
+        <v>97.5</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="2">
+      <c r="A205" s="1">
         <v>464.87</v>
       </c>
-      <c r="B205" s="1">
-        <v>980000</v>
+      <c r="B205" s="2">
+        <v>98</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="2">
+      <c r="A206" s="1">
         <v>2250</v>
       </c>
-      <c r="B206" s="1">
-        <v>993000</v>
+      <c r="B206" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="2">
+      <c r="A207" s="1">
         <v>60253.5</v>
       </c>
-      <c r="B207" s="1">
-        <v>997200</v>
+      <c r="B207" s="2">
+        <v>99.72</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="2">
+      <c r="A208" s="1">
         <v>1040.8699999999999</v>
       </c>
-      <c r="B208" s="1">
-        <v>992000</v>
+      <c r="B208" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="2">
+      <c r="A209" s="1">
         <v>1472.44</v>
       </c>
-      <c r="B209" s="1">
-        <v>993500</v>
+      <c r="B209" s="2">
+        <v>99.35</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="2">
+      <c r="A210" s="1">
         <v>36499.019999999997</v>
       </c>
-      <c r="B210" s="1">
-        <v>996500</v>
+      <c r="B210" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="2">
+      <c r="A211" s="1">
         <v>43885.4</v>
       </c>
-      <c r="B211" s="1">
-        <v>996900</v>
+      <c r="B211" s="2">
+        <v>99.69</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="2">
+      <c r="A212" s="1">
         <v>1003.46</v>
       </c>
-      <c r="B212" s="1">
-        <v>993000</v>
+      <c r="B212" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="2">
+      <c r="A213" s="1">
         <v>2362.5</v>
       </c>
-      <c r="B213" s="1">
-        <v>993300</v>
+      <c r="B213" s="2">
+        <v>99.33</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="2">
+      <c r="A214" s="1">
         <v>359.28</v>
       </c>
-      <c r="B214" s="1">
-        <v>950000</v>
+      <c r="B214" s="2">
+        <v>95</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="2">
+      <c r="A215" s="1">
         <v>6320.56</v>
       </c>
-      <c r="B215" s="1">
-        <v>990500</v>
+      <c r="B215" s="2">
+        <v>99.05</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="2">
+      <c r="A216" s="1">
         <v>27952.41</v>
       </c>
-      <c r="B216" s="1">
-        <v>996000</v>
+      <c r="B216" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="2">
+      <c r="A217" s="1">
         <v>62207.76</v>
       </c>
-      <c r="B217" s="1">
-        <v>996600</v>
+      <c r="B217" s="2">
+        <v>99.66</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="2">
+      <c r="A218" s="1">
         <v>54037.82</v>
       </c>
-      <c r="B218" s="1">
-        <v>997000</v>
+      <c r="B218" s="2">
+        <v>99.7</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="2">
+      <c r="A219" s="1">
         <v>32600</v>
       </c>
-      <c r="B219" s="1">
-        <v>997000</v>
+      <c r="B219" s="2">
+        <v>99.7</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="2">
+      <c r="A220" s="1">
         <v>79139.56</v>
       </c>
-      <c r="B220" s="1">
-        <v>997200</v>
+      <c r="B220" s="2">
+        <v>99.72</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="2">
+      <c r="A221" s="1">
         <v>1600</v>
       </c>
-      <c r="B221" s="1">
-        <v>992000</v>
+      <c r="B221" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="2">
+      <c r="A222" s="1">
         <v>3617.2</v>
       </c>
-      <c r="B222" s="1">
-        <v>993500</v>
+      <c r="B222" s="2">
+        <v>99.35</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="2">
+      <c r="A223" s="1">
         <v>1023.95</v>
       </c>
-      <c r="B223" s="1">
-        <v>992000</v>
+      <c r="B223" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="2">
+      <c r="A224" s="1">
         <v>63622.55</v>
       </c>
-      <c r="B224" s="1">
-        <v>997200</v>
+      <c r="B224" s="2">
+        <v>99.72</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="2">
+      <c r="A225" s="1">
         <v>318400.19</v>
       </c>
-      <c r="B225" s="1">
-        <v>997800</v>
+      <c r="B225" s="2">
+        <v>99.78</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="2">
+      <c r="A226" s="1">
         <v>241.13</v>
       </c>
-      <c r="B226" s="1">
-        <v>960001</v>
+      <c r="B226" s="2">
+        <v>96</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="2">
+      <c r="A227" s="1">
         <v>93275.33</v>
       </c>
-      <c r="B227" s="1">
-        <v>997850</v>
+      <c r="B227" s="2">
+        <v>99.78</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="2">
+      <c r="A228" s="1">
         <v>582.74</v>
       </c>
-      <c r="B228" s="1">
-        <v>990000</v>
+      <c r="B228" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" s="2">
+      <c r="A229" s="1">
         <v>484.48</v>
       </c>
-      <c r="B229" s="1">
-        <v>960000</v>
+      <c r="B229" s="2">
+        <v>96</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" s="2">
+      <c r="A230" s="1">
         <v>1470.14</v>
       </c>
-      <c r="B230" s="1">
-        <v>993000</v>
+      <c r="B230" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="2">
+      <c r="A231" s="1">
         <v>721.74</v>
       </c>
-      <c r="B231" s="1">
-        <v>990500</v>
+      <c r="B231" s="2">
+        <v>99.05</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="2">
+      <c r="A232" s="1">
         <v>34196.36</v>
       </c>
-      <c r="B232" s="1">
-        <v>996700</v>
+      <c r="B232" s="2">
+        <v>99.67</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="2">
+      <c r="A233" s="1">
         <v>86978.16</v>
       </c>
-      <c r="B233" s="1">
-        <v>997500</v>
+      <c r="B233" s="2">
+        <v>99.75</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="2">
+      <c r="A234" s="1">
         <v>3147.88</v>
       </c>
-      <c r="B234" s="1">
-        <v>993000</v>
+      <c r="B234" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="2">
+      <c r="A235" s="1">
         <v>340263.59</v>
       </c>
-      <c r="B235" s="1">
-        <v>997800</v>
+      <c r="B235" s="2">
+        <v>99.78</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="2">
+      <c r="A236" s="1">
         <v>1654.75</v>
       </c>
-      <c r="B236" s="1">
-        <v>990000</v>
+      <c r="B236" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="2">
+      <c r="A237" s="1">
         <v>2278.33</v>
       </c>
-      <c r="B237" s="1">
-        <v>993000</v>
+      <c r="B237" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="2">
+      <c r="A238" s="1">
         <v>4865.71</v>
       </c>
-      <c r="B238" s="1">
-        <v>994000</v>
+      <c r="B238" s="2">
+        <v>99.4</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="2">
+      <c r="A239" s="1">
         <v>1961.53</v>
       </c>
-      <c r="B239" s="1">
-        <v>992000</v>
+      <c r="B239" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="2">
+      <c r="A240" s="1">
         <v>2174.9299999999998</v>
       </c>
-      <c r="B240" s="1">
-        <v>990000</v>
+      <c r="B240" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="2">
+      <c r="A241" s="1">
         <v>77109.14</v>
       </c>
-      <c r="B241" s="1">
-        <v>997500</v>
+      <c r="B241" s="2">
+        <v>99.75</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="2">
+      <c r="A242" s="1">
         <v>3500</v>
       </c>
-      <c r="B242" s="1">
-        <v>995000</v>
+      <c r="B242" s="2">
+        <v>99.5</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="2">
+      <c r="A243" s="1">
         <v>2498.0500000000002</v>
       </c>
-      <c r="B243" s="1">
-        <v>994000</v>
+      <c r="B243" s="2">
+        <v>99.4</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="2">
+      <c r="A244" s="1">
         <v>2127569.62</v>
       </c>
-      <c r="B244" s="1">
-        <v>998223</v>
+      <c r="B244" s="2">
+        <v>99.82</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="2">
+      <c r="A245" s="1">
         <v>2472.88</v>
       </c>
-      <c r="B245" s="1">
-        <v>993000</v>
+      <c r="B245" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="2">
+      <c r="A246" s="1">
         <v>17509.400000000001</v>
       </c>
-      <c r="B246" s="1">
-        <v>996500</v>
+      <c r="B246" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="2">
+      <c r="A247" s="1">
         <v>14619.07</v>
       </c>
-      <c r="B247" s="1">
-        <v>993000</v>
+      <c r="B247" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="2">
+      <c r="A248" s="1">
         <v>580.07000000000005</v>
       </c>
-      <c r="B248" s="1">
-        <v>980000</v>
+      <c r="B248" s="2">
+        <v>98</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="2">
+      <c r="A249" s="1">
         <v>352584.61</v>
       </c>
-      <c r="B249" s="1">
-        <v>998200</v>
+      <c r="B249" s="2">
+        <v>99.82</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="2">
+      <c r="A250" s="1">
         <v>10567.58</v>
       </c>
-      <c r="B250" s="1">
-        <v>992500</v>
+      <c r="B250" s="2">
+        <v>99.25</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="2">
+      <c r="A251" s="1">
         <v>6229.31</v>
       </c>
-      <c r="B251" s="1">
-        <v>990000</v>
+      <c r="B251" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="2">
+      <c r="A252" s="1">
         <v>690</v>
       </c>
-      <c r="B252" s="1">
-        <v>980000</v>
+      <c r="B252" s="2">
+        <v>98</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="2">
+      <c r="A253" s="1">
         <v>1967.1</v>
       </c>
-      <c r="B253" s="1">
-        <v>993000</v>
+      <c r="B253" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="2">
+      <c r="A254" s="1">
         <v>28709.74</v>
       </c>
-      <c r="B254" s="1">
-        <v>996000</v>
+      <c r="B254" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="2">
+      <c r="A255" s="1">
         <v>651.36</v>
       </c>
-      <c r="B255" s="1">
-        <v>980000</v>
+      <c r="B255" s="2">
+        <v>98</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="2">
+      <c r="A256" s="1">
         <v>159803.97</v>
       </c>
-      <c r="B256" s="1">
-        <v>997500</v>
+      <c r="B256" s="2">
+        <v>99.75</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="2">
+      <c r="A257" s="1">
         <v>990.31</v>
       </c>
-      <c r="B257" s="1">
-        <v>990000</v>
+      <c r="B257" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="2">
+      <c r="A258" s="1">
         <v>3030</v>
       </c>
-      <c r="B258" s="1">
-        <v>990000</v>
+      <c r="B258" s="2">
+        <v>99</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="2">
+      <c r="A259" s="1">
         <v>156980.94</v>
       </c>
-      <c r="B259" s="1">
-        <v>997900</v>
+      <c r="B259" s="2">
+        <v>99.79</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="2">
+      <c r="A260" s="1">
         <v>25275.89</v>
       </c>
-      <c r="B260" s="1">
-        <v>992000</v>
+      <c r="B260" s="2">
+        <v>99.2</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="2">
+      <c r="A261" s="1">
         <v>13370.05</v>
       </c>
-      <c r="B261" s="1">
-        <v>996000</v>
+      <c r="B261" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="2">
+      <c r="A262" s="1">
         <v>6879.34</v>
       </c>
-      <c r="B262" s="1">
-        <v>996000</v>
+      <c r="B262" s="2">
+        <v>99.6</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="2">
+      <c r="A263" s="1">
         <v>3017062.22</v>
       </c>
-      <c r="B263" s="1">
-        <v>998550</v>
+      <c r="B263" s="2">
+        <v>99.85</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="2">
+      <c r="A264" s="1">
         <v>447031.91</v>
       </c>
-      <c r="B264" s="1">
-        <v>998100</v>
+      <c r="B264" s="2">
+        <v>99.81</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="2">
+      <c r="A265" s="1">
         <v>28192.54</v>
       </c>
-      <c r="B265" s="1">
-        <v>996500</v>
+      <c r="B265" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="2">
+      <c r="A266" s="1">
         <v>4240.0600000000004</v>
       </c>
-      <c r="B266" s="1">
-        <v>994500</v>
+      <c r="B266" s="2">
+        <v>99.45</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="2">
+      <c r="A267" s="1">
         <v>150585.21</v>
       </c>
-      <c r="B267" s="1">
-        <v>998000</v>
+      <c r="B267" s="2">
+        <v>99.8</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="2">
+      <c r="A268" s="1">
         <v>104934.71</v>
       </c>
-      <c r="B268" s="1">
-        <v>998000</v>
+      <c r="B268" s="2">
+        <v>99.8</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="2">
+      <c r="A269" s="1">
         <v>61079.67</v>
       </c>
-      <c r="B269" s="1">
-        <v>997200</v>
+      <c r="B269" s="2">
+        <v>99.72</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="2">
+      <c r="A270" s="1">
         <v>621809.68999999994</v>
       </c>
-      <c r="B270" s="1">
-        <v>998200</v>
+      <c r="B270" s="2">
+        <v>99.82</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="2">
+      <c r="A271" s="1">
         <v>1869.56</v>
       </c>
-      <c r="B271" s="1">
-        <v>993000</v>
+      <c r="B271" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="2">
+      <c r="A272" s="1">
         <v>453651.18</v>
       </c>
-      <c r="B272" s="1">
-        <v>998100</v>
+      <c r="B272" s="2">
+        <v>99.81</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="2">
+      <c r="A273" s="1">
         <v>62730.96</v>
       </c>
-      <c r="B273" s="1">
-        <v>997200</v>
+      <c r="B273" s="2">
+        <v>99.72</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="2">
+      <c r="A274" s="1">
         <v>23621.26</v>
       </c>
-      <c r="B274" s="1">
-        <v>996500</v>
+      <c r="B274" s="2">
+        <v>99.65</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="2">
+      <c r="A275" s="1">
         <v>110145.46</v>
       </c>
-      <c r="B275" s="1">
-        <v>998000</v>
+      <c r="B275" s="2">
+        <v>99.8</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="2">
+      <c r="A276" s="1">
         <v>2197.5700000000002</v>
       </c>
-      <c r="B276" s="1">
-        <v>993000</v>
+      <c r="B276" s="2">
+        <v>99.3</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="2">
+      <c r="A277" s="1">
         <v>401.67</v>
       </c>
-      <c r="B277" s="1">
-        <v>980000</v>
+      <c r="B277" s="2">
+        <v>98</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="2">
+      <c r="A278" s="1">
         <v>487.17</v>
       </c>
-      <c r="B278" s="1">
-        <v>985000</v>
+      <c r="B278" s="2">
+        <v>98.5</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="2">
+      <c r="A279" s="1">
         <v>127047.01</v>
       </c>
-      <c r="B279" s="1">
-        <v>998000</v>
+      <c r="B279" s="2">
+        <v>99.8</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="2">
+      <c r="A280" s="1">
         <v>4065.67</v>
       </c>
-      <c r="B280" s="1">
-        <v>994500</v>
+      <c r="B280" s="2">
+        <v>99.45</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="2">
+      <c r="A281" s="1">
         <v>41393.57</v>
       </c>
-      <c r="B281" s="1">
-        <v>996600</v>
+      <c r="B281" s="2">
+        <v>99.66</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="2">
+      <c r="A282" s="1">
         <v>493.85</v>
       </c>
-      <c r="B282" s="1">
-        <v>985000</v>
+      <c r="B282" s="2">
+        <v>98.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
29 de septiembre y actualizacion nc
</commit_message>
<xml_diff>
--- a/data/NC_semanal.xlsx
+++ b/data/NC_semanal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Desktop\MetrovaloresApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B000E28-FFE8-44DA-B6A3-090A2DC2301C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8698C29-B89B-439F-AE96-45EE9B83BE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{9E78C8B1-ED59-4A81-8FF9-F1A88ED1C1A0}"/>
   </bookViews>
@@ -901,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077B50AF-9C9F-4CF5-BB56-A27ACF5565DE}">
-  <dimension ref="A1:B282"/>
+  <dimension ref="A1:B283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B282"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,711 +922,711 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1140.92</v>
-      </c>
-      <c r="B2" s="2">
-        <v>99.2</v>
+        <v>4493.05</v>
+      </c>
+      <c r="B2">
+        <v>99.15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>135.96</v>
+        <v>1031.67</v>
       </c>
       <c r="B3" s="2">
-        <v>93</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>128516.33</v>
+        <v>161.66999999999999</v>
       </c>
       <c r="B4" s="2">
-        <v>99.76</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>19510.89</v>
+        <v>5921.75</v>
       </c>
       <c r="B5" s="2">
-        <v>99.6</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>19872.64</v>
+        <v>5113.4399999999996</v>
       </c>
       <c r="B6" s="2">
-        <v>99.55</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>196370.73</v>
+        <v>15825.92</v>
       </c>
       <c r="B7" s="2">
-        <v>99.76</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>220718.91</v>
+        <v>16306.25</v>
       </c>
       <c r="B8" s="2">
-        <v>99.8</v>
+        <v>99.62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>15970.77</v>
+        <v>49704.67</v>
       </c>
       <c r="B9" s="2">
-        <v>99.3</v>
+        <v>99.72</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>143503.24</v>
+        <v>14565.41</v>
       </c>
       <c r="B10" s="2">
-        <v>99.76</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>37838.129999999997</v>
+        <v>9829.4500000000007</v>
       </c>
       <c r="B11" s="2">
-        <v>99.65</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>2159.81</v>
+        <v>14399.72</v>
       </c>
       <c r="B12" s="2">
-        <v>99.37</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1092.1199999999999</v>
+        <v>26827.34</v>
       </c>
       <c r="B13" s="2">
-        <v>99.2</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2030.94</v>
+        <v>282.12</v>
       </c>
       <c r="B14" s="2">
-        <v>99.4</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>407.92</v>
+        <v>57386.73</v>
       </c>
       <c r="B15" s="2">
-        <v>96</v>
+        <v>99.72</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>4203.99</v>
+        <v>2625</v>
       </c>
       <c r="B16" s="2">
-        <v>99.45</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1582.39</v>
+        <v>3284.76</v>
       </c>
       <c r="B17" s="2">
-        <v>99.2</v>
+        <v>99.52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>729.88</v>
+        <v>2178.37</v>
       </c>
       <c r="B18" s="2">
-        <v>99</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1208.1500000000001</v>
+        <v>39901.919999999998</v>
       </c>
       <c r="B19" s="2">
-        <v>99.25</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>121071.23</v>
+        <v>41791.61</v>
       </c>
       <c r="B20" s="2">
-        <v>99.77</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1838.43</v>
+        <v>209792.03</v>
       </c>
       <c r="B21" s="2">
-        <v>99.2</v>
+        <v>99.78</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>21138.55</v>
+        <v>1849.48</v>
       </c>
       <c r="B22" s="2">
-        <v>99.35</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1678.31</v>
+        <v>1334</v>
       </c>
       <c r="B23" s="2">
-        <v>99.35</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>746.67</v>
+        <v>7520.77</v>
       </c>
       <c r="B24" s="2">
-        <v>99</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1633</v>
+        <v>2018.63</v>
       </c>
       <c r="B25" s="2">
-        <v>99.36</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>92712.45</v>
+        <v>14242.15</v>
       </c>
       <c r="B26" s="2">
-        <v>99.76</v>
+        <v>99.15</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>2826.47</v>
+        <v>15572.89</v>
       </c>
       <c r="B27" s="2">
-        <v>99.47</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>2604.63</v>
+        <v>460.08</v>
       </c>
       <c r="B28" s="2">
-        <v>99.05</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>17874.7</v>
+        <v>2812.12</v>
       </c>
       <c r="B29" s="2">
-        <v>99.65</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>7158.8</v>
+        <v>6101.96</v>
       </c>
       <c r="B30" s="2">
-        <v>99.56</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>23212.28</v>
+        <v>117.77</v>
       </c>
       <c r="B31" s="2">
-        <v>99.65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>102698.4</v>
+        <v>25111.63</v>
       </c>
       <c r="B32" s="2">
-        <v>99.79</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>26435.4</v>
+        <v>64707.27</v>
       </c>
       <c r="B33" s="2">
-        <v>99.2</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>4501.6899999999996</v>
+        <v>330951.02</v>
       </c>
       <c r="B34" s="2">
-        <v>99.4</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>9254.33</v>
+        <v>18398.25</v>
       </c>
       <c r="B35" s="2">
-        <v>99.57</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>1730.63</v>
+        <v>502.03</v>
       </c>
       <c r="B36" s="2">
-        <v>99.35</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>7198.93</v>
+        <v>1500</v>
       </c>
       <c r="B37" s="2">
-        <v>99.4</v>
+        <v>99.15</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>908.93</v>
+        <v>1595.06</v>
       </c>
       <c r="B38" s="2">
-        <v>99.2</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>10344.200000000001</v>
+        <v>119.83</v>
       </c>
       <c r="B39" s="2">
-        <v>99.68</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>15154.55</v>
+        <v>15710.59</v>
       </c>
       <c r="B40" s="2">
-        <v>99.5</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>1599.49</v>
+        <v>8635.35</v>
       </c>
       <c r="B41" s="2">
-        <v>99.3</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>468343.59</v>
+        <v>3922.79</v>
       </c>
       <c r="B42" s="2">
-        <v>99.8</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>13339.09</v>
+        <v>400.47</v>
       </c>
       <c r="B43" s="2">
-        <v>99.55</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>12118.39</v>
+        <v>695429.82</v>
       </c>
       <c r="B44" s="2">
-        <v>99.55</v>
+        <v>99.79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>28384.13</v>
+        <v>138546.67000000001</v>
       </c>
       <c r="B45" s="2">
-        <v>99.65</v>
+        <v>99.79</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>10996.8</v>
+        <v>2010.41</v>
       </c>
       <c r="B46" s="2">
-        <v>99.65</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>400.21</v>
+        <v>710.81</v>
       </c>
       <c r="B47" s="2">
-        <v>97</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>1614.57</v>
+        <v>1444.52</v>
       </c>
       <c r="B48" s="2">
-        <v>99.1</v>
+        <v>99.15</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>8290.57</v>
+        <v>114547.39</v>
       </c>
       <c r="B49" s="2">
-        <v>99.05</v>
+        <v>99.76</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>1977.79</v>
+        <v>1140.28</v>
       </c>
       <c r="B50" s="2">
-        <v>99</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>669.01</v>
+        <v>811.81</v>
       </c>
       <c r="B51" s="2">
-        <v>98.5</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>21656.03</v>
+        <v>102443.69</v>
       </c>
       <c r="B52" s="2">
-        <v>99.75</v>
+        <v>99.78</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>93116.6</v>
+        <v>6571.32</v>
       </c>
       <c r="B53" s="2">
-        <v>99.76</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>1957.17</v>
+        <v>1085.05</v>
       </c>
       <c r="B54" s="2">
-        <v>99.25</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>12524.24</v>
+        <v>1487.02</v>
       </c>
       <c r="B55" s="2">
-        <v>99.5</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>10000</v>
+        <v>269.95999999999998</v>
       </c>
       <c r="B56" s="2">
-        <v>99.6</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>39527.01</v>
+        <v>969.96</v>
       </c>
       <c r="B57" s="2">
-        <v>99.67</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>3136.98</v>
+        <v>1255.0899999999999</v>
       </c>
       <c r="B58" s="2">
-        <v>99.35</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>969.95</v>
+        <v>7849.26</v>
       </c>
       <c r="B59" s="2">
-        <v>99.2</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>1172.46</v>
+        <v>2096.0500000000002</v>
       </c>
       <c r="B60" s="2">
-        <v>99.25</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>3232.92</v>
+        <v>41394.82</v>
       </c>
       <c r="B61" s="2">
-        <v>99.35</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>6070.04</v>
+        <v>200000</v>
       </c>
       <c r="B62" s="2">
-        <v>99.4</v>
+        <v>99.78</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>10586.42</v>
+        <v>121124.27</v>
       </c>
       <c r="B63" s="2">
-        <v>99.4</v>
+        <v>99.76</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>7921.52</v>
+        <v>31544.11</v>
       </c>
       <c r="B64" s="2">
-        <v>99.45</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>3298.82</v>
+        <v>1700000</v>
       </c>
       <c r="B65" s="2">
-        <v>99.2</v>
+        <v>99.83</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>310950.89</v>
+        <v>326486.19</v>
       </c>
       <c r="B66" s="2">
-        <v>99.77</v>
+        <v>99.79</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>10680.91</v>
+        <v>544.33000000000004</v>
       </c>
       <c r="B67" s="2">
-        <v>99.5</v>
+        <v>98.51</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>289559.96000000002</v>
+        <v>450.13</v>
       </c>
       <c r="B68" s="2">
-        <v>99.72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>6653.77</v>
+        <v>1781.31</v>
       </c>
       <c r="B69" s="2">
-        <v>99.4</v>
+        <v>99</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>1559.85</v>
+        <v>164573.99</v>
       </c>
       <c r="B70" s="2">
-        <v>99.1</v>
+        <v>99.78</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>7988.39</v>
+        <v>166502.71</v>
       </c>
       <c r="B71" s="2">
-        <v>99.5</v>
+        <v>99.79</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>44956.800000000003</v>
+        <v>227209.88</v>
       </c>
       <c r="B72" s="2">
-        <v>99.65</v>
+        <v>99.79</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>361851.73</v>
+        <v>10975.63</v>
       </c>
       <c r="B73" s="2">
-        <v>99.81</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>39886.6</v>
+        <v>32297.01</v>
       </c>
       <c r="B74" s="2">
-        <v>99.67</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>93715.28</v>
+        <v>467177.31</v>
       </c>
       <c r="B75" s="2">
-        <v>99.76</v>
+        <v>99.81</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>9111.18</v>
+        <v>34540.199999999997</v>
       </c>
       <c r="B76" s="2">
-        <v>99.6</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>3295.46</v>
+        <v>241.91</v>
       </c>
       <c r="B77" s="2">
-        <v>99.3</v>
+        <v>92</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>100703.09</v>
+        <v>21031.43</v>
       </c>
       <c r="B78" s="2">
-        <v>99.76</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>153194.67000000001</v>
+        <v>47693.120000000003</v>
       </c>
       <c r="B79" s="2">
-        <v>99.76</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>44552.76</v>
+        <v>809.42</v>
       </c>
       <c r="B80" s="2">
-        <v>99.67</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>1139.22</v>
+        <v>3260.35</v>
       </c>
       <c r="B81" s="2">
-        <v>99.3</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>9354.5499999999993</v>
+        <v>10835.88</v>
       </c>
       <c r="B82" s="2">
-        <v>99.59</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>30542.51</v>
+        <v>24877.62</v>
       </c>
       <c r="B83" s="2">
-        <v>99.6</v>
+        <v>99.62</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>1342.4</v>
+        <v>4324.57</v>
       </c>
       <c r="B84" s="2">
-        <v>99.25</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>106916.71</v>
+        <v>185910.06</v>
       </c>
       <c r="B85" s="2">
-        <v>99.75</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>36148.730000000003</v>
+        <v>18046.7</v>
       </c>
       <c r="B86" s="2">
-        <v>99.7</v>
+        <v>99.62</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>1548.59</v>
+        <v>889.02</v>
       </c>
       <c r="B87" s="2">
-        <v>99.22</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>1097.1500000000001</v>
+        <v>125984.34</v>
       </c>
       <c r="B88" s="2">
-        <v>99</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>1210.3900000000001</v>
+        <v>4041.88</v>
       </c>
       <c r="B89" s="2">
-        <v>99</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>1392.34</v>
+        <v>3231.59</v>
       </c>
       <c r="B90" s="2">
         <v>99</v>
@@ -1634,15 +1634,15 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>265636.02</v>
+        <v>957.12</v>
       </c>
       <c r="B91" s="2">
-        <v>99.77</v>
+        <v>99</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>2330.15</v>
+        <v>1255.96</v>
       </c>
       <c r="B92" s="2">
         <v>99</v>
@@ -1650,543 +1650,543 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>1136.31</v>
+        <v>3436.55</v>
       </c>
       <c r="B93" s="2">
-        <v>99.3</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>3209.98</v>
+        <v>104947.02</v>
       </c>
       <c r="B94" s="2">
-        <v>99</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>3997.6</v>
+        <v>16960.46</v>
       </c>
       <c r="B95" s="2">
-        <v>99</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>15960.72</v>
+        <v>12951.78</v>
       </c>
       <c r="B96" s="2">
-        <v>99.62</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>12958.81</v>
+        <v>59372.55</v>
       </c>
       <c r="B97" s="2">
-        <v>99.63</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>381487.86</v>
+        <v>2393.73</v>
       </c>
       <c r="B98" s="2">
-        <v>99.8</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>1934.71</v>
+        <v>1810.48</v>
       </c>
       <c r="B99" s="2">
-        <v>99.3</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>2751.03</v>
+        <v>420.09</v>
       </c>
       <c r="B100" s="2">
-        <v>99.3</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>1001.55</v>
+        <v>1225.94</v>
       </c>
       <c r="B101" s="2">
-        <v>99.2</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>536.4</v>
+        <v>7619.63</v>
       </c>
       <c r="B102" s="2">
-        <v>98.75</v>
+        <v>99.52</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>1991.16</v>
+        <v>591.54</v>
       </c>
       <c r="B103" s="2">
-        <v>99.25</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>22200.26</v>
+        <v>2350.1999999999998</v>
       </c>
       <c r="B104" s="2">
-        <v>99.65</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>1388.76</v>
+        <v>419622.69</v>
       </c>
       <c r="B105" s="2">
-        <v>99.3</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>60014.19</v>
+        <v>2241.52</v>
       </c>
       <c r="B106" s="2">
-        <v>99.75</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>66630.89</v>
+        <v>97164.160000000003</v>
       </c>
       <c r="B107" s="2">
-        <v>99.75</v>
+        <v>99.76</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>2998.65</v>
+        <v>553.79999999999995</v>
       </c>
       <c r="B108" s="2">
-        <v>99.3</v>
+        <v>99</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>116823.47</v>
+        <v>3555.9</v>
       </c>
       <c r="B109" s="2">
-        <v>99.76</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>1361935.73</v>
+        <v>172321.15</v>
       </c>
       <c r="B110" s="2">
-        <v>99.82</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>25696.49</v>
+        <v>24793.62</v>
       </c>
       <c r="B111" s="2">
-        <v>99.65</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>6890.48</v>
+        <v>987.98</v>
       </c>
       <c r="B112" s="2">
-        <v>99.4</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>525381.06000000006</v>
+        <v>397.54</v>
       </c>
       <c r="B113" s="2">
-        <v>99.8</v>
+        <v>98</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>42513.11</v>
+        <v>1903.27</v>
       </c>
       <c r="B114" s="2">
-        <v>99.65</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>1294.99</v>
+        <v>107432.49</v>
       </c>
       <c r="B115" s="2">
-        <v>99.3</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>27015.42</v>
+        <v>18430.45</v>
       </c>
       <c r="B116" s="2">
-        <v>99.66</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>300.18</v>
+        <v>3271.15</v>
       </c>
       <c r="B117" s="2">
-        <v>97</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>5951.24</v>
+        <v>15318.89</v>
       </c>
       <c r="B118" s="2">
-        <v>99.5</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>2399354.2799999998</v>
+        <v>52562.69</v>
       </c>
       <c r="B119" s="2">
-        <v>99.83</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>118299.66</v>
+        <v>29509.38</v>
       </c>
       <c r="B120" s="2">
-        <v>99.76</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>349.1</v>
+        <v>8184.63</v>
       </c>
       <c r="B121" s="2">
-        <v>95</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>9684.14</v>
+        <v>1404.21</v>
       </c>
       <c r="B122" s="2">
-        <v>99.6</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>1370.05</v>
+        <v>667.39</v>
       </c>
       <c r="B123" s="2">
-        <v>99.2</v>
+        <v>99</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>220506.75</v>
+        <v>555.63</v>
       </c>
       <c r="B124" s="2">
-        <v>99.78</v>
+        <v>99</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>7094.43</v>
+        <v>8714.48</v>
       </c>
       <c r="B125" s="2">
-        <v>99.55</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>1258.3599999999999</v>
+        <v>5843.66</v>
       </c>
       <c r="B126" s="2">
-        <v>99.1</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>218266.96</v>
+        <v>47460.5</v>
       </c>
       <c r="B127" s="2">
-        <v>99.77</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>655.82</v>
+        <v>3344.24</v>
       </c>
       <c r="B128" s="2">
-        <v>98.75</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>5159</v>
+        <v>72838.240000000005</v>
       </c>
       <c r="B129" s="2">
-        <v>99.5</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>26359.83</v>
+        <v>18022.88</v>
       </c>
       <c r="B130" s="2">
-        <v>99.65</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>564.86</v>
+        <v>2331.37</v>
       </c>
       <c r="B131" s="2">
-        <v>99</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>171135.24</v>
+        <v>21101.91</v>
       </c>
       <c r="B132" s="2">
-        <v>99.78</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>8763.2000000000007</v>
+        <v>4885.8</v>
       </c>
       <c r="B133" s="2">
-        <v>99.55</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>19134.32</v>
+        <v>1146.69</v>
       </c>
       <c r="B134" s="2">
-        <v>99.6</v>
+        <v>99</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>2130.34</v>
+        <v>16532.43</v>
       </c>
       <c r="B135" s="2">
-        <v>99.05</v>
+        <v>99.15</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>520.66999999999996</v>
+        <v>866.56</v>
       </c>
       <c r="B136" s="2">
-        <v>99.05</v>
+        <v>98</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>4054.47</v>
+        <v>1297.2</v>
       </c>
       <c r="B137" s="2">
-        <v>99</v>
+        <v>99.05</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>58048.63</v>
+        <v>1464.55</v>
       </c>
       <c r="B138" s="2">
-        <v>99.7</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>85567.3</v>
+        <v>713.97</v>
       </c>
       <c r="B139" s="2">
-        <v>99.75</v>
+        <v>99</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>235968.46</v>
+        <v>33829.97</v>
       </c>
       <c r="B140" s="2">
-        <v>99.78</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>95305.7</v>
+        <v>139.43</v>
       </c>
       <c r="B141" s="2">
-        <v>99.75</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>865.58</v>
+        <v>24262.14</v>
       </c>
       <c r="B142" s="2">
-        <v>98.75</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>333.64</v>
+        <v>1366108.33</v>
       </c>
       <c r="B143" s="2">
-        <v>97</v>
+        <v>99.82</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>1263.5999999999999</v>
+        <v>47640.41</v>
       </c>
       <c r="B144" s="2">
-        <v>99.1</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>17026.400000000001</v>
+        <v>255637.55</v>
       </c>
       <c r="B145" s="2">
-        <v>99.56</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>339478.68</v>
+        <v>29000</v>
       </c>
       <c r="B146" s="2">
-        <v>99.79</v>
+        <v>99.62</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>14985.34</v>
+        <v>13733.87</v>
       </c>
       <c r="B147" s="2">
-        <v>99.65</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>32350.02</v>
+        <v>12049.58</v>
       </c>
       <c r="B148" s="2">
-        <v>99.7</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>30858.43</v>
+        <v>637741.18999999994</v>
       </c>
       <c r="B149" s="2">
-        <v>99.65</v>
+        <v>99.81</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>63977.85</v>
+        <v>273925.57</v>
       </c>
       <c r="B150" s="2">
-        <v>99.7</v>
+        <v>99.81</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>4342.51</v>
+        <v>35408.629999999997</v>
       </c>
       <c r="B151" s="2">
-        <v>99.45</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>78509.600000000006</v>
+        <v>6754.79</v>
       </c>
       <c r="B152" s="2">
-        <v>99.7</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>1065.17</v>
+        <v>126.6</v>
       </c>
       <c r="B153" s="2">
-        <v>99.25</v>
+        <v>96.15</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>4474.4799999999996</v>
+        <v>599.26</v>
       </c>
       <c r="B154" s="2">
-        <v>99.45</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>1168.03</v>
+        <v>1032.8699999999999</v>
       </c>
       <c r="B155" s="2">
-        <v>99.34</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>11072.98</v>
+        <v>66767.38</v>
       </c>
       <c r="B156" s="2">
-        <v>99.5</v>
+        <v>99.72</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>49722.58</v>
+        <v>6550</v>
       </c>
       <c r="B157" s="2">
-        <v>99.66</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>31729.22</v>
+        <v>216164.22</v>
       </c>
       <c r="B158" s="2">
-        <v>99.35</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>841.46</v>
+        <v>5577.69</v>
       </c>
       <c r="B159" s="2">
-        <v>99</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>526.89</v>
+        <v>745.17</v>
       </c>
       <c r="B160" s="2">
         <v>99</v>
@@ -2194,7 +2194,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>1751.05</v>
+        <v>6836.57</v>
       </c>
       <c r="B161" s="2">
         <v>99</v>
@@ -2202,103 +2202,103 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>25541.19</v>
+        <v>21867.75</v>
       </c>
       <c r="B162" s="2">
-        <v>99.25</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>563.03</v>
+        <v>7000</v>
       </c>
       <c r="B163" s="2">
-        <v>96</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>1001.53</v>
+        <v>4994.08</v>
       </c>
       <c r="B164" s="2">
-        <v>99.25</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>1640.67</v>
+        <v>10430.31</v>
       </c>
       <c r="B165" s="2">
-        <v>99.25</v>
+        <v>99.61</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>9780.32</v>
+        <v>10581.41</v>
       </c>
       <c r="B166" s="2">
-        <v>99.5</v>
+        <v>99.62</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>2153.3200000000002</v>
+        <v>6821.15</v>
       </c>
       <c r="B167" s="2">
-        <v>99.25</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>791.16</v>
+        <v>18792.560000000001</v>
       </c>
       <c r="B168" s="2">
-        <v>99</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>373.09</v>
+        <v>24418.42</v>
       </c>
       <c r="B169" s="2">
-        <v>97</v>
+        <v>99.66</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>957</v>
+        <v>237841.18</v>
       </c>
       <c r="B170" s="2">
-        <v>99.1</v>
+        <v>99.82</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>3434.39</v>
+        <v>40027.68</v>
       </c>
       <c r="B171" s="2">
-        <v>99.4</v>
+        <v>99.68</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>183322.32</v>
+        <v>827.57</v>
       </c>
       <c r="B172" s="2">
-        <v>99.78</v>
+        <v>99</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>312453.14</v>
+        <v>271.3</v>
       </c>
       <c r="B173" s="2">
-        <v>99.78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>2404.66</v>
+        <v>3049.87</v>
       </c>
       <c r="B174" s="2">
         <v>99.35</v>
@@ -2306,23 +2306,23 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>2149.46</v>
+        <v>5753.34</v>
       </c>
       <c r="B175" s="2">
-        <v>99.4</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>1515167.74</v>
+        <v>1094.01</v>
       </c>
       <c r="B176" s="2">
-        <v>99.81</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>1093.83</v>
+        <v>1101.68</v>
       </c>
       <c r="B177" s="2">
         <v>99.1</v>
@@ -2330,87 +2330,87 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>199646.2</v>
+        <v>24104.74</v>
       </c>
       <c r="B178" s="2">
-        <v>99.79</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>6871.39</v>
+        <v>62081.91</v>
       </c>
       <c r="B179" s="2">
-        <v>99.45</v>
+        <v>99.72</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>403.24</v>
+        <v>3477.29</v>
       </c>
       <c r="B180" s="2">
-        <v>98.75</v>
+        <v>99.37</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>3152853.96</v>
+        <v>839.1</v>
       </c>
       <c r="B181" s="2">
-        <v>99.83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>16598.689999999999</v>
+        <v>264005.87</v>
       </c>
       <c r="B182" s="2">
-        <v>99.39</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>907.86</v>
+        <v>75581.94</v>
       </c>
       <c r="B183" s="2">
-        <v>99.1</v>
+        <v>99.69</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>11602.88</v>
+        <v>2710.9</v>
       </c>
       <c r="B184" s="2">
-        <v>99.5</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>1578.78</v>
+        <v>375550.59</v>
       </c>
       <c r="B185" s="2">
-        <v>99.1</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>20943.599999999999</v>
+        <v>2470.96</v>
       </c>
       <c r="B186" s="2">
-        <v>99.55</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>139.08000000000001</v>
+        <v>22431.05</v>
       </c>
       <c r="B187" s="2">
-        <v>93</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>36426.89</v>
+        <v>48641.9</v>
       </c>
       <c r="B188" s="2">
         <v>99.65</v>
@@ -2418,175 +2418,175 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>3500</v>
+        <v>10872.36</v>
       </c>
       <c r="B189" s="2">
-        <v>99.1</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>28564.28</v>
+        <v>2268.09</v>
       </c>
       <c r="B190" s="2">
-        <v>99.65</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>13749.05</v>
+        <v>5144.9399999999996</v>
       </c>
       <c r="B191" s="2">
-        <v>99.6</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>29344.15</v>
+        <v>25531.84</v>
       </c>
       <c r="B192" s="2">
-        <v>99.25</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>33034.29</v>
+        <v>3838.05</v>
       </c>
       <c r="B193" s="2">
-        <v>99.6</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>36391.839999999997</v>
+        <v>277695.44</v>
       </c>
       <c r="B194" s="2">
-        <v>99.7</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>3210.66</v>
+        <v>166296.44</v>
       </c>
       <c r="B195" s="2">
-        <v>99.3</v>
+        <v>99.82</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>23583.74</v>
+        <v>189894.52</v>
       </c>
       <c r="B196" s="2">
-        <v>99.3</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>873.38</v>
+        <v>201632.9</v>
       </c>
       <c r="B197" s="2">
-        <v>98</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>10802</v>
+        <v>1761.06</v>
       </c>
       <c r="B198" s="2">
-        <v>99.5</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>61553.73</v>
+        <v>37936.11</v>
       </c>
       <c r="B199" s="2">
-        <v>99.72</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>10510.02</v>
+        <v>14478.09</v>
       </c>
       <c r="B200" s="2">
-        <v>99.6</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>4789.8999999999996</v>
+        <v>7474.4</v>
       </c>
       <c r="B201" s="2">
-        <v>99.3</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>1048.1099999999999</v>
+        <v>4998.8900000000003</v>
       </c>
       <c r="B202" s="2">
-        <v>99.2</v>
+        <v>99</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>1856.87</v>
+        <v>7333.2</v>
       </c>
       <c r="B203" s="2">
-        <v>99.3</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>313.66000000000003</v>
+        <v>1342.43</v>
       </c>
       <c r="B204" s="2">
-        <v>97.5</v>
+        <v>99.26</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
-        <v>464.87</v>
+        <v>9179.9500000000007</v>
       </c>
       <c r="B205" s="2">
-        <v>98</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
-        <v>2250</v>
+        <v>557.25</v>
       </c>
       <c r="B206" s="2">
-        <v>99.3</v>
+        <v>98</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>60253.5</v>
+        <v>5100</v>
       </c>
       <c r="B207" s="2">
-        <v>99.72</v>
+        <v>99.46</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
-        <v>1040.8699999999999</v>
+        <v>440.13</v>
       </c>
       <c r="B208" s="2">
-        <v>99.2</v>
+        <v>98</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
-        <v>1472.44</v>
+        <v>1121.0899999999999</v>
       </c>
       <c r="B209" s="2">
-        <v>99.35</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>36499.019999999997</v>
+        <v>75431.03</v>
       </c>
       <c r="B210" s="2">
         <v>99.65</v>
@@ -2594,375 +2594,375 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>43885.4</v>
+        <v>89292.88</v>
       </c>
       <c r="B211" s="2">
-        <v>99.69</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>1003.46</v>
+        <v>4841.99</v>
       </c>
       <c r="B212" s="2">
-        <v>99.3</v>
+        <v>99.47</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>2362.5</v>
+        <v>6612.48</v>
       </c>
       <c r="B213" s="2">
-        <v>99.33</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
-        <v>359.28</v>
+        <v>19823.93</v>
       </c>
       <c r="B214" s="2">
-        <v>95</v>
+        <v>99.62</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
-        <v>6320.56</v>
+        <v>1386.89</v>
       </c>
       <c r="B215" s="2">
-        <v>99.05</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
-        <v>27952.41</v>
+        <v>110343.45</v>
       </c>
       <c r="B216" s="2">
-        <v>99.6</v>
+        <v>99.78</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
-        <v>62207.76</v>
+        <v>914.12</v>
       </c>
       <c r="B217" s="2">
-        <v>99.66</v>
+        <v>99</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
-        <v>54037.82</v>
+        <v>616.22</v>
       </c>
       <c r="B218" s="2">
-        <v>99.7</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
-        <v>32600</v>
+        <v>2318.23</v>
       </c>
       <c r="B219" s="2">
-        <v>99.7</v>
+        <v>99.46</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
-        <v>79139.56</v>
+        <v>166199.21</v>
       </c>
       <c r="B220" s="2">
-        <v>99.72</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>1600</v>
+        <v>113899.23</v>
       </c>
       <c r="B221" s="2">
-        <v>99.2</v>
+        <v>99.78</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
-        <v>3617.2</v>
+        <v>21758.43</v>
       </c>
       <c r="B222" s="2">
-        <v>99.35</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
-        <v>1023.95</v>
+        <v>5034.3599999999997</v>
       </c>
       <c r="B223" s="2">
-        <v>99.2</v>
+        <v>99.47</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
-        <v>63622.55</v>
+        <v>88558.35</v>
       </c>
       <c r="B224" s="2">
-        <v>99.72</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>318400.19</v>
+        <v>128022.86</v>
       </c>
       <c r="B225" s="2">
-        <v>99.78</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
-        <v>241.13</v>
+        <v>43637.32</v>
       </c>
       <c r="B226" s="2">
-        <v>96</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>93275.33</v>
+        <v>680.06</v>
       </c>
       <c r="B227" s="2">
-        <v>99.78</v>
+        <v>99</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>582.74</v>
+        <v>63573.13</v>
       </c>
       <c r="B228" s="2">
-        <v>99</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
-        <v>484.48</v>
+        <v>5881.94</v>
       </c>
       <c r="B229" s="2">
-        <v>96</v>
+        <v>99.61</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
-        <v>1470.14</v>
+        <v>22838.31</v>
       </c>
       <c r="B230" s="2">
-        <v>99.3</v>
+        <v>99.57</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
-        <v>721.74</v>
+        <v>770.88</v>
       </c>
       <c r="B231" s="2">
-        <v>99.05</v>
+        <v>99.08</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
-        <v>34196.36</v>
+        <v>3432.08</v>
       </c>
       <c r="B232" s="2">
-        <v>99.67</v>
+        <v>99.57</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
-        <v>86978.16</v>
+        <v>2800</v>
       </c>
       <c r="B233" s="2">
-        <v>99.75</v>
+        <v>99.22</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
-        <v>3147.88</v>
+        <v>17438.22</v>
       </c>
       <c r="B234" s="2">
-        <v>99.3</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>340263.59</v>
+        <v>140000</v>
       </c>
       <c r="B235" s="2">
-        <v>99.78</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>1654.75</v>
+        <v>508.09</v>
       </c>
       <c r="B236" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>2278.33</v>
+        <v>495.1</v>
       </c>
       <c r="B237" s="2">
-        <v>99.3</v>
+        <v>99</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>4865.71</v>
+        <v>4413.0200000000004</v>
       </c>
       <c r="B238" s="2">
-        <v>99.4</v>
+        <v>99</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>1961.53</v>
+        <v>148203.47</v>
       </c>
       <c r="B239" s="2">
-        <v>99.2</v>
+        <v>99.78</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
-        <v>2174.9299999999998</v>
+        <v>1442.53</v>
       </c>
       <c r="B240" s="2">
-        <v>99</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
-        <v>77109.14</v>
+        <v>19247.91</v>
       </c>
       <c r="B241" s="2">
-        <v>99.75</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
-        <v>3500</v>
+        <v>19970.61</v>
       </c>
       <c r="B242" s="2">
-        <v>99.5</v>
+        <v>99.61</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
-        <v>2498.0500000000002</v>
+        <v>18193.52</v>
       </c>
       <c r="B243" s="2">
-        <v>99.4</v>
+        <v>99.62</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
-        <v>2127569.62</v>
+        <v>33227.019999999997</v>
       </c>
       <c r="B244" s="2">
-        <v>99.82</v>
+        <v>99.66</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
-        <v>2472.88</v>
+        <v>128.11000000000001</v>
       </c>
       <c r="B245" s="2">
-        <v>99.3</v>
+        <v>93</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
-        <v>17509.400000000001</v>
+        <v>6391.35</v>
       </c>
       <c r="B246" s="2">
-        <v>99.65</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
-        <v>14619.07</v>
+        <v>133852.98000000001</v>
       </c>
       <c r="B247" s="2">
-        <v>99.3</v>
+        <v>99.78</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
-        <v>580.07000000000005</v>
+        <v>216114.15</v>
       </c>
       <c r="B248" s="2">
-        <v>98</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
-        <v>352584.61</v>
+        <v>718.51</v>
       </c>
       <c r="B249" s="2">
-        <v>99.82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
-        <v>10567.58</v>
+        <v>101652.2</v>
       </c>
       <c r="B250" s="2">
-        <v>99.25</v>
+        <v>99.78</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
-        <v>6229.31</v>
+        <v>346.98</v>
       </c>
       <c r="B251" s="2">
-        <v>99</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
-        <v>690</v>
+        <v>439923.76</v>
       </c>
       <c r="B252" s="2">
-        <v>98</v>
+        <v>99.81</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
-        <v>1967.1</v>
+        <v>80000</v>
       </c>
       <c r="B253" s="2">
-        <v>99.3</v>
+        <v>99.74</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
-        <v>28709.74</v>
+        <v>187371.89</v>
       </c>
       <c r="B254" s="2">
-        <v>99.6</v>
+        <v>99.78</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
-        <v>651.36</v>
+        <v>1137.24</v>
       </c>
       <c r="B255" s="2">
-        <v>98</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
-        <v>159803.97</v>
+        <v>2669.73</v>
       </c>
       <c r="B256" s="2">
-        <v>99.75</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
-        <v>990.31</v>
+        <v>952.51</v>
       </c>
       <c r="B257" s="2">
         <v>99</v>
@@ -2970,203 +2970,126 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
-        <v>3030</v>
+        <v>186350.28</v>
       </c>
       <c r="B258" s="2">
-        <v>99</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
-        <v>156980.94</v>
+        <v>424109.85</v>
       </c>
       <c r="B259" s="2">
-        <v>99.79</v>
+        <v>99.81</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
-        <v>25275.89</v>
+        <v>302.87</v>
       </c>
       <c r="B260" s="2">
-        <v>99.2</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
-        <v>13370.05</v>
+        <v>280.66000000000003</v>
       </c>
       <c r="B261" s="2">
-        <v>99.6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
-        <v>6879.34</v>
+        <v>6316.68</v>
       </c>
       <c r="B262" s="2">
-        <v>99.6</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
-        <v>3017062.22</v>
+        <v>933.79</v>
       </c>
       <c r="B263" s="2">
-        <v>99.85</v>
+        <v>99</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
-        <v>447031.91</v>
+        <v>2786.2</v>
       </c>
       <c r="B264" s="2">
-        <v>99.81</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
-        <v>28192.54</v>
+        <v>4781.01</v>
       </c>
       <c r="B265" s="2">
-        <v>99.65</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
-        <v>4240.0600000000004</v>
+        <v>1952.42</v>
       </c>
       <c r="B266" s="2">
-        <v>99.45</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="1">
-        <v>150585.21</v>
-      </c>
-      <c r="B267" s="2">
-        <v>99.8</v>
-      </c>
+      <c r="B267" s="2"/>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="1">
-        <v>104934.71</v>
-      </c>
-      <c r="B268" s="2">
-        <v>99.8</v>
-      </c>
+      <c r="B268" s="2"/>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="1">
-        <v>61079.67</v>
-      </c>
-      <c r="B269" s="2">
-        <v>99.72</v>
-      </c>
+      <c r="B269" s="2"/>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="1">
-        <v>621809.68999999994</v>
-      </c>
-      <c r="B270" s="2">
-        <v>99.82</v>
-      </c>
+      <c r="B270" s="2"/>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="1">
-        <v>1869.56</v>
-      </c>
-      <c r="B271" s="2">
-        <v>99.3</v>
-      </c>
+      <c r="B271" s="2"/>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="1">
-        <v>453651.18</v>
-      </c>
-      <c r="B272" s="2">
-        <v>99.81</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="1">
-        <v>62730.96</v>
-      </c>
-      <c r="B273" s="2">
-        <v>99.72</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="1">
-        <v>23621.26</v>
-      </c>
-      <c r="B274" s="2">
-        <v>99.65</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="1">
-        <v>110145.46</v>
-      </c>
-      <c r="B275" s="2">
-        <v>99.8</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="1">
-        <v>2197.5700000000002</v>
-      </c>
-      <c r="B276" s="2">
-        <v>99.3</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="1">
-        <v>401.67</v>
-      </c>
-      <c r="B277" s="2">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="1">
-        <v>487.17</v>
-      </c>
-      <c r="B278" s="2">
-        <v>98.5</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="1">
-        <v>127047.01</v>
-      </c>
-      <c r="B279" s="2">
-        <v>99.8</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="1">
-        <v>4065.67</v>
-      </c>
-      <c r="B280" s="2">
-        <v>99.45</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="1">
-        <v>41393.57</v>
-      </c>
-      <c r="B281" s="2">
-        <v>99.66</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="1">
-        <v>493.85</v>
-      </c>
-      <c r="B282" s="2">
-        <v>98.5</v>
-      </c>
+      <c r="B272" s="2"/>
+    </row>
+    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B273" s="2"/>
+    </row>
+    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B274" s="2"/>
+    </row>
+    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B275" s="2"/>
+    </row>
+    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B276" s="2"/>
+    </row>
+    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B277" s="2"/>
+    </row>
+    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B278" s="2"/>
+    </row>
+    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B279" s="2"/>
+    </row>
+    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B280" s="2"/>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B281" s="2"/>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B282" s="2"/>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B283" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modelo predictivo notas de credito semana 20 de octubre
</commit_message>
<xml_diff>
--- a/data/NC_semanal.xlsx
+++ b/data/NC_semanal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Desktop\MetrovaloresApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62F5C20-669C-40C8-A45C-78CC49433B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06410918-EBD7-4DE7-8F5C-B43D9744662D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{9E78C8B1-ED59-4A81-8FF9-F1A88ED1C1A0}"/>
   </bookViews>
@@ -373,7 +373,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -503,6 +503,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -549,10 +562,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="18" fillId="33" borderId="10" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="18" fillId="33" borderId="11" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -931,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077B50AF-9C9F-4CF5-BB56-A27ACF5565DE}">
   <dimension ref="A1:B389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A374" workbookViewId="0">
-      <selection activeCell="A389" sqref="A389"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,175 +964,175 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>19483.759999999998</v>
+        <v>1062.77</v>
       </c>
       <c r="B2" s="2">
-        <v>99.65</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>3177.58</v>
+        <v>2619.98</v>
       </c>
       <c r="B3" s="2">
-        <v>99.4</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>5103</v>
+        <v>2365.84</v>
       </c>
       <c r="B4" s="2">
-        <v>99.4</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>1156838.6299999999</v>
+        <v>78280.11</v>
       </c>
       <c r="B5" s="2">
-        <v>99.83</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>2633.28</v>
+        <v>20373.650000000001</v>
       </c>
       <c r="B6" s="2">
-        <v>99.35</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>9601.69</v>
+        <v>439423.47</v>
       </c>
       <c r="B7" s="2">
-        <v>99.3</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>5109.2700000000004</v>
+        <v>1766272.97</v>
       </c>
       <c r="B8" s="2">
-        <v>99.45</v>
+        <v>99.81</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>1268.9000000000001</v>
+        <v>593.45000000000005</v>
       </c>
       <c r="B9" s="2">
-        <v>99.35</v>
+        <v>98.9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>332.67</v>
+        <v>151361.76999999999</v>
       </c>
       <c r="B10" s="2">
-        <v>95</v>
+        <v>99.66</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>718967.8</v>
+        <v>420855.24</v>
       </c>
       <c r="B11" s="2">
-        <v>99.832300000000004</v>
+        <v>99.74</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>3788.84</v>
+        <v>82749.009999999995</v>
       </c>
       <c r="B12" s="2">
-        <v>99.05</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>12664.5</v>
+        <v>44571.88</v>
       </c>
       <c r="B13" s="2">
-        <v>99.1</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>1941.6</v>
+        <v>33847.11</v>
       </c>
       <c r="B14" s="2">
-        <v>99.15</v>
+        <v>99.57</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>5926.96</v>
+        <v>680.35</v>
       </c>
       <c r="B15" s="2">
-        <v>99.5</v>
+        <v>98.9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>4597.5</v>
+        <v>30965.35</v>
       </c>
       <c r="B16" s="2">
-        <v>99.47</v>
+        <v>99.56</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>210219.93</v>
+        <v>13564.64</v>
       </c>
       <c r="B17" s="2">
-        <v>99.82</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>249834.55</v>
+        <v>10948.79</v>
       </c>
       <c r="B18" s="2">
-        <v>99.81</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>12243</v>
+        <v>562.91999999999996</v>
       </c>
       <c r="B19" s="2">
-        <v>99.65</v>
+        <v>98.9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>2346.67</v>
+        <v>46705.279999999999</v>
       </c>
       <c r="B20" s="2">
-        <v>99.45</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>632.55999999999995</v>
+        <v>175337.55</v>
       </c>
       <c r="B21" s="2">
-        <v>99</v>
+        <v>99.66</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>40100.400000000001</v>
+        <v>178802.52</v>
       </c>
       <c r="B22" s="2">
-        <v>99.65</v>
+        <v>99.66</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>19936.48</v>
+        <v>50752.66</v>
       </c>
       <c r="B23" s="2">
         <v>99.6</v>
@@ -1126,303 +1140,303 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>150000</v>
+        <v>1488.29</v>
       </c>
       <c r="B24" s="2">
-        <v>99.825000000000003</v>
+        <v>99.05</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>19230.16</v>
+        <v>16154.34</v>
       </c>
       <c r="B25" s="2">
-        <v>99.650099999999995</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>2044.8</v>
+        <v>13506.34</v>
       </c>
       <c r="B26" s="2">
-        <v>99.3</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>100000</v>
+        <v>2172.86</v>
       </c>
       <c r="B27" s="2">
-        <v>99.82</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>109170.26</v>
+        <v>562.17999999999995</v>
       </c>
       <c r="B28" s="2">
-        <v>99.8</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>13012.05</v>
+        <v>21727.54</v>
       </c>
       <c r="B29" s="2">
-        <v>99.72</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>440.08</v>
+        <v>5257.42</v>
       </c>
       <c r="B30" s="2">
-        <v>98</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>6309.07</v>
+        <v>335449.78000000003</v>
       </c>
       <c r="B31" s="2">
-        <v>99.55</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>659717.56999999995</v>
+        <v>262772.74</v>
       </c>
       <c r="B32" s="2">
-        <v>99.83</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>2045.55</v>
+        <v>160000</v>
       </c>
       <c r="B33" s="2">
-        <v>99.4</v>
+        <v>99.66</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>1082.9100000000001</v>
+        <v>173672.74</v>
       </c>
       <c r="B34" s="2">
-        <v>99.4</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>1920.63</v>
+        <v>303268.67</v>
       </c>
       <c r="B35" s="2">
-        <v>99.4</v>
+        <v>99.74</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>23785.03</v>
+        <v>263237.71999999997</v>
       </c>
       <c r="B36" s="2">
-        <v>99.65</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>71691.86</v>
+        <v>55241.43</v>
       </c>
       <c r="B37" s="2">
-        <v>99.671000000000006</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>197.15</v>
+        <v>29938.78</v>
       </c>
       <c r="B38" s="2">
-        <v>98</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>608</v>
+        <v>17953.150000000001</v>
       </c>
       <c r="B39" s="2">
-        <v>99</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>997.13</v>
+        <v>5592.45</v>
       </c>
       <c r="B40" s="2">
-        <v>99</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>3813.69</v>
+        <v>1503.83</v>
       </c>
       <c r="B41" s="2">
-        <v>99.1</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>2970.78</v>
+        <v>2452.89</v>
       </c>
       <c r="B42" s="2">
-        <v>99.05</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>1561.99</v>
+        <v>25685.09</v>
       </c>
       <c r="B43" s="2">
-        <v>99.36</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>102115.66</v>
+        <v>367.2</v>
       </c>
       <c r="B44" s="2">
-        <v>99.8</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>641.42999999999995</v>
+        <v>66756.53</v>
       </c>
       <c r="B45" s="2">
-        <v>99</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>560.01</v>
+        <v>1449.61</v>
       </c>
       <c r="B46" s="2">
-        <v>98.75</v>
+        <v>99.1905</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>133.05000000000001</v>
+        <v>2046</v>
       </c>
       <c r="B47" s="2">
-        <v>98.5</v>
+        <v>99.26</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>185914.02</v>
+        <v>879.76</v>
       </c>
       <c r="B48" s="2">
-        <v>99.78</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>16777.66</v>
+        <v>9641.39</v>
       </c>
       <c r="B49" s="2">
-        <v>99.65</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>16180.93</v>
+        <v>331257.40000000002</v>
       </c>
       <c r="B50" s="2">
-        <v>99.65</v>
+        <v>99.74</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>5522.46</v>
+        <v>42499.99</v>
       </c>
       <c r="B51" s="2">
-        <v>99.5</v>
+        <v>99.51</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>43616.6</v>
+        <v>10342.59</v>
       </c>
       <c r="B52" s="2">
-        <v>99.7</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>378000.2</v>
+        <v>92267.98</v>
       </c>
       <c r="B53" s="2">
-        <v>99.82</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>166729.67000000001</v>
+        <v>20444.32</v>
       </c>
       <c r="B54" s="2">
-        <v>99.8</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>836.59</v>
+        <v>7663.43</v>
       </c>
       <c r="B55" s="2">
-        <v>99</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>18800</v>
+        <v>21300.04</v>
       </c>
       <c r="B56" s="2">
-        <v>99.6</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>2444.33</v>
+        <v>3402.13</v>
       </c>
       <c r="B57" s="2">
-        <v>99.38</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>5800</v>
+        <v>443922.84</v>
       </c>
       <c r="B58" s="2">
-        <v>99.4</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>1074.72</v>
+        <v>1091.26</v>
       </c>
       <c r="B59" s="2">
-        <v>99.2</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>7759.15</v>
+        <v>6687.45</v>
       </c>
       <c r="B60" s="2">
-        <v>99.55</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>668.16</v>
+        <v>2087.23</v>
       </c>
       <c r="B61" s="2">
         <v>99</v>
@@ -1430,263 +1444,263 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>1167.42</v>
+        <v>33485.24</v>
       </c>
       <c r="B62" s="2">
-        <v>99.25</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>1193.43</v>
+        <v>2072.7199999999998</v>
       </c>
       <c r="B63" s="2">
-        <v>99.3</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>2654.28</v>
+        <v>1081.74</v>
       </c>
       <c r="B64" s="2">
-        <v>99.4</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>638489.93999999994</v>
+        <v>494.13</v>
       </c>
       <c r="B65" s="2">
-        <v>99.82</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>3522.61</v>
+        <v>3105.86</v>
       </c>
       <c r="B66" s="2">
-        <v>99.45</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>86070.68</v>
+        <v>27256.799999999999</v>
       </c>
       <c r="B67" s="2">
-        <v>99.7</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>933.79</v>
+        <v>4488.5</v>
       </c>
       <c r="B68" s="2">
-        <v>99</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>65706.720000000001</v>
+        <v>14071.76</v>
       </c>
       <c r="B69" s="2">
-        <v>99.69</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>62682.3</v>
+        <v>310.36</v>
       </c>
       <c r="B70" s="2">
-        <v>99.65</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>4708.54</v>
+        <v>25482.11</v>
       </c>
       <c r="B71" s="2">
-        <v>99.45</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>2243.33</v>
+        <v>209413.57</v>
       </c>
       <c r="B72" s="2">
-        <v>99.2</v>
+        <v>99.67</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>35617.03</v>
+        <v>50000</v>
       </c>
       <c r="B73" s="2">
-        <v>99.67</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>219885.01</v>
+        <v>3549.35</v>
       </c>
       <c r="B74" s="2">
-        <v>99.825000000000003</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>114524.93</v>
+        <v>22908.720000000001</v>
       </c>
       <c r="B75" s="2">
-        <v>99.79</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>1977.99</v>
+        <v>726.21</v>
       </c>
       <c r="B76" s="2">
-        <v>99.1</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>785.28</v>
+        <v>803.19</v>
       </c>
       <c r="B77" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>457.64</v>
+        <v>2723.85</v>
       </c>
       <c r="B78" s="2">
-        <v>97</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>1970</v>
+        <v>1683.52</v>
       </c>
       <c r="B79" s="2">
-        <v>99.1</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>3617.13</v>
+        <v>748.61</v>
       </c>
       <c r="B80" s="2">
-        <v>99.15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>1468.93</v>
+        <v>170895.61</v>
       </c>
       <c r="B81" s="2">
-        <v>99.3</v>
+        <v>99.67</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>138057.44</v>
+        <v>58275.67</v>
       </c>
       <c r="B82" s="2">
-        <v>99.811000000000007</v>
+        <v>99.53</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>66389.09</v>
+        <v>5500</v>
       </c>
       <c r="B83" s="2">
-        <v>99.7</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>89000</v>
+        <v>1544.97</v>
       </c>
       <c r="B84" s="2">
-        <v>99.75</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>53203.78</v>
+        <v>4401.03</v>
       </c>
       <c r="B85" s="2">
-        <v>99.55</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>3875</v>
+        <v>4981.8100000000004</v>
       </c>
       <c r="B86" s="2">
-        <v>99.05</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>860.48</v>
+        <v>1094.52</v>
       </c>
       <c r="B87" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>1699.57</v>
+        <v>563540.86</v>
       </c>
       <c r="B88" s="2">
-        <v>99</v>
+        <v>99.78</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>544.49</v>
+        <v>14000</v>
       </c>
       <c r="B89" s="2">
-        <v>99.02</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>140360.43</v>
+        <v>1288.99</v>
       </c>
       <c r="B90" s="2">
-        <v>99.81</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>21770.44</v>
+        <v>36009.550000000003</v>
       </c>
       <c r="B91" s="2">
-        <v>99.671999999999997</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>14266.33</v>
+        <v>2296.23</v>
       </c>
       <c r="B92" s="2">
-        <v>99.5</v>
+        <v>99.15</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>3471.88</v>
+        <v>24588.73</v>
       </c>
       <c r="B93" s="2">
-        <v>99.47</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>6307.47</v>
+        <v>69388.42</v>
       </c>
       <c r="B94" s="2">
         <v>99.55</v>
@@ -1694,15 +1708,15 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>586.12</v>
+        <v>66860</v>
       </c>
       <c r="B95" s="2">
-        <v>98.5</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>22661.200000000001</v>
+        <v>112177.4</v>
       </c>
       <c r="B96" s="2">
         <v>99.7</v>
@@ -1710,119 +1724,119 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>1425.4</v>
+        <v>3228.53</v>
       </c>
       <c r="B97" s="2">
-        <v>99.1</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>1338.09</v>
+        <v>6141.92</v>
       </c>
       <c r="B98" s="2">
-        <v>99.31</v>
+        <v>99.15</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>157739.75</v>
+        <v>700</v>
       </c>
       <c r="B99" s="2">
-        <v>99.81</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>15100</v>
+        <v>3470.11</v>
       </c>
       <c r="B100" s="2">
-        <v>99.55</v>
+        <v>99.15</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>670296.88</v>
+        <v>1428.38</v>
       </c>
       <c r="B101" s="2">
-        <v>99.832300000000004</v>
+        <v>99.22</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>17961.189999999999</v>
+        <v>92501.65</v>
       </c>
       <c r="B102" s="2">
-        <v>99.72</v>
+        <v>99.63</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>5395.2</v>
+        <v>469.19</v>
       </c>
       <c r="B103" s="2">
-        <v>99.5</v>
+        <v>97</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>5700.62</v>
+        <v>4981.25</v>
       </c>
       <c r="B104" s="2">
-        <v>99.5</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>3704.51</v>
+        <v>147355.1</v>
       </c>
       <c r="B105" s="2">
-        <v>99.4</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>24124.92</v>
+        <v>1196.53</v>
       </c>
       <c r="B106" s="2">
-        <v>99.674999999999997</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>5222.62</v>
+        <v>1491.08</v>
       </c>
       <c r="B107" s="2">
-        <v>99.56</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>19191.54</v>
+        <v>6489.43</v>
       </c>
       <c r="B108" s="2">
-        <v>99.68</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>16140.44</v>
+        <v>8000</v>
       </c>
       <c r="B109" s="2">
-        <v>99.650099999999995</v>
+        <v>99.41</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>515099.06</v>
+        <v>412294.84</v>
       </c>
       <c r="B110" s="2">
-        <v>99.82</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>5925.4</v>
+        <v>17796.16</v>
       </c>
       <c r="B111" s="2">
         <v>99.55</v>
@@ -1830,7 +1844,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>734.65</v>
+        <v>877.42</v>
       </c>
       <c r="B112" s="2">
         <v>99</v>
@@ -1838,167 +1852,167 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>31202.97</v>
+        <v>2990.76</v>
       </c>
       <c r="B113" s="2">
-        <v>99.61</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>5093.25</v>
+        <v>802.91</v>
       </c>
       <c r="B114" s="2">
-        <v>99.05</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>7832.81</v>
+        <v>212715.79</v>
       </c>
       <c r="B115" s="2">
-        <v>99</v>
+        <v>99.72</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>16982.88</v>
+        <v>1633.63</v>
       </c>
       <c r="B116" s="2">
-        <v>99.15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>24514.3</v>
+        <v>27940.57</v>
       </c>
       <c r="B117" s="2">
-        <v>99.68</v>
+        <v>99.46</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>33190.53</v>
+        <v>3653.94</v>
       </c>
       <c r="B118" s="2">
-        <v>99.65</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>250000</v>
+        <v>1533.09</v>
       </c>
       <c r="B119" s="2">
-        <v>99.814999999999998</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>1108.9000000000001</v>
+        <v>600</v>
       </c>
       <c r="B120" s="2">
-        <v>99.3</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>963.95</v>
+        <v>1865277.23</v>
       </c>
       <c r="B121" s="2">
-        <v>99.05</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>540.04999999999995</v>
+        <v>467906.16</v>
       </c>
       <c r="B122" s="2">
-        <v>96</v>
+        <v>99.74</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>22786.78</v>
+        <v>44834.86</v>
       </c>
       <c r="B123" s="2">
-        <v>99.65</v>
+        <v>99.52</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>6137.69</v>
+        <v>80775.56</v>
       </c>
       <c r="B124" s="2">
-        <v>99.35</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>144.04</v>
+        <v>592.11</v>
       </c>
       <c r="B125" s="2">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>1554.09</v>
+        <v>3240.09</v>
       </c>
       <c r="B126" s="2">
-        <v>99.05</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>4092.12</v>
+        <v>754.69</v>
       </c>
       <c r="B127" s="2">
-        <v>99.4405</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>49746.78</v>
+        <v>6483.91</v>
       </c>
       <c r="B128" s="2">
-        <v>99.65</v>
+        <v>99</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>1741.28</v>
+        <v>276473.68</v>
       </c>
       <c r="B129" s="2">
-        <v>99.3</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>2818.55</v>
+        <v>23148.36</v>
       </c>
       <c r="B130" s="2">
-        <v>99.350499999999997</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>184834.79</v>
+        <v>34126.9</v>
       </c>
       <c r="B131" s="2">
-        <v>99.81</v>
+        <v>99.410499999999999</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>392.66</v>
+        <v>673.6</v>
       </c>
       <c r="B132" s="2">
-        <v>97.55</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>6021.13</v>
+        <v>22304.74</v>
       </c>
       <c r="B133" s="2">
         <v>99.45</v>
@@ -2006,327 +2020,327 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>4208</v>
+        <v>3341.55</v>
       </c>
       <c r="B134" s="2">
-        <v>99.5</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>61427.63</v>
+        <v>8145.25</v>
       </c>
       <c r="B135" s="2">
-        <v>99.7</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>21646.16</v>
+        <v>302.38</v>
       </c>
       <c r="B136" s="2">
-        <v>99.65</v>
+        <v>97</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>171115.66</v>
+        <v>1027.55</v>
       </c>
       <c r="B137" s="2">
-        <v>99.82</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>104267.17</v>
+        <v>2604.9699999999998</v>
       </c>
       <c r="B138" s="2">
-        <v>99.79</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>705.25</v>
+        <v>17691.73</v>
       </c>
       <c r="B139" s="2">
-        <v>99</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>26609.46</v>
+        <v>65504.99</v>
       </c>
       <c r="B140" s="2">
-        <v>99.5</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>30095.93</v>
+        <v>7853.75</v>
       </c>
       <c r="B141" s="2">
-        <v>99.710099999999997</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>567.15</v>
+        <v>158932.10999999999</v>
       </c>
       <c r="B142" s="2">
-        <v>98.5</v>
+        <v>99.68</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>72634.63</v>
+        <v>124237.69</v>
       </c>
       <c r="B143" s="2">
-        <v>99.8</v>
+        <v>99.66</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>1644.58</v>
+        <v>40000</v>
       </c>
       <c r="B144" s="2">
-        <v>99.35</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>1851.18</v>
+        <v>1754.86</v>
       </c>
       <c r="B145" s="2">
-        <v>99.1</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>2416.58</v>
+        <v>149901.49</v>
       </c>
       <c r="B146" s="2">
-        <v>99.35</v>
+        <v>99.700500000000005</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>432.44</v>
+        <v>3886.49</v>
       </c>
       <c r="B147" s="2">
-        <v>98.75</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>484.72</v>
+        <v>129.55000000000001</v>
       </c>
       <c r="B148" s="2">
-        <v>98.75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>24725.29</v>
+        <v>2665.28</v>
       </c>
       <c r="B149" s="2">
-        <v>99.7</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>1084.9000000000001</v>
+        <v>1029.45</v>
       </c>
       <c r="B150" s="2">
-        <v>99.3</v>
+        <v>99.15</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>20203.7</v>
+        <v>25275.74</v>
       </c>
       <c r="B151" s="2">
-        <v>99.65</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>72920.81</v>
+        <v>37592.83</v>
       </c>
       <c r="B152" s="2">
-        <v>99.81</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>17248.09</v>
+        <v>120721.06</v>
       </c>
       <c r="B153" s="2">
-        <v>99.2</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>214158.3</v>
+        <v>1813.98</v>
       </c>
       <c r="B154" s="2">
-        <v>99.8</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>3079.26</v>
+        <v>10000</v>
       </c>
       <c r="B155" s="2">
-        <v>99.36</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>185820.16</v>
+        <v>629.6</v>
       </c>
       <c r="B156" s="2">
-        <v>99.82</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>4905.93</v>
+        <v>53000</v>
       </c>
       <c r="B157" s="2">
-        <v>99.1</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>1638.61</v>
+        <v>530.44000000000005</v>
       </c>
       <c r="B158" s="2">
-        <v>99.05</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>605.59</v>
+        <v>80000</v>
       </c>
       <c r="B159" s="2">
-        <v>97</v>
+        <v>99.62</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>15270.09</v>
+        <v>196711.15</v>
       </c>
       <c r="B160" s="2">
-        <v>99.65</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>608.27</v>
+        <v>111389.01</v>
       </c>
       <c r="B161" s="2">
-        <v>98.760099999999994</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>155240.43</v>
+        <v>306790.46999999997</v>
       </c>
       <c r="B162" s="2">
-        <v>99.81</v>
+        <v>99.74</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>5042.1400000000003</v>
+        <v>6572.41</v>
       </c>
       <c r="B163" s="2">
-        <v>99.5</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>22610.9</v>
+        <v>11429.41</v>
       </c>
       <c r="B164" s="2">
-        <v>99.65</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>210249.91</v>
+        <v>54651.25</v>
       </c>
       <c r="B165" s="2">
-        <v>99.82</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>23753.48</v>
+        <v>2872.46</v>
       </c>
       <c r="B166" s="2">
-        <v>99.65</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>17206.07</v>
+        <v>256066.59</v>
       </c>
       <c r="B167" s="2">
-        <v>99.6</v>
+        <v>99.727999999999994</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>1461.54</v>
+        <v>420433</v>
       </c>
       <c r="B168" s="2">
-        <v>99.3</v>
+        <v>99.73</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>29833.040000000001</v>
+        <v>331098.94</v>
       </c>
       <c r="B169" s="2">
-        <v>99.7</v>
+        <v>99.73</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>80691.38</v>
+        <v>3508.82</v>
       </c>
       <c r="B170" s="2">
-        <v>99.8</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>15931.61</v>
+        <v>102349.51</v>
       </c>
       <c r="B171" s="2">
-        <v>99.65</v>
+        <v>99.62</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>10919.85</v>
+        <v>23642.79</v>
       </c>
       <c r="B172" s="2">
-        <v>99.15</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>17410.599999999999</v>
+        <v>16259.92</v>
       </c>
       <c r="B173" s="2">
-        <v>99.680199999999999</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>1351.05</v>
+        <v>14504.23</v>
       </c>
       <c r="B174" s="2">
         <v>99.35</v>
@@ -2334,55 +2348,55 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>304.3</v>
+        <v>34430.26</v>
       </c>
       <c r="B175" s="2">
-        <v>95</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>1156.32</v>
+        <v>208876.84</v>
       </c>
       <c r="B176" s="2">
-        <v>99</v>
+        <v>99.72</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>17840.98</v>
+        <v>1816.24</v>
       </c>
       <c r="B177" s="2">
-        <v>99.6</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>1939.11</v>
+        <v>1040.33</v>
       </c>
       <c r="B178" s="2">
-        <v>99.360100000000003</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>1762.67</v>
+        <v>3042.27</v>
       </c>
       <c r="B179" s="2">
-        <v>99.47</v>
+        <v>99</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>3157.36</v>
+        <v>5551.01</v>
       </c>
       <c r="B180" s="2">
-        <v>99.5</v>
+        <v>99</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>1295.55</v>
+        <v>11262</v>
       </c>
       <c r="B181" s="2">
         <v>99.1</v>
@@ -2390,1667 +2404,1175 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>1231.79</v>
+        <v>32000.07</v>
       </c>
       <c r="B182" s="2">
-        <v>99.1</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>968440.66</v>
+        <v>295.94</v>
       </c>
       <c r="B183" s="2">
-        <v>99.852000000000004</v>
+        <v>95</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>863.99</v>
+        <v>35686.36</v>
       </c>
       <c r="B184" s="2">
-        <v>99</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>1103.6400000000001</v>
+        <v>33610.949999999997</v>
       </c>
       <c r="B185" s="2">
-        <v>99</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>1104.69</v>
+        <v>2670.39</v>
       </c>
       <c r="B186" s="2">
-        <v>99</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>2043.41</v>
+        <v>1212.83</v>
       </c>
       <c r="B187" s="2">
-        <v>99</v>
+        <v>99.15</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>3385.96</v>
+        <v>1473.64</v>
       </c>
       <c r="B188" s="2">
-        <v>99.39</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>685.25</v>
+        <v>1545.45</v>
       </c>
       <c r="B189" s="2">
-        <v>97</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>63167.63</v>
+        <v>3815.4</v>
       </c>
       <c r="B190" s="2">
-        <v>99.67</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>468933.58</v>
+        <v>90000</v>
       </c>
       <c r="B191" s="2">
-        <v>99.84</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
-        <v>23496.55</v>
+        <v>6034.85</v>
       </c>
       <c r="B192" s="2">
-        <v>99.55</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
-        <v>4579.1899999999996</v>
+        <v>4576.84</v>
       </c>
       <c r="B193" s="2">
-        <v>99.41</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>2605.42</v>
+        <v>22872.82</v>
       </c>
       <c r="B194" s="2">
-        <v>99.4</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>2890.42</v>
+        <v>539.24</v>
       </c>
       <c r="B195" s="2">
-        <v>99.35</v>
+        <v>99</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
-        <v>1498.83</v>
+        <v>24478.54</v>
       </c>
       <c r="B196" s="2">
-        <v>99.3</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
-        <v>960.9</v>
+        <v>1050.79</v>
       </c>
       <c r="B197" s="2">
-        <v>99.05</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
-        <v>62058.2</v>
+        <v>1476.11</v>
       </c>
       <c r="B198" s="2">
-        <v>99.7</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
-        <v>70000</v>
+        <v>417.77</v>
       </c>
       <c r="B199" s="2">
-        <v>99.7</v>
+        <v>99</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
-        <v>1980.33</v>
+        <v>19841.330000000002</v>
       </c>
       <c r="B200" s="2">
-        <v>99.4</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
-        <v>959.28</v>
+        <v>3816.8</v>
       </c>
       <c r="B201" s="2">
-        <v>99.3</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
-        <v>73951.839999999997</v>
+        <v>3238.68</v>
       </c>
       <c r="B202" s="2">
-        <v>99.72</v>
+        <v>99.15</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
-        <v>2544.11</v>
+        <v>7559.8</v>
       </c>
       <c r="B203" s="2">
-        <v>99.4</v>
+        <v>99.36</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
-        <v>175.66</v>
+        <v>3281.92</v>
       </c>
       <c r="B204" s="2">
-        <v>96</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
-        <v>3790.21</v>
+        <v>69111.740000000005</v>
       </c>
       <c r="B205" s="2">
-        <v>99.45</v>
+        <v>99.66</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
-        <v>607.72</v>
+        <v>914.3</v>
       </c>
       <c r="B206" s="2">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
-        <v>8000</v>
+        <v>28915.99</v>
       </c>
       <c r="B207" s="2">
-        <v>99.55</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
-        <v>81775.72</v>
+        <v>69111.740000000005</v>
       </c>
       <c r="B208" s="2">
-        <v>99.801000000000002</v>
+        <v>99.73</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
-        <v>11077.09</v>
+        <v>13935.04</v>
       </c>
       <c r="B209" s="2">
-        <v>99.65</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
-        <v>305.68</v>
+        <v>233172.74</v>
       </c>
       <c r="B210" s="2">
-        <v>98</v>
+        <v>99.72</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
-        <v>99986.26</v>
+        <v>864026.68</v>
       </c>
       <c r="B211" s="2">
-        <v>99.78</v>
+        <v>99.73</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
-        <v>18374.95</v>
+        <v>7941.92</v>
       </c>
       <c r="B212" s="2">
-        <v>99.65</v>
+        <v>99.51</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
-        <v>22594.22</v>
+        <v>990.43</v>
       </c>
       <c r="B213" s="2">
-        <v>99.67</v>
+        <v>99.15</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
-        <v>210.51</v>
+        <v>40007.18</v>
       </c>
       <c r="B214" s="2">
-        <v>98</v>
+        <v>99.64</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
-        <v>32803.089999999997</v>
+        <v>967.85</v>
       </c>
       <c r="B215" s="2">
-        <v>99.67</v>
+        <v>99</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
-        <v>3822.16</v>
+        <v>11024.86</v>
       </c>
       <c r="B216" s="2">
-        <v>99.35</v>
+        <v>99.31</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
-        <v>290.58999999999997</v>
+        <v>16437.07</v>
       </c>
       <c r="B217" s="2">
-        <v>95</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
-        <v>426591.13</v>
+        <v>23227.99</v>
       </c>
       <c r="B218" s="2">
-        <v>99.814999999999998</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
-        <v>3485.85</v>
+        <v>69514.87</v>
       </c>
       <c r="B219" s="2">
-        <v>99.355000000000004</v>
+        <v>99.66</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
-        <v>3178583.5</v>
+        <v>57059.19</v>
       </c>
       <c r="B220" s="2">
-        <v>99.88</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
-        <v>5558.38</v>
+        <v>32251.86</v>
       </c>
       <c r="B221" s="2">
-        <v>99.48</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
-        <v>85963.07</v>
+        <v>985.02</v>
       </c>
       <c r="B222" s="2">
-        <v>99.81</v>
+        <v>99.15</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
-        <v>78015.08</v>
+        <v>10964.09</v>
       </c>
       <c r="B223" s="2">
-        <v>99.81</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
-        <v>33876.81</v>
+        <v>11755.65</v>
       </c>
       <c r="B224" s="2">
-        <v>99.66</v>
+        <v>99.25</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
-        <v>129987.9</v>
+        <v>2500.39</v>
       </c>
       <c r="B225" s="2">
-        <v>99.82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
-        <v>22918.14</v>
+        <v>5476.84</v>
       </c>
       <c r="B226" s="2">
-        <v>99.5</v>
+        <v>99</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
-        <v>42458.18</v>
+        <v>158976.51</v>
       </c>
       <c r="B227" s="2">
-        <v>99.65</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
-        <v>10017.459999999999</v>
+        <v>3542.86</v>
       </c>
       <c r="B228" s="2">
-        <v>99.55</v>
+        <v>99</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
-        <v>4506.3100000000004</v>
+        <v>1908.31</v>
       </c>
       <c r="B229" s="2">
-        <v>99.35</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
-        <v>75000</v>
+        <v>8275.23</v>
       </c>
       <c r="B230" s="2">
-        <v>99.75</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
-        <v>34045.42</v>
+        <v>692512.32</v>
       </c>
       <c r="B231" s="2">
-        <v>99.7</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
-        <v>1566.5</v>
+        <v>13275.85</v>
       </c>
       <c r="B232" s="2">
-        <v>99.45</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
-        <v>5977.71</v>
+        <v>5500</v>
       </c>
       <c r="B233" s="2">
-        <v>99.55</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
-        <v>1975.95</v>
+        <v>10960.3</v>
       </c>
       <c r="B234" s="2">
-        <v>99.25</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
-        <v>2163.25</v>
+        <v>2131.63</v>
       </c>
       <c r="B235" s="2">
-        <v>99.35</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
-        <v>136611.94</v>
+        <v>757.36</v>
       </c>
       <c r="B236" s="2">
-        <v>99.82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
-        <v>2772.01</v>
+        <v>27849.79</v>
       </c>
       <c r="B237" s="2">
-        <v>99.41</v>
+        <v>99.35</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
-        <v>106150.79</v>
+        <v>204674.66</v>
       </c>
       <c r="B238" s="2">
-        <v>99.825000000000003</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
-        <v>430557.39</v>
+        <v>41044.01</v>
       </c>
       <c r="B239" s="2">
-        <v>99.8</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
-        <v>380.23</v>
+        <v>66707.820000000007</v>
       </c>
       <c r="B240" s="2">
-        <v>97.500100000000003</v>
+        <v>99.66</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
-        <v>10000</v>
+        <v>21207.82</v>
       </c>
       <c r="B241" s="2">
-        <v>99.55</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
-        <v>167.02</v>
+        <v>8278.59</v>
       </c>
       <c r="B242" s="2">
-        <v>93</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
-        <v>891.93</v>
+        <v>30903.18</v>
       </c>
       <c r="B243" s="2">
-        <v>99</v>
+        <v>99.58</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
-        <v>2821.58</v>
+        <v>99818.93</v>
       </c>
       <c r="B244" s="2">
-        <v>99.3</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
-        <v>3966.87</v>
+        <v>17292.34</v>
       </c>
       <c r="B245" s="2">
-        <v>99</v>
+        <v>99.51</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
-        <v>8795.2800000000007</v>
+        <v>4738.8</v>
       </c>
       <c r="B246" s="2">
-        <v>99</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
-        <v>47398.03</v>
+        <v>330320.12</v>
       </c>
       <c r="B247" s="2">
-        <v>99.65</v>
+        <v>99.72</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
-        <v>19387.240000000002</v>
+        <v>79273.08</v>
       </c>
       <c r="B248" s="2">
-        <v>99.15</v>
+        <v>99.66</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
-        <v>25223.4</v>
+        <v>20685.53</v>
       </c>
       <c r="B249" s="2">
-        <v>99.6</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
-        <v>448.04</v>
+        <v>2477.6799999999998</v>
       </c>
       <c r="B250" s="2">
-        <v>96</v>
+        <v>99.1</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
-        <v>1506.65</v>
+        <v>38003.81</v>
       </c>
       <c r="B251" s="2">
-        <v>99.05</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
-        <v>969.42</v>
+        <v>259010.91</v>
       </c>
       <c r="B252" s="2">
-        <v>99</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
-        <v>189.35</v>
+        <v>290091.05</v>
       </c>
       <c r="B253" s="2">
-        <v>92</v>
+        <v>99.7</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
-        <v>812.62</v>
+        <v>9568.66</v>
       </c>
       <c r="B254" s="2">
-        <v>99.05</v>
+        <v>99.45</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
-        <v>2279.4</v>
+        <v>4142.7</v>
       </c>
       <c r="B255" s="2">
-        <v>99.2</v>
+        <v>99.31</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
-        <v>2170.5500000000002</v>
+        <v>133395.54999999999</v>
       </c>
       <c r="B256" s="2">
-        <v>99.2</v>
+        <v>99.67</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
-        <v>8368.73</v>
+        <v>9781.01</v>
       </c>
       <c r="B257" s="2">
-        <v>99.56</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
-        <v>1500</v>
+        <v>429.5</v>
       </c>
       <c r="B258" s="2">
-        <v>99.39</v>
+        <v>95</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
-        <v>374690.75</v>
+        <v>3928.17</v>
       </c>
       <c r="B259" s="2">
-        <v>99.82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
-        <v>3407.99</v>
+        <v>9496.83</v>
       </c>
       <c r="B260" s="2">
-        <v>99.4</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
-        <v>33201.21</v>
+        <v>4837.3900000000003</v>
       </c>
       <c r="B261" s="2">
-        <v>99.67</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
-        <v>232054.5</v>
+        <v>93.77</v>
       </c>
       <c r="B262" s="2">
-        <v>99.8</v>
+        <v>91</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
-        <v>57673.16</v>
+        <v>110550.82</v>
       </c>
       <c r="B263" s="2">
-        <v>99.7</v>
+        <v>99.69</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
-        <v>3146.57</v>
+        <v>13411.55</v>
       </c>
       <c r="B264" s="2">
-        <v>99.3</v>
+        <v>99.4</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
-        <v>198725.56</v>
+        <v>516.57000000000005</v>
       </c>
       <c r="B265" s="2">
-        <v>99.8</v>
+        <v>99</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="2">
-        <v>7000</v>
-      </c>
-      <c r="B266" s="2">
-        <v>99.55</v>
+      <c r="A266" s="3">
+        <v>1092.2</v>
+      </c>
+      <c r="B266" s="3">
+        <v>99</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="2">
-        <v>11606.52</v>
-      </c>
-      <c r="B267" s="2">
-        <v>99.45</v>
-      </c>
+      <c r="A267" s="2"/>
+      <c r="B267" s="2"/>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="2">
-        <v>16944.490000000002</v>
-      </c>
-      <c r="B268" s="2">
-        <v>99.6</v>
-      </c>
+      <c r="A268" s="2"/>
+      <c r="B268" s="2"/>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="2">
-        <v>704.35</v>
-      </c>
-      <c r="B269" s="2">
-        <v>98.65</v>
-      </c>
+      <c r="A269" s="2"/>
+      <c r="B269" s="2"/>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="2">
-        <v>2019.91</v>
-      </c>
-      <c r="B270" s="2">
-        <v>99.355000000000004</v>
-      </c>
+      <c r="A270" s="2"/>
+      <c r="B270" s="2"/>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="2">
-        <v>35906.5</v>
-      </c>
-      <c r="B271" s="2">
-        <v>99.67</v>
-      </c>
+      <c r="A271" s="2"/>
+      <c r="B271" s="2"/>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="2">
-        <v>751.77</v>
-      </c>
-      <c r="B272" s="2">
-        <v>98.5</v>
-      </c>
+      <c r="A272" s="2"/>
+      <c r="B272" s="2"/>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="2">
-        <v>1221.8800000000001</v>
-      </c>
-      <c r="B273" s="2">
-        <v>99.33</v>
-      </c>
+      <c r="A273" s="2"/>
+      <c r="B273" s="2"/>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="2">
-        <v>1906.22</v>
-      </c>
-      <c r="B274" s="2">
-        <v>99.4</v>
-      </c>
+      <c r="A274" s="2"/>
+      <c r="B274" s="2"/>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="2">
-        <v>14706.76</v>
-      </c>
-      <c r="B275" s="2">
-        <v>99.6</v>
-      </c>
+      <c r="A275" s="2"/>
+      <c r="B275" s="2"/>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="2">
-        <v>4737.22</v>
-      </c>
-      <c r="B276" s="2">
-        <v>99.41</v>
-      </c>
+      <c r="A276" s="2"/>
+      <c r="B276" s="2"/>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="2">
-        <v>159123.74</v>
-      </c>
-      <c r="B277" s="2">
-        <v>99.75</v>
-      </c>
+      <c r="A277" s="2"/>
+      <c r="B277" s="2"/>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="2">
-        <v>3463.06</v>
-      </c>
-      <c r="B278" s="2">
-        <v>99.56</v>
-      </c>
+      <c r="A278" s="2"/>
+      <c r="B278" s="2"/>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="2">
-        <v>4198.3500000000004</v>
-      </c>
-      <c r="B279" s="2">
-        <v>99.56</v>
-      </c>
+      <c r="A279" s="2"/>
+      <c r="B279" s="2"/>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="2">
-        <v>6600</v>
-      </c>
-      <c r="B280" s="2">
-        <v>99.55</v>
-      </c>
+      <c r="A280" s="2"/>
+      <c r="B280" s="2"/>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="2">
-        <v>12632.97</v>
-      </c>
-      <c r="B281" s="2">
-        <v>99.6</v>
-      </c>
+      <c r="A281" s="2"/>
+      <c r="B281" s="2"/>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="2">
-        <v>45020.57</v>
-      </c>
-      <c r="B282" s="2">
-        <v>99.7</v>
-      </c>
+      <c r="A282" s="2"/>
+      <c r="B282" s="2"/>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="2">
-        <v>13362.94</v>
-      </c>
-      <c r="B283" s="2">
-        <v>99.55</v>
-      </c>
+      <c r="A283" s="2"/>
+      <c r="B283" s="2"/>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="2">
-        <v>18610.53</v>
-      </c>
-      <c r="B284" s="2">
-        <v>99.55</v>
-      </c>
+      <c r="A284" s="2"/>
+      <c r="B284" s="2"/>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="2">
-        <v>51083.62</v>
-      </c>
-      <c r="B285" s="2">
-        <v>99.65</v>
-      </c>
+      <c r="A285" s="2"/>
+      <c r="B285" s="2"/>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="2">
-        <v>39253.06</v>
-      </c>
-      <c r="B286" s="2">
-        <v>99.65</v>
-      </c>
+      <c r="A286" s="2"/>
+      <c r="B286" s="2"/>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="2">
-        <v>2391.5</v>
-      </c>
-      <c r="B287" s="2">
-        <v>99.35</v>
-      </c>
+      <c r="A287" s="2"/>
+      <c r="B287" s="2"/>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="2">
-        <v>339558.89</v>
-      </c>
-      <c r="B288" s="2">
-        <v>99.82</v>
-      </c>
+      <c r="A288" s="2"/>
+      <c r="B288" s="2"/>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="2">
-        <v>2935.44</v>
-      </c>
-      <c r="B289" s="2">
-        <v>99.4</v>
-      </c>
+      <c r="A289" s="2"/>
+      <c r="B289" s="2"/>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="2">
-        <v>1898.1</v>
-      </c>
-      <c r="B290" s="2">
-        <v>99.3</v>
-      </c>
+      <c r="A290" s="2"/>
+      <c r="B290" s="2"/>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="2">
-        <v>29586.45</v>
-      </c>
-      <c r="B291" s="2">
-        <v>99.55</v>
-      </c>
+      <c r="A291" s="2"/>
+      <c r="B291" s="2"/>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="2">
-        <v>1493.35</v>
-      </c>
-      <c r="B292" s="2">
-        <v>99.3</v>
-      </c>
+      <c r="A292" s="2"/>
+      <c r="B292" s="2"/>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="2">
-        <v>1670.36</v>
-      </c>
-      <c r="B293" s="2">
-        <v>99.35</v>
-      </c>
+      <c r="A293" s="2"/>
+      <c r="B293" s="2"/>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="2">
-        <v>29180</v>
-      </c>
-      <c r="B294" s="2">
-        <v>99.72</v>
-      </c>
+      <c r="A294" s="2"/>
+      <c r="B294" s="2"/>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="2">
-        <v>819.61</v>
-      </c>
-      <c r="B295" s="2">
-        <v>99</v>
-      </c>
+      <c r="A295" s="2"/>
+      <c r="B295" s="2"/>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" s="2">
-        <v>78394.960000000006</v>
-      </c>
-      <c r="B296" s="2">
-        <v>99.74</v>
-      </c>
+      <c r="A296" s="2"/>
+      <c r="B296" s="2"/>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" s="2">
-        <v>34720.82</v>
-      </c>
-      <c r="B297" s="2">
-        <v>99.67</v>
-      </c>
+      <c r="A297" s="2"/>
+      <c r="B297" s="2"/>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="2">
-        <v>440.28</v>
-      </c>
-      <c r="B298" s="2">
-        <v>99</v>
-      </c>
+      <c r="A298" s="2"/>
+      <c r="B298" s="2"/>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" s="2">
-        <v>27138.54</v>
-      </c>
-      <c r="B299" s="2">
-        <v>99.5</v>
-      </c>
+      <c r="A299" s="2"/>
+      <c r="B299" s="2"/>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" s="2">
-        <v>4250.33</v>
-      </c>
-      <c r="B300" s="2">
-        <v>99.4</v>
-      </c>
+      <c r="A300" s="2"/>
+      <c r="B300" s="2"/>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" s="2">
-        <v>27931.49</v>
-      </c>
-      <c r="B301" s="2">
-        <v>99.7</v>
-      </c>
+      <c r="A301" s="2"/>
+      <c r="B301" s="2"/>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" s="2">
-        <v>2315.58</v>
-      </c>
-      <c r="B302" s="2">
-        <v>99.35</v>
-      </c>
+      <c r="A302" s="2"/>
+      <c r="B302" s="2"/>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" s="2">
-        <v>13340.89</v>
-      </c>
-      <c r="B303" s="2">
-        <v>99.6</v>
-      </c>
+      <c r="A303" s="2"/>
+      <c r="B303" s="2"/>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" s="2">
-        <v>4649.7</v>
-      </c>
-      <c r="B304" s="2">
-        <v>99.35</v>
-      </c>
+      <c r="A304" s="2"/>
+      <c r="B304" s="2"/>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="2">
-        <v>5487.75</v>
-      </c>
-      <c r="B305" s="2">
-        <v>99.4</v>
-      </c>
+      <c r="A305" s="2"/>
+      <c r="B305" s="2"/>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306" s="2">
-        <v>378.62</v>
-      </c>
-      <c r="B306" s="2">
-        <v>97</v>
-      </c>
+      <c r="A306" s="2"/>
+      <c r="B306" s="2"/>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" s="2">
-        <v>39213.33</v>
-      </c>
-      <c r="B307" s="2">
-        <v>99.7</v>
-      </c>
+      <c r="A307" s="2"/>
+      <c r="B307" s="2"/>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="2">
-        <v>2006.21</v>
-      </c>
-      <c r="B308" s="2">
-        <v>99.4</v>
-      </c>
+      <c r="A308" s="2"/>
+      <c r="B308" s="2"/>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" s="2">
-        <v>641.33000000000004</v>
-      </c>
-      <c r="B309" s="2">
-        <v>96</v>
-      </c>
+      <c r="A309" s="2"/>
+      <c r="B309" s="2"/>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" s="2">
-        <v>5054.6400000000003</v>
-      </c>
-      <c r="B310" s="2">
-        <v>99</v>
-      </c>
+      <c r="A310" s="2"/>
+      <c r="B310" s="2"/>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" s="2">
-        <v>115092.81</v>
-      </c>
-      <c r="B311" s="2">
-        <v>99.78</v>
-      </c>
+      <c r="A311" s="2"/>
+      <c r="B311" s="2"/>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A312" s="2">
-        <v>81214.149999999994</v>
-      </c>
-      <c r="B312" s="2">
-        <v>99.72</v>
-      </c>
+      <c r="A312" s="2"/>
+      <c r="B312" s="2"/>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A313" s="2">
-        <v>22771.45</v>
-      </c>
-      <c r="B313" s="2">
-        <v>99.6</v>
-      </c>
+      <c r="A313" s="2"/>
+      <c r="B313" s="2"/>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A314" s="2">
-        <v>107733.04</v>
-      </c>
-      <c r="B314" s="2">
-        <v>99.79</v>
-      </c>
+      <c r="A314" s="2"/>
+      <c r="B314" s="2"/>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A315" s="2">
-        <v>8176.09</v>
-      </c>
-      <c r="B315" s="2">
-        <v>99.1</v>
-      </c>
+      <c r="A315" s="2"/>
+      <c r="B315" s="2"/>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A316" s="2">
-        <v>294472.7</v>
-      </c>
-      <c r="B316" s="2">
-        <v>99.81</v>
-      </c>
+      <c r="A316" s="2"/>
+      <c r="B316" s="2"/>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" s="2">
-        <v>89031.37</v>
-      </c>
-      <c r="B317" s="2">
-        <v>99.72</v>
-      </c>
+      <c r="A317" s="2"/>
+      <c r="B317" s="2"/>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318" s="2">
-        <v>738.42</v>
-      </c>
-      <c r="B318" s="2">
-        <v>99</v>
-      </c>
+      <c r="A318" s="2"/>
+      <c r="B318" s="2"/>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319" s="2">
-        <v>70000</v>
-      </c>
-      <c r="B319" s="2">
-        <v>99.72</v>
-      </c>
+      <c r="A319" s="2"/>
+      <c r="B319" s="2"/>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A320" s="2">
-        <v>15944.61</v>
-      </c>
-      <c r="B320" s="2">
-        <v>99.5</v>
-      </c>
+      <c r="A320" s="2"/>
+      <c r="B320" s="2"/>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321" s="2">
-        <v>5329.47</v>
-      </c>
-      <c r="B321" s="2">
-        <v>99.4</v>
-      </c>
+      <c r="A321" s="2"/>
+      <c r="B321" s="2"/>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A322" s="2">
-        <v>144876.71</v>
-      </c>
-      <c r="B322" s="2">
-        <v>99.79</v>
-      </c>
+      <c r="A322" s="2"/>
+      <c r="B322" s="2"/>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A323" s="2">
-        <v>602.74</v>
-      </c>
-      <c r="B323" s="2">
-        <v>99</v>
-      </c>
+      <c r="A323" s="2"/>
+      <c r="B323" s="2"/>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A324" s="2">
-        <v>1496.11</v>
-      </c>
-      <c r="B324" s="2">
-        <v>99.35</v>
-      </c>
+      <c r="A324" s="2"/>
+      <c r="B324" s="2"/>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" s="2">
-        <v>2001.69</v>
-      </c>
-      <c r="B325" s="2">
-        <v>99.35</v>
-      </c>
+      <c r="A325" s="2"/>
+      <c r="B325" s="2"/>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" s="2">
-        <v>1056.77</v>
-      </c>
-      <c r="B326" s="2">
-        <v>99.4</v>
-      </c>
+      <c r="A326" s="2"/>
+      <c r="B326" s="2"/>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327" s="2">
-        <v>234096.27</v>
-      </c>
-      <c r="B327" s="2">
-        <v>99.82</v>
-      </c>
+      <c r="A327" s="2"/>
+      <c r="B327" s="2"/>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" s="2">
-        <v>5659.8</v>
-      </c>
-      <c r="B328" s="2">
-        <v>99.504999999999995</v>
-      </c>
+      <c r="A328" s="2"/>
+      <c r="B328" s="2"/>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="2">
-        <v>5812.48</v>
-      </c>
-      <c r="B329" s="2">
-        <v>99.52</v>
-      </c>
+      <c r="A329" s="2"/>
+      <c r="B329" s="2"/>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" s="2">
-        <v>874.71</v>
-      </c>
-      <c r="B330" s="2">
-        <v>99.25</v>
-      </c>
+      <c r="A330" s="2"/>
+      <c r="B330" s="2"/>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" s="2">
-        <v>787.87</v>
-      </c>
-      <c r="B331" s="2">
-        <v>99.16</v>
-      </c>
+      <c r="A331" s="2"/>
+      <c r="B331" s="2"/>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" s="2">
-        <v>2001.3</v>
-      </c>
-      <c r="B332" s="2">
-        <v>99.45</v>
-      </c>
+      <c r="A332" s="2"/>
+      <c r="B332" s="2"/>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" s="2">
-        <v>3061.97</v>
-      </c>
-      <c r="B333" s="2">
-        <v>99.3</v>
-      </c>
+      <c r="A333" s="2"/>
+      <c r="B333" s="2"/>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" s="2">
-        <v>170690.98</v>
-      </c>
-      <c r="B334" s="2">
-        <v>99.75</v>
-      </c>
+      <c r="A334" s="2"/>
+      <c r="B334" s="2"/>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A335" s="2">
-        <v>8563.19</v>
-      </c>
-      <c r="B335" s="2">
-        <v>99.55</v>
-      </c>
+      <c r="A335" s="2"/>
+      <c r="B335" s="2"/>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A336" s="2">
-        <v>7028.74</v>
-      </c>
-      <c r="B336" s="2">
-        <v>99.560199999999995</v>
-      </c>
+      <c r="A336" s="2"/>
+      <c r="B336" s="2"/>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A337" s="2">
-        <v>445.64</v>
-      </c>
-      <c r="B337" s="2">
-        <v>99.01</v>
-      </c>
+      <c r="A337" s="2"/>
+      <c r="B337" s="2"/>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A338" s="2">
-        <v>21059.23</v>
-      </c>
-      <c r="B338" s="2">
-        <v>99.7</v>
-      </c>
+      <c r="A338" s="2"/>
+      <c r="B338" s="2"/>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A339" s="2">
-        <v>254.73</v>
-      </c>
-      <c r="B339" s="2">
-        <v>98.670100000000005</v>
-      </c>
+      <c r="A339" s="2"/>
+      <c r="B339" s="2"/>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A340" s="2">
-        <v>2982</v>
-      </c>
-      <c r="B340" s="2">
-        <v>99.58</v>
-      </c>
+      <c r="A340" s="2"/>
+      <c r="B340" s="2"/>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A341" s="2">
-        <v>493.06</v>
-      </c>
-      <c r="B341" s="2">
-        <v>99.07</v>
-      </c>
+      <c r="A341" s="2"/>
+      <c r="B341" s="2"/>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A342" s="2">
-        <v>24698.400000000001</v>
-      </c>
-      <c r="B342" s="2">
-        <v>99.6</v>
-      </c>
+      <c r="A342" s="2"/>
+      <c r="B342" s="2"/>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A343" s="2">
-        <v>1378.11</v>
-      </c>
-      <c r="B343" s="2">
-        <v>99.3</v>
-      </c>
+      <c r="A343" s="2"/>
+      <c r="B343" s="2"/>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A344" s="2">
-        <v>20485.03</v>
-      </c>
-      <c r="B344" s="2">
-        <v>99.6</v>
-      </c>
+      <c r="A344" s="2"/>
+      <c r="B344" s="2"/>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A345" s="2">
-        <v>2787.37</v>
-      </c>
-      <c r="B345" s="2">
-        <v>99.5</v>
-      </c>
+      <c r="A345" s="2"/>
+      <c r="B345" s="2"/>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A346" s="2">
-        <v>1491.66</v>
-      </c>
-      <c r="B346" s="2">
-        <v>99.05</v>
-      </c>
+      <c r="A346" s="2"/>
+      <c r="B346" s="2"/>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A347" s="2">
-        <v>307.11</v>
-      </c>
-      <c r="B347" s="2">
-        <v>94</v>
-      </c>
+      <c r="A347" s="2"/>
+      <c r="B347" s="2"/>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A348" s="2">
-        <v>156.61000000000001</v>
-      </c>
-      <c r="B348" s="2">
-        <v>93</v>
-      </c>
+      <c r="A348" s="2"/>
+      <c r="B348" s="2"/>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A349" s="2">
-        <v>480648.93</v>
-      </c>
-      <c r="B349" s="2">
-        <v>99.82</v>
-      </c>
+      <c r="A349" s="2"/>
+      <c r="B349" s="2"/>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A350" s="2">
-        <v>154999.47</v>
-      </c>
-      <c r="B350" s="2">
-        <v>99.78</v>
-      </c>
+      <c r="A350" s="2"/>
+      <c r="B350" s="2"/>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A351" s="2">
-        <v>1283.3399999999999</v>
-      </c>
-      <c r="B351" s="2">
-        <v>99.2</v>
-      </c>
+      <c r="A351" s="2"/>
+      <c r="B351" s="2"/>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A352" s="2">
-        <v>4483.07</v>
-      </c>
-      <c r="B352" s="2">
-        <v>99.55</v>
-      </c>
+      <c r="A352" s="2"/>
+      <c r="B352" s="2"/>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A353" s="2">
-        <v>2432.27</v>
-      </c>
-      <c r="B353" s="2">
-        <v>99.1</v>
-      </c>
+      <c r="A353" s="2"/>
+      <c r="B353" s="2"/>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A354" s="2">
-        <v>6112.66</v>
-      </c>
-      <c r="B354" s="2">
-        <v>99.620099999999994</v>
-      </c>
+      <c r="A354" s="2"/>
+      <c r="B354" s="2"/>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A355" s="2">
-        <v>2430.9899999999998</v>
-      </c>
-      <c r="B355" s="2">
-        <v>99.45</v>
-      </c>
+      <c r="A355" s="2"/>
+      <c r="B355" s="2"/>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A356" s="2">
-        <v>1570.78</v>
-      </c>
-      <c r="B356" s="2">
-        <v>99.1</v>
-      </c>
+      <c r="A356" s="2"/>
+      <c r="B356" s="2"/>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A357" s="2">
-        <v>257.35000000000002</v>
-      </c>
-      <c r="B357" s="2">
-        <v>95</v>
-      </c>
+      <c r="A357" s="2"/>
+      <c r="B357" s="2"/>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A358" s="2">
-        <v>1471.71</v>
-      </c>
-      <c r="B358" s="2">
-        <v>99.3</v>
-      </c>
+      <c r="A358" s="2"/>
+      <c r="B358" s="2"/>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A359" s="2">
-        <v>827.29</v>
-      </c>
-      <c r="B359" s="2">
-        <v>99</v>
-      </c>
+      <c r="A359" s="2"/>
+      <c r="B359" s="2"/>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A360" s="2">
-        <v>1994.88</v>
-      </c>
-      <c r="B360" s="2">
-        <v>99</v>
-      </c>
+      <c r="A360" s="2"/>
+      <c r="B360" s="2"/>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A361" s="2">
-        <v>50972.6</v>
-      </c>
-      <c r="B361" s="2">
-        <v>99.7</v>
-      </c>
+      <c r="A361" s="2"/>
+      <c r="B361" s="2"/>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A362" s="2">
-        <v>16386.509999999998</v>
-      </c>
-      <c r="B362" s="2">
-        <v>99.67</v>
-      </c>
+      <c r="A362" s="2"/>
+      <c r="B362" s="2"/>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A363" s="2">
-        <v>1473.18</v>
-      </c>
-      <c r="B363" s="2">
-        <v>99.3</v>
-      </c>
+      <c r="A363" s="2"/>
+      <c r="B363" s="2"/>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A364" s="2">
-        <v>149510.28</v>
-      </c>
-      <c r="B364" s="2">
-        <v>99.74</v>
-      </c>
+      <c r="A364" s="2"/>
+      <c r="B364" s="2"/>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A365" s="2">
-        <v>22089.54</v>
-      </c>
-      <c r="B365" s="2">
-        <v>99.6</v>
-      </c>
+      <c r="A365" s="2"/>
+      <c r="B365" s="2"/>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A366" s="2">
-        <v>300</v>
-      </c>
-      <c r="B366" s="2">
-        <v>98.5</v>
-      </c>
+      <c r="A366" s="2"/>
+      <c r="B366" s="2"/>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A367" s="2">
-        <v>2944.1</v>
-      </c>
-      <c r="B367" s="2">
-        <v>99.350099999999998</v>
-      </c>
+      <c r="A367" s="2"/>
+      <c r="B367" s="2"/>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A368" s="2">
-        <v>8737.57</v>
-      </c>
-      <c r="B368" s="2">
-        <v>99.45</v>
-      </c>
+      <c r="A368" s="2"/>
+      <c r="B368" s="2"/>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A369" s="2">
-        <v>1330038.6499999999</v>
-      </c>
-      <c r="B369" s="2">
-        <v>99.85</v>
-      </c>
+      <c r="A369" s="2"/>
+      <c r="B369" s="2"/>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A370" s="2">
-        <v>24447.63</v>
-      </c>
-      <c r="B370" s="2">
-        <v>99.7</v>
-      </c>
+      <c r="A370" s="2"/>
+      <c r="B370" s="2"/>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A371" s="2">
-        <v>447.66</v>
-      </c>
-      <c r="B371" s="2">
-        <v>99</v>
-      </c>
+      <c r="A371" s="2"/>
+      <c r="B371" s="2"/>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A372" s="2">
-        <v>788.81</v>
-      </c>
-      <c r="B372" s="2">
-        <v>99.1</v>
-      </c>
+      <c r="A372" s="2"/>
+      <c r="B372" s="2"/>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A373" s="2">
-        <v>1329950.1000000001</v>
-      </c>
-      <c r="B373" s="2">
-        <v>99.85</v>
-      </c>
+      <c r="A373" s="2"/>
+      <c r="B373" s="2"/>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A374" s="2">
-        <v>1610.04</v>
-      </c>
-      <c r="B374" s="2">
-        <v>99.4</v>
-      </c>
+      <c r="A374" s="2"/>
+      <c r="B374" s="2"/>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A375" s="2">
-        <v>1234.9000000000001</v>
-      </c>
-      <c r="B375" s="2">
-        <v>99.3</v>
-      </c>
+      <c r="A375" s="2"/>
+      <c r="B375" s="2"/>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A376" s="2">
-        <v>2914.98</v>
-      </c>
-      <c r="B376" s="2">
-        <v>99.35</v>
-      </c>
+      <c r="A376" s="2"/>
+      <c r="B376" s="2"/>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A377" s="2">
-        <v>352</v>
-      </c>
-      <c r="B377" s="2">
-        <v>95</v>
-      </c>
+      <c r="A377" s="2"/>
+      <c r="B377" s="2"/>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A378" s="2">
-        <v>2107.2600000000002</v>
-      </c>
-      <c r="B378" s="2">
-        <v>99.45</v>
-      </c>
+      <c r="A378" s="2"/>
+      <c r="B378" s="2"/>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A379" s="2">
-        <v>1070.95</v>
-      </c>
-      <c r="B379" s="2">
-        <v>99.25</v>
-      </c>
+      <c r="A379" s="2"/>
+      <c r="B379" s="2"/>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A380" s="2">
-        <v>2892.17</v>
-      </c>
-      <c r="B380" s="2">
-        <v>99.4</v>
-      </c>
+      <c r="A380" s="2"/>
+      <c r="B380" s="2"/>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A381" s="2">
-        <v>27740.720000000001</v>
-      </c>
-      <c r="B381" s="2">
-        <v>99.65</v>
-      </c>
+      <c r="A381" s="2"/>
+      <c r="B381" s="2"/>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A382" s="2">
-        <v>615.20000000000005</v>
-      </c>
-      <c r="B382" s="2">
-        <v>99.1</v>
-      </c>
+      <c r="A382" s="2"/>
+      <c r="B382" s="2"/>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A383" s="2">
-        <v>1134.9000000000001</v>
-      </c>
-      <c r="B383" s="2">
-        <v>99.15</v>
-      </c>
+      <c r="A383" s="2"/>
+      <c r="B383" s="2"/>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A384" s="2">
-        <v>40219.199999999997</v>
-      </c>
-      <c r="B384" s="2">
-        <v>99.76</v>
-      </c>
+      <c r="A384" s="2"/>
+      <c r="B384" s="2"/>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A385" s="2">
-        <v>146843.64000000001</v>
-      </c>
-      <c r="B385" s="2">
-        <v>99.72</v>
-      </c>
+      <c r="A385" s="2"/>
+      <c r="B385" s="2"/>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A386" s="2">
-        <v>20377.16</v>
-      </c>
-      <c r="B386" s="2">
-        <v>99.6</v>
-      </c>
+      <c r="A386" s="2"/>
+      <c r="B386" s="2"/>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A387" s="2">
-        <v>3507.91</v>
-      </c>
-      <c r="B387" s="2">
-        <v>99.5</v>
-      </c>
+      <c r="A387" s="2"/>
+      <c r="B387" s="2"/>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A388" s="2">
-        <v>101075.42</v>
-      </c>
-      <c r="B388" s="2">
-        <v>99.801000000000002</v>
-      </c>
+      <c r="A388" s="2"/>
+      <c r="B388" s="2"/>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A389" s="2">
-        <v>14934.14</v>
-      </c>
-      <c r="B389" s="2">
-        <v>99.6</v>
-      </c>
+      <c r="A389" s="2"/>
+      <c r="B389" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
notas de credito semana 12 al 16 de enero 2026
</commit_message>
<xml_diff>
--- a/data/NC_semanal.xlsx
+++ b/data/NC_semanal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Desktop\MetrovaloresApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BB7DBC-B085-467F-BCA0-4E56B9D02C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB6923B-422B-4201-942A-4FBA486FC39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{9E78C8B1-ED59-4A81-8FF9-F1A88ED1C1A0}"/>
   </bookViews>
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077B50AF-9C9F-4CF5-BB56-A27ACF5565DE}">
   <dimension ref="A1:B389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="A240" sqref="A240:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,847 +964,847 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>21162.6</v>
+        <v>2008.26</v>
       </c>
       <c r="B2" s="2">
-        <v>99.66</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>12553</v>
+        <v>54793.61</v>
       </c>
       <c r="B3" s="2">
-        <v>99.5</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>2852.9</v>
+        <v>613.41</v>
       </c>
       <c r="B4" s="2">
-        <v>99.25</v>
+        <v>96.8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>2388.9899999999998</v>
+        <v>1155.96</v>
       </c>
       <c r="B5" s="2">
-        <v>99.4</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>2031.37</v>
+        <v>10644.52</v>
       </c>
       <c r="B6" s="2">
-        <v>99.4</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>1305.8699999999999</v>
+        <v>1353.61</v>
       </c>
       <c r="B7" s="2">
-        <v>99.3</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>1102.3900000000001</v>
+        <v>3130.24</v>
       </c>
       <c r="B8" s="2">
-        <v>99.3</v>
+        <v>97.2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>7124.53</v>
+        <v>4465.5</v>
       </c>
       <c r="B9" s="2">
-        <v>99.53</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>33439.08</v>
+        <v>1259.18</v>
       </c>
       <c r="B10" s="2">
-        <v>99.6</v>
+        <v>97.510099999999994</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>38125.449999999997</v>
+        <v>4420.6899999999996</v>
       </c>
       <c r="B11" s="2">
-        <v>99.55</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>102703.84</v>
+        <v>388.15</v>
       </c>
       <c r="B12" s="2">
-        <v>99.8</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>564.66999999999996</v>
+        <v>4316.37</v>
       </c>
       <c r="B13" s="2">
-        <v>98.5</v>
+        <v>97.75</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>674.46</v>
+        <v>1073.7</v>
       </c>
       <c r="B14" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>3588.98</v>
+        <v>69306.559999999998</v>
       </c>
       <c r="B15" s="2">
-        <v>99.25</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>1218.8599999999999</v>
+        <v>674831.05</v>
       </c>
       <c r="B16" s="2">
-        <v>99.1</v>
+        <v>98.65</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>135258.49</v>
+        <v>23762.2</v>
       </c>
       <c r="B17" s="2">
-        <v>99.8</v>
+        <v>97.4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>996.45</v>
+        <v>6638.76</v>
       </c>
       <c r="B18" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>14068.91</v>
+        <v>10089.709999999999</v>
       </c>
       <c r="B19" s="2">
-        <v>99.55</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>42750.51</v>
+        <v>122321.32</v>
       </c>
       <c r="B20" s="2">
-        <v>99.82</v>
+        <v>98.42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>829.61</v>
+        <v>7373.8</v>
       </c>
       <c r="B21" s="2">
-        <v>99</v>
+        <v>97.75</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>1586.02</v>
+        <v>39049.86</v>
       </c>
       <c r="B22" s="2">
-        <v>99.3</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>23113.46</v>
+        <v>90498.16</v>
       </c>
       <c r="B23" s="2">
-        <v>99.65</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>3079.54</v>
+        <v>238170.79</v>
       </c>
       <c r="B24" s="2">
-        <v>99.4</v>
+        <v>98.42</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>83469.63</v>
+        <v>775933</v>
       </c>
       <c r="B25" s="2">
-        <v>99.731200000000001</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>1102.92</v>
+        <v>93287.32</v>
       </c>
       <c r="B26" s="2">
-        <v>99</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>1738.34</v>
+        <v>25754.639999999999</v>
       </c>
       <c r="B27" s="2">
-        <v>99</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>1586.02</v>
+        <v>45927.839999999997</v>
       </c>
       <c r="B28" s="2">
-        <v>99</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>1023.49</v>
+        <v>5827.78</v>
       </c>
       <c r="B29" s="2">
-        <v>99.1</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>4225702.78</v>
+        <v>1002.25</v>
       </c>
       <c r="B30" s="2">
-        <v>99.843000000000004</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>46570.34</v>
+        <v>365213.93</v>
       </c>
       <c r="B31" s="2">
-        <v>99.7</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>204371.8</v>
+        <v>6825.12</v>
       </c>
       <c r="B32" s="2">
-        <v>99.8</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>17563.54</v>
+        <v>6965.38</v>
       </c>
       <c r="B33" s="2">
-        <v>99.6</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>1067.22</v>
+        <v>8333.86</v>
       </c>
       <c r="B34" s="2">
-        <v>99.15</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>342263.91</v>
+        <v>115126.44</v>
       </c>
       <c r="B35" s="2">
-        <v>99.83</v>
+        <v>98.44</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>1419.22</v>
+        <v>574.45000000000005</v>
       </c>
       <c r="B36" s="2">
-        <v>99.2</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>550000</v>
+        <v>28779.18</v>
       </c>
       <c r="B37" s="2">
-        <v>99.83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>105807.12</v>
+        <v>3085.85</v>
       </c>
       <c r="B38" s="2">
-        <v>99.8</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>32808.089999999997</v>
+        <v>8350</v>
       </c>
       <c r="B39" s="2">
-        <v>99.68</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>2056.42</v>
+        <v>47620.68</v>
       </c>
       <c r="B40" s="2">
-        <v>99.2</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>1327.72</v>
+        <v>8963.11</v>
       </c>
       <c r="B41" s="2">
-        <v>99.31</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>63619.7</v>
+        <v>13294.58</v>
       </c>
       <c r="B42" s="2">
-        <v>99.75</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>3146.85</v>
+        <v>4491.75</v>
       </c>
       <c r="B43" s="2">
-        <v>99.3</v>
+        <v>97.55</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>4933.29</v>
+        <v>370.39</v>
       </c>
       <c r="B44" s="2">
-        <v>99.4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>558.16999999999996</v>
+        <v>1113.9000000000001</v>
       </c>
       <c r="B45" s="2">
-        <v>99</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>594.92999999999995</v>
+        <v>831.62</v>
       </c>
       <c r="B46" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>26134.29</v>
+        <v>1050.71</v>
       </c>
       <c r="B47" s="2">
-        <v>99.6</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>4962.53</v>
+        <v>1168.2</v>
       </c>
       <c r="B48" s="2">
-        <v>99.2</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>12885.29</v>
+        <v>2724.65</v>
       </c>
       <c r="B49" s="2">
-        <v>99.55</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>1493.86</v>
+        <v>3143.37</v>
       </c>
       <c r="B50" s="2">
-        <v>99</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>19638.759999999998</v>
+        <v>20216.96</v>
       </c>
       <c r="B51" s="2">
-        <v>99.2</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>812.34</v>
+        <v>11866.16</v>
       </c>
       <c r="B52" s="2">
-        <v>99</v>
+        <v>97.65</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>2106.9299999999998</v>
+        <v>274.43</v>
       </c>
       <c r="B53" s="2">
-        <v>99.2</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>1012.18</v>
+        <v>641.19000000000005</v>
       </c>
       <c r="B54" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>200.8</v>
+        <v>2386.7399999999998</v>
       </c>
       <c r="B55" s="2">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>981.16</v>
+        <v>432288.6</v>
       </c>
       <c r="B56" s="2">
-        <v>99</v>
+        <v>98.42</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>2874.95</v>
+        <v>1628.85</v>
       </c>
       <c r="B57" s="2">
-        <v>99.1</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>2177.5300000000002</v>
+        <v>7466.46</v>
       </c>
       <c r="B58" s="2">
-        <v>99.36</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>16905.87</v>
+        <v>3660.88</v>
       </c>
       <c r="B59" s="2">
-        <v>99.5</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>6210</v>
+        <v>86.85</v>
       </c>
       <c r="B60" s="2">
-        <v>99.46</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>544.44000000000005</v>
+        <v>188080.47</v>
       </c>
       <c r="B61" s="2">
-        <v>98</v>
+        <v>98.42</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>46779.5</v>
+        <v>18659.689999999999</v>
       </c>
       <c r="B62" s="2">
-        <v>99.62</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>8916.2199999999993</v>
+        <v>19279.13</v>
       </c>
       <c r="B63" s="2">
-        <v>99.5</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>1480</v>
+        <v>48253.33</v>
       </c>
       <c r="B64" s="2">
-        <v>99.2</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>637.86</v>
+        <v>606312.66</v>
       </c>
       <c r="B65" s="2">
-        <v>99</v>
+        <v>98.42</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>7753.15</v>
+        <v>20908.59</v>
       </c>
       <c r="B66" s="2">
-        <v>99.4</v>
+        <v>97.4</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>1158.8900000000001</v>
+        <v>101380.19</v>
       </c>
       <c r="B67" s="2">
-        <v>99.2</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>46679.03</v>
+        <v>126521.71</v>
       </c>
       <c r="B68" s="2">
-        <v>99.6</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>32220.45</v>
+        <v>1005.94</v>
       </c>
       <c r="B69" s="2">
-        <v>99.65</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>148.04</v>
+        <v>2063.58</v>
       </c>
       <c r="B70" s="2">
-        <v>99.1</v>
+        <v>97.15</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>20845.330000000002</v>
+        <v>2206.73</v>
       </c>
       <c r="B71" s="2">
-        <v>99.65</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>561.54</v>
+        <v>39806.69</v>
       </c>
       <c r="B72" s="2">
-        <v>99</v>
+        <v>97.93</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>58426.13</v>
+        <v>31959.09</v>
       </c>
       <c r="B73" s="2">
-        <v>99.75</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>9486.7000000000007</v>
+        <v>91244.54</v>
       </c>
       <c r="B74" s="2">
-        <v>99.53</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>15623.56</v>
+        <v>7534.1</v>
       </c>
       <c r="B75" s="2">
-        <v>99.6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>3942.45</v>
+        <v>13293.48</v>
       </c>
       <c r="B76" s="2">
-        <v>99.4</v>
+        <v>98</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>3091.27</v>
+        <v>700005.14</v>
       </c>
       <c r="B77" s="2">
-        <v>99.4</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>708.59</v>
+        <v>206218.01</v>
       </c>
       <c r="B78" s="2">
-        <v>98.5</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>89134.399999999994</v>
+        <v>4824.87</v>
       </c>
       <c r="B79" s="2">
-        <v>99.75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>1455.97</v>
+        <v>59287.33</v>
       </c>
       <c r="B80" s="2">
-        <v>99.12</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>110884.03</v>
+        <v>122173.95</v>
       </c>
       <c r="B81" s="2">
-        <v>99.8</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>852.51</v>
+        <v>702103.38</v>
       </c>
       <c r="B82" s="2">
-        <v>99.05</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>5292</v>
+        <v>22300.6</v>
       </c>
       <c r="B83" s="2">
-        <v>99.55</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>2259</v>
+        <v>8624.44</v>
       </c>
       <c r="B84" s="2">
-        <v>99.25</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>2901.2</v>
+        <v>644.20000000000005</v>
       </c>
       <c r="B85" s="2">
-        <v>99.25</v>
+        <v>97</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>2824.47</v>
+        <v>4672.6099999999997</v>
       </c>
       <c r="B86" s="2">
-        <v>99.35</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>2171.94</v>
+        <v>588.91999999999996</v>
       </c>
       <c r="B87" s="2">
-        <v>99.35</v>
+        <v>97.15</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>53208.03</v>
+        <v>1900</v>
       </c>
       <c r="B88" s="2">
-        <v>99.75</v>
+        <v>97.15</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>626731.62</v>
+        <v>5987.25</v>
       </c>
       <c r="B89" s="2">
-        <v>99.83</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>3066.69</v>
+        <v>955.85</v>
       </c>
       <c r="B90" s="2">
-        <v>99.4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>17464.77</v>
+        <v>8877.14</v>
       </c>
       <c r="B91" s="2">
-        <v>99.15</v>
+        <v>97.55</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>48349.48</v>
+        <v>1288.26</v>
       </c>
       <c r="B92" s="2">
-        <v>99.75</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>166162.95000000001</v>
+        <v>1069.68</v>
       </c>
       <c r="B93" s="2">
-        <v>99.75</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>880</v>
+        <v>1301.6199999999999</v>
       </c>
       <c r="B94" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>1373.97</v>
+        <v>324.60000000000002</v>
       </c>
       <c r="B95" s="2">
-        <v>99.3</v>
+        <v>96.05</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>4000</v>
+        <v>1437.1</v>
       </c>
       <c r="B96" s="2">
-        <v>99.45</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>50000</v>
+        <v>8484652.6400000006</v>
       </c>
       <c r="B97" s="2">
-        <v>99.72</v>
+        <v>98.9</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>163687.35</v>
+        <v>19099.34</v>
       </c>
       <c r="B98" s="2">
-        <v>99.810599999999994</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>61457.41</v>
+        <v>54383.43</v>
       </c>
       <c r="B99" s="2">
-        <v>99.75</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>3888.16</v>
+        <v>16941.97</v>
       </c>
       <c r="B100" s="2">
-        <v>99.3</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>39980.449999999997</v>
+        <v>308181.24</v>
       </c>
       <c r="B101" s="2">
-        <v>99.68</v>
+        <v>98.440299999999993</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>29993.34</v>
+        <v>16433.830000000002</v>
       </c>
       <c r="B102" s="2">
-        <v>99.65</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>72405.42</v>
+        <v>24414.7</v>
       </c>
       <c r="B103" s="2">
-        <v>99.7</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>347.11</v>
+        <v>1176.3399999999999</v>
       </c>
       <c r="B104" s="2">
-        <v>98</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>8373.6</v>
+        <v>505.08</v>
       </c>
       <c r="B105" s="2">
-        <v>99.5</v>
+        <v>97</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>3666.4</v>
+        <v>1241.72</v>
       </c>
       <c r="B106" s="2">
-        <v>99.4</v>
+        <v>97.2</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>395.04</v>
+        <v>3240.93</v>
       </c>
       <c r="B107" s="2">
         <v>97.5</v>
@@ -1812,1323 +1812,1587 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>26941.65</v>
+        <v>27533.06</v>
       </c>
       <c r="B108" s="2">
-        <v>99.62</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>2921.59</v>
+        <v>7276.62</v>
       </c>
       <c r="B109" s="2">
-        <v>99.25</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>485.88</v>
+        <v>69144.08</v>
       </c>
       <c r="B110" s="2">
-        <v>99</v>
+        <v>98.05</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>707.46</v>
+        <v>37519.839999999997</v>
       </c>
       <c r="B111" s="2">
-        <v>99</v>
+        <v>97.85</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>1208.06</v>
+        <v>12517.89</v>
       </c>
       <c r="B112" s="2">
-        <v>99.25</v>
+        <v>98</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>248938.07</v>
+        <v>519.39</v>
       </c>
       <c r="B113" s="2">
-        <v>99.79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>61125.599999999999</v>
+        <v>242962.04</v>
       </c>
       <c r="B114" s="2">
-        <v>99.76</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>154215.4</v>
+        <v>802.07</v>
       </c>
       <c r="B115" s="2">
-        <v>99.8</v>
+        <v>97</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>3657.42</v>
+        <v>4388.97</v>
       </c>
       <c r="B116" s="2">
-        <v>99.25</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>1721.94</v>
+        <v>658519.4</v>
       </c>
       <c r="B117" s="2">
-        <v>99.3</v>
+        <v>98.72</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>410.63</v>
+        <v>196044.62</v>
       </c>
       <c r="B118" s="2">
-        <v>96</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>14312.92</v>
+        <v>143285.32</v>
       </c>
       <c r="B119" s="2">
-        <v>99.65</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>118605.33</v>
+        <v>50153.9</v>
       </c>
       <c r="B120" s="2">
-        <v>99.82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>1115.33</v>
+        <v>9309.9</v>
       </c>
       <c r="B121" s="2">
-        <v>99.12</v>
+        <v>97.4</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>568.42999999999995</v>
+        <v>24241.37</v>
       </c>
       <c r="B122" s="2">
-        <v>96</v>
+        <v>97.9</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>694.37</v>
+        <v>1022.53</v>
       </c>
       <c r="B123" s="2">
-        <v>97</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>2239.0700000000002</v>
+        <v>31921.16</v>
       </c>
       <c r="B124" s="2">
-        <v>99.35</v>
+        <v>98</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>2171.2199999999998</v>
+        <v>1456.49</v>
       </c>
       <c r="B125" s="2">
-        <v>99.35</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>1074.8900000000001</v>
+        <v>191409.69</v>
       </c>
       <c r="B126" s="2">
-        <v>99.2</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>25476.3</v>
+        <v>207454.02</v>
       </c>
       <c r="B127" s="2">
-        <v>99.700199999999995</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>1244.05</v>
+        <v>131648.16</v>
       </c>
       <c r="B128" s="2">
-        <v>99.2</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>784894.26</v>
+        <v>2799.36</v>
       </c>
       <c r="B129" s="2">
-        <v>99.84</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>39728.61</v>
+        <v>3183.41</v>
       </c>
       <c r="B130" s="2">
-        <v>99.720299999999995</v>
+        <v>97.35</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>5457.67</v>
+        <v>2258.35</v>
       </c>
       <c r="B131" s="2">
-        <v>99.5</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>50744.38</v>
+        <v>1726.46</v>
       </c>
       <c r="B132" s="2">
-        <v>99.74</v>
+        <v>97.2</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>2018.75</v>
+        <v>3000</v>
       </c>
       <c r="B133" s="2">
-        <v>99.3</v>
+        <v>97.2</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>3999.52</v>
+        <v>33303.64</v>
       </c>
       <c r="B134" s="2">
-        <v>99.46</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>3380.85</v>
+        <v>22525.54</v>
       </c>
       <c r="B135" s="2">
-        <v>99.43</v>
+        <v>98</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>1205.4100000000001</v>
+        <v>1568.2</v>
       </c>
       <c r="B136" s="2">
-        <v>99.35</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>46958.46</v>
+        <v>2862.06</v>
       </c>
       <c r="B137" s="2">
-        <v>99.75</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>15623.2</v>
+        <v>4357.3100000000004</v>
       </c>
       <c r="B138" s="2">
-        <v>99.674999999999997</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>80433.45</v>
+        <v>4407.7</v>
       </c>
       <c r="B139" s="2">
-        <v>99.76</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>673.05</v>
+        <v>3391.31</v>
       </c>
       <c r="B140" s="2">
-        <v>99.100099999999998</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>4806.96</v>
+        <v>4293.72</v>
       </c>
       <c r="B141" s="2">
-        <v>99.504999999999995</v>
+        <v>97.45</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>1152.3399999999999</v>
+        <v>281.42</v>
       </c>
       <c r="B142" s="2">
-        <v>99.35</v>
+        <v>96.9</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>18107.64</v>
+        <v>892.21</v>
       </c>
       <c r="B143" s="2">
-        <v>99.15</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>1244.42</v>
+        <v>1636.91</v>
       </c>
       <c r="B144" s="2">
-        <v>99.37</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>772.12</v>
+        <v>2232.73</v>
       </c>
       <c r="B145" s="2">
-        <v>99.2</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>6779.55</v>
+        <v>726663.93</v>
       </c>
       <c r="B146" s="2">
-        <v>99.5</v>
+        <v>99.09</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>129813.21</v>
+        <v>11854.5</v>
       </c>
       <c r="B147" s="2">
-        <v>99.82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>22620.66</v>
+        <v>397.85</v>
       </c>
       <c r="B148" s="2">
-        <v>99.65</v>
+        <v>96</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>220.26</v>
+        <v>718.95</v>
       </c>
       <c r="B149" s="2">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>6147.73</v>
+        <v>126.12</v>
       </c>
       <c r="B150" s="2">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>907.34</v>
+        <v>187937.62</v>
       </c>
       <c r="B151" s="2">
-        <v>99.25</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>20758.830000000002</v>
+        <v>25779.03</v>
       </c>
       <c r="B152" s="2">
-        <v>99.6</v>
+        <v>98.03</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>1850.54</v>
+        <v>471787.35</v>
       </c>
       <c r="B153" s="2">
-        <v>99.35</v>
+        <v>98.72</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>1607.01</v>
+        <v>225.32</v>
       </c>
       <c r="B154" s="2">
-        <v>99.35</v>
+        <v>94</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>1826.32</v>
+        <v>609521.35</v>
       </c>
       <c r="B155" s="2">
-        <v>99.25</v>
+        <v>98.72</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>37552.839999999997</v>
+        <v>219740.56</v>
       </c>
       <c r="B156" s="2">
-        <v>99.7</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>4719.0600000000004</v>
+        <v>143300.63</v>
       </c>
       <c r="B157" s="2">
-        <v>99.5</v>
+        <v>98.48</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>582000</v>
+        <v>1577.86</v>
       </c>
       <c r="B158" s="2">
-        <v>99.844999999999999</v>
+        <v>97.2</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>2349.35</v>
+        <v>3563.99</v>
       </c>
       <c r="B159" s="2">
-        <v>99.35</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>586.64</v>
+        <v>433878.58</v>
       </c>
       <c r="B160" s="2">
-        <v>97</v>
+        <v>98.72</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>1173.77</v>
+        <v>4710.09</v>
       </c>
       <c r="B161" s="2">
-        <v>99.1</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>689.17</v>
+        <v>13030.84</v>
       </c>
       <c r="B162" s="2">
-        <v>98.5</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>319079</v>
+        <v>81666.67</v>
       </c>
       <c r="B163" s="2">
-        <v>99.83</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>909.52</v>
+        <v>123445.71</v>
       </c>
       <c r="B164" s="2">
-        <v>99</v>
+        <v>98.48</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>2055.61</v>
+        <v>5203.0200000000004</v>
       </c>
       <c r="B165" s="2">
-        <v>99.1</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>6530.88</v>
+        <v>359.16</v>
       </c>
       <c r="B166" s="2">
-        <v>99.1</v>
+        <v>96</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>4379.3100000000004</v>
+        <v>48500</v>
       </c>
       <c r="B167" s="2">
-        <v>99.25</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>3650.09</v>
+        <v>39793.68</v>
       </c>
       <c r="B168" s="2">
-        <v>99.35</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>466205.94</v>
+        <v>3242.36</v>
       </c>
       <c r="B169" s="2">
-        <v>99.85</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>13929.52</v>
+        <v>280327.90000000002</v>
       </c>
       <c r="B170" s="2">
-        <v>99.55</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>716.7</v>
+        <v>740.29</v>
       </c>
       <c r="B171" s="2">
-        <v>99.05</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>1180.98</v>
+        <v>571.46</v>
       </c>
       <c r="B172" s="2">
-        <v>99.3</v>
+        <v>96</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>198.74</v>
+        <v>1255.92</v>
       </c>
       <c r="B173" s="2">
-        <v>93</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>516.37</v>
+        <v>14645.92</v>
       </c>
       <c r="B174" s="2">
-        <v>96</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>2571.73</v>
+        <v>2948.38</v>
       </c>
       <c r="B175" s="2">
-        <v>99</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>19047.599999999999</v>
+        <v>40140.589999999997</v>
       </c>
       <c r="B176" s="2">
-        <v>99.2</v>
+        <v>98.32</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>20628.2</v>
+        <v>32539.32</v>
       </c>
       <c r="B177" s="2">
-        <v>99.6</v>
+        <v>98</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>2560.7199999999998</v>
+        <v>60000</v>
       </c>
       <c r="B178" s="2">
-        <v>99.35</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>909.39</v>
+        <v>1022.53</v>
       </c>
       <c r="B179" s="2">
-        <v>99</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>12798</v>
+        <v>1032.5899999999999</v>
       </c>
       <c r="B180" s="2">
-        <v>99.1</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>17146.63</v>
+        <v>5828.15</v>
       </c>
       <c r="B181" s="2">
-        <v>99.15</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>22264.99</v>
+        <v>57622.26</v>
       </c>
       <c r="B182" s="2">
-        <v>99.2</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>141999.69</v>
+        <v>1294.94</v>
       </c>
       <c r="B183" s="2">
-        <v>99.76</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>33950.51</v>
+        <v>16208.57</v>
       </c>
       <c r="B184" s="2">
-        <v>99.7</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>56.05</v>
+        <v>8802.8700000000008</v>
       </c>
       <c r="B185" s="2">
-        <v>92</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>105.38</v>
+        <v>1092.79</v>
       </c>
       <c r="B186" s="2">
-        <v>95.05</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>1110.3900000000001</v>
+        <v>3495.49</v>
       </c>
       <c r="B187" s="2">
-        <v>99.2</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>357126.46</v>
+        <v>2538.0100000000002</v>
       </c>
       <c r="B188" s="2">
-        <v>99.82</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>12000</v>
+        <v>1537.62</v>
       </c>
       <c r="B189" s="2">
-        <v>99.5</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>722.96</v>
+        <v>24622.26</v>
       </c>
       <c r="B190" s="2">
-        <v>98.5</v>
+        <v>97.45</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>61565.58</v>
+        <v>7022.42</v>
       </c>
       <c r="B191" s="2">
-        <v>99.75</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
-        <v>4905.2299999999996</v>
+        <v>49447.75</v>
       </c>
       <c r="B192" s="2">
-        <v>99.45</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
-        <v>527.63</v>
+        <v>67121.279999999999</v>
       </c>
       <c r="B193" s="2">
-        <v>99</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>3580.02</v>
+        <v>1974.48</v>
       </c>
       <c r="B194" s="2">
-        <v>99.4</v>
+        <v>97.850499999999997</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>750.13</v>
+        <v>6432</v>
       </c>
       <c r="B195" s="2">
-        <v>99.1</v>
+        <v>98.25</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
-        <v>14427.61</v>
+        <v>45804.7</v>
       </c>
       <c r="B196" s="2">
-        <v>99.65</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
-        <v>541.6</v>
+        <v>1933.75</v>
       </c>
       <c r="B197" s="2">
-        <v>99</v>
+        <v>97.35</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
-        <v>105482.76</v>
+        <v>4427.45</v>
       </c>
       <c r="B198" s="2">
-        <v>99.82</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
-        <v>1142.74</v>
+        <v>11136.06</v>
       </c>
       <c r="B199" s="2">
-        <v>99.15</v>
+        <v>97.9</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
-        <v>44209.15</v>
+        <v>17100.29</v>
       </c>
       <c r="B200" s="2">
-        <v>99.77</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
-        <v>12657.16</v>
+        <v>389343.12</v>
       </c>
       <c r="B201" s="2">
-        <v>99.6</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
-        <v>115075.46</v>
+        <v>126130.94</v>
       </c>
       <c r="B202" s="2">
-        <v>99.8</v>
+        <v>98.67</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
-        <v>13908.98</v>
+        <v>3591.78</v>
       </c>
       <c r="B203" s="2">
-        <v>99.564999999999998</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
-        <v>5538.57</v>
+        <v>400.42</v>
       </c>
       <c r="B204" s="2">
-        <v>99.05</v>
+        <v>97</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
-        <v>19515.71</v>
+        <v>7959.87</v>
       </c>
       <c r="B205" s="2">
-        <v>99.15</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
-        <v>63301.19</v>
+        <v>20164.400000000001</v>
       </c>
       <c r="B206" s="2">
-        <v>99.75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
-        <v>196077.92</v>
+        <v>63509.97</v>
       </c>
       <c r="B207" s="2">
-        <v>99.82</v>
+        <v>98.25</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
-        <v>8000</v>
+        <v>1232.76</v>
       </c>
       <c r="B208" s="2">
-        <v>99.8</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
-        <v>38561.67</v>
+        <v>10692.97</v>
       </c>
       <c r="B209" s="2">
-        <v>99.7</v>
+        <v>97.9</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
-        <v>1737.04</v>
+        <v>24598.22</v>
       </c>
       <c r="B210" s="2">
-        <v>99.25</v>
+        <v>98</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
-        <v>186.99</v>
+        <v>32701.99</v>
       </c>
       <c r="B211" s="2">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
-        <v>1975.54</v>
+        <v>53653.4</v>
       </c>
       <c r="B212" s="2">
-        <v>99.1</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
-        <v>3300</v>
+        <v>15130.54</v>
       </c>
       <c r="B213" s="2">
-        <v>99.4</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
-        <v>65785.52</v>
+        <v>55535.79</v>
       </c>
       <c r="B214" s="2">
-        <v>99.75</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
-        <v>9420.36</v>
+        <v>5260.25</v>
       </c>
       <c r="B215" s="2">
-        <v>99.5</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
-        <v>584.4</v>
+        <v>4983.41</v>
       </c>
       <c r="B216" s="2">
-        <v>98</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
-        <v>5937.46</v>
+        <v>696.38</v>
       </c>
       <c r="B217" s="2">
-        <v>99.45</v>
+        <v>94</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
-        <v>956.51</v>
+        <v>1464.54</v>
       </c>
       <c r="B218" s="2">
-        <v>99</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
-        <v>648.59</v>
+        <v>55165.64</v>
       </c>
       <c r="B219" s="2">
-        <v>99</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
-        <v>629.6</v>
+        <v>235865.58</v>
       </c>
       <c r="B220" s="2">
-        <v>98</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
-        <v>3325.49</v>
+        <v>1198.46</v>
       </c>
       <c r="B221" s="2">
-        <v>99.4</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
-        <v>6173.52</v>
+        <v>2725.45</v>
       </c>
       <c r="B222" s="2">
-        <v>99.45</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
-        <v>10468.620000000001</v>
+        <v>89179.19</v>
       </c>
       <c r="B223" s="2">
-        <v>99.5</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
-        <v>1667.99</v>
+        <v>549.66</v>
       </c>
       <c r="B224" s="2">
-        <v>99.2</v>
+        <v>97</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
-        <v>10434.11</v>
+        <v>5164.82</v>
       </c>
       <c r="B225" s="2">
-        <v>99.6</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
-        <v>33975.980000000003</v>
+        <v>1235.97</v>
       </c>
       <c r="B226" s="2">
-        <v>99.62</v>
+        <v>97.05</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
-        <v>201429.21</v>
+        <v>473.32</v>
       </c>
       <c r="B227" s="2">
-        <v>99.81</v>
+        <v>97</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
-        <v>55568</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="B228" s="2">
-        <v>99.75</v>
+        <v>97.4</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
-        <v>4212.95</v>
+        <v>14106.52</v>
       </c>
       <c r="B229" s="2">
-        <v>99.15</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
-        <v>1943.85</v>
+        <v>1521.33</v>
       </c>
       <c r="B230" s="2">
-        <v>99.25</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
-        <v>6287.3</v>
+        <v>54674.13</v>
       </c>
       <c r="B231" s="2">
-        <v>99.45</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
-        <v>4767.83</v>
+        <v>10758.91</v>
       </c>
       <c r="B232" s="2">
-        <v>99.4</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
-        <v>1338.13</v>
+        <v>4525.8900000000003</v>
       </c>
       <c r="B233" s="2">
-        <v>99.25</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
-        <v>1694.7</v>
+        <v>5647.91</v>
       </c>
       <c r="B234" s="2">
-        <v>99.254999999999995</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
-        <v>6195.77</v>
+        <v>33276.39</v>
       </c>
       <c r="B235" s="2">
-        <v>99.45</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
-        <v>20521.43</v>
+        <v>3003.83</v>
       </c>
       <c r="B236" s="2">
-        <v>99.610100000000003</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
-        <v>1163.4000000000001</v>
+        <v>2091.66</v>
       </c>
       <c r="B237" s="2">
-        <v>99</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
-        <v>48718.720000000001</v>
+        <v>47484.160000000003</v>
       </c>
       <c r="B238" s="2">
-        <v>99.5</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
-        <v>424.93</v>
+        <v>256024.52</v>
       </c>
       <c r="B239" s="2">
-        <v>99</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="2"/>
-      <c r="B240" s="2"/>
+      <c r="A240" s="2">
+        <v>2644.63</v>
+      </c>
+      <c r="B240" s="2">
+        <v>97.3</v>
+      </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="2"/>
-      <c r="B241" s="2"/>
+      <c r="A241" s="2">
+        <v>2432.98</v>
+      </c>
+      <c r="B241" s="2">
+        <v>97.5</v>
+      </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="2"/>
-      <c r="B242" s="2"/>
+      <c r="A242" s="2">
+        <v>3613.66</v>
+      </c>
+      <c r="B242" s="2">
+        <v>97.55</v>
+      </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="2"/>
-      <c r="B243" s="2"/>
+      <c r="A243" s="2">
+        <v>28593.919999999998</v>
+      </c>
+      <c r="B243" s="2">
+        <v>98.2</v>
+      </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="2"/>
-      <c r="B244" s="2"/>
+      <c r="A244" s="2">
+        <v>3176.74</v>
+      </c>
+      <c r="B244" s="2">
+        <v>97.55</v>
+      </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="2"/>
-      <c r="B245" s="2"/>
+      <c r="A245" s="2">
+        <v>814405.89</v>
+      </c>
+      <c r="B245" s="2">
+        <v>98.8</v>
+      </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="2"/>
-      <c r="B246" s="2"/>
+      <c r="A246" s="2">
+        <v>1046092.83</v>
+      </c>
+      <c r="B246" s="2">
+        <v>98.77</v>
+      </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="2"/>
-      <c r="B247" s="2"/>
+      <c r="A247" s="2">
+        <v>766.89</v>
+      </c>
+      <c r="B247" s="2">
+        <v>97</v>
+      </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="2"/>
-      <c r="B248" s="2"/>
+      <c r="A248" s="2">
+        <v>28822.35</v>
+      </c>
+      <c r="B248" s="2">
+        <v>98.25</v>
+      </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="2"/>
-      <c r="B249" s="2"/>
+      <c r="A249" s="2">
+        <v>28071.52</v>
+      </c>
+      <c r="B249" s="2">
+        <v>98.25</v>
+      </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="2"/>
-      <c r="B250" s="2"/>
+      <c r="A250" s="2">
+        <v>12044.34</v>
+      </c>
+      <c r="B250" s="2">
+        <v>98.2</v>
+      </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="2"/>
-      <c r="B251" s="2"/>
+      <c r="A251" s="2">
+        <v>76467.570000000007</v>
+      </c>
+      <c r="B251" s="2">
+        <v>98.25</v>
+      </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="2"/>
-      <c r="B252" s="2"/>
+      <c r="A252" s="2">
+        <v>87088.67</v>
+      </c>
+      <c r="B252" s="2">
+        <v>98.3</v>
+      </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="2"/>
-      <c r="B253" s="2"/>
+      <c r="A253" s="2">
+        <v>10749.86</v>
+      </c>
+      <c r="B253" s="2">
+        <v>97.8</v>
+      </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="2"/>
-      <c r="B254" s="2"/>
+      <c r="A254" s="2">
+        <v>85500.86</v>
+      </c>
+      <c r="B254" s="2">
+        <v>98</v>
+      </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="2"/>
-      <c r="B255" s="2"/>
+      <c r="A255" s="2">
+        <v>173388.28</v>
+      </c>
+      <c r="B255" s="2">
+        <v>98.45</v>
+      </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="2"/>
-      <c r="B256" s="2"/>
+      <c r="A256" s="2">
+        <v>6186.61</v>
+      </c>
+      <c r="B256" s="2">
+        <v>97.5</v>
+      </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="2"/>
-      <c r="B257" s="2"/>
+      <c r="A257" s="2">
+        <v>81456.160000000003</v>
+      </c>
+      <c r="B257" s="2">
+        <v>98.5</v>
+      </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="2"/>
-      <c r="B258" s="2"/>
+      <c r="A258" s="2">
+        <v>2750.07</v>
+      </c>
+      <c r="B258" s="2">
+        <v>97.3</v>
+      </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="2"/>
-      <c r="B259" s="2"/>
+      <c r="A259" s="2">
+        <v>5279.1</v>
+      </c>
+      <c r="B259" s="2">
+        <v>97.5</v>
+      </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="2"/>
-      <c r="B260" s="2"/>
+      <c r="A260" s="2">
+        <v>34942.67</v>
+      </c>
+      <c r="B260" s="2">
+        <v>98</v>
+      </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="2"/>
-      <c r="B261" s="2"/>
+      <c r="A261" s="2">
+        <v>1303.9100000000001</v>
+      </c>
+      <c r="B261" s="2">
+        <v>97.25</v>
+      </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="2"/>
-      <c r="B262" s="2"/>
+      <c r="A262" s="2">
+        <v>1375.02</v>
+      </c>
+      <c r="B262" s="2">
+        <v>97.1</v>
+      </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="2"/>
-      <c r="B263" s="2"/>
+      <c r="A263" s="2">
+        <v>335.43</v>
+      </c>
+      <c r="B263" s="2">
+        <v>93</v>
+      </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="2"/>
-      <c r="B264" s="2"/>
+      <c r="A264" s="2">
+        <v>422209.99</v>
+      </c>
+      <c r="B264" s="2">
+        <v>98.72</v>
+      </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="3"/>
-      <c r="B265" s="3"/>
+      <c r="A265" s="3">
+        <v>9035.51</v>
+      </c>
+      <c r="B265" s="2">
+        <v>97.25</v>
+      </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="2"/>
-      <c r="B266" s="2"/>
+      <c r="A266" s="2">
+        <v>419190.92</v>
+      </c>
+      <c r="B266" s="2">
+        <v>98.7</v>
+      </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="2"/>
-      <c r="B267" s="2"/>
+      <c r="A267" s="2">
+        <v>123530.42</v>
+      </c>
+      <c r="B267" s="2">
+        <v>98.3</v>
+      </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="2"/>
-      <c r="B268" s="2"/>
+      <c r="A268" s="2">
+        <v>62700</v>
+      </c>
+      <c r="B268" s="2">
+        <v>98.3</v>
+      </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="2"/>
-      <c r="B269" s="2"/>
+      <c r="A269" s="2">
+        <v>2461023.2000000002</v>
+      </c>
+      <c r="B269" s="2">
+        <v>98.88</v>
+      </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="2"/>
-      <c r="B270" s="2"/>
+      <c r="A270" s="2">
+        <v>94489.12</v>
+      </c>
+      <c r="B270" s="2">
+        <v>98.35</v>
+      </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="2"/>
-      <c r="B271" s="2"/>
+      <c r="A271" s="2">
+        <v>10065.33</v>
+      </c>
+      <c r="B271" s="2">
+        <v>97.6</v>
+      </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="2"/>
-      <c r="B272" s="2"/>
+      <c r="A272" s="2">
+        <v>2473</v>
+      </c>
+      <c r="B272" s="2">
+        <v>97.6</v>
+      </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="2"/>
-      <c r="B273" s="2"/>
+      <c r="A273" s="2">
+        <v>58226.47</v>
+      </c>
+      <c r="B273" s="2">
+        <v>98</v>
+      </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="2"/>
-      <c r="B274" s="2"/>
+      <c r="A274" s="2">
+        <v>576531.79</v>
+      </c>
+      <c r="B274" s="2">
+        <v>98.7</v>
+      </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="2"/>
-      <c r="B275" s="2"/>
+      <c r="A275" s="2">
+        <v>106296.15</v>
+      </c>
+      <c r="B275" s="2">
+        <v>98.4</v>
+      </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="2"/>
-      <c r="B276" s="2"/>
+      <c r="A276" s="2">
+        <v>163482.74</v>
+      </c>
+      <c r="B276" s="2">
+        <v>98.5</v>
+      </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="2"/>
-      <c r="B277" s="2"/>
+      <c r="A277" s="2">
+        <v>59376.17</v>
+      </c>
+      <c r="B277" s="2">
+        <v>98.5</v>
+      </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="2"/>
-      <c r="B278" s="2"/>
+      <c r="A278" s="2">
+        <v>136229.60999999999</v>
+      </c>
+      <c r="B278" s="2">
+        <v>98.45</v>
+      </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="2"/>
-      <c r="B279" s="2"/>
+      <c r="A279" s="2">
+        <v>6365.78</v>
+      </c>
+      <c r="B279" s="2">
+        <v>97.6</v>
+      </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="2"/>
-      <c r="B280" s="2"/>
+      <c r="A280" s="2">
+        <v>123196.99</v>
+      </c>
+      <c r="B280" s="2">
+        <v>98.5</v>
+      </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="2"/>
-      <c r="B281" s="2"/>
+      <c r="A281" s="2">
+        <v>3266.46</v>
+      </c>
+      <c r="B281" s="2">
+        <v>97.3</v>
+      </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="2"/>
-      <c r="B282" s="2"/>
+      <c r="A282" s="2">
+        <v>2031.25</v>
+      </c>
+      <c r="B282" s="2">
+        <v>97.5</v>
+      </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="2"/>
-      <c r="B283" s="2"/>
+      <c r="A283" s="2">
+        <v>92308.64</v>
+      </c>
+      <c r="B283" s="2">
+        <v>98.5</v>
+      </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="2"/>
-      <c r="B284" s="2"/>
+      <c r="A284" s="2">
+        <v>9266.52</v>
+      </c>
+      <c r="B284" s="2">
+        <v>97.6</v>
+      </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="2"/>
-      <c r="B285" s="2"/>
+      <c r="A285" s="2">
+        <v>131945.69</v>
+      </c>
+      <c r="B285" s="2">
+        <v>98.5</v>
+      </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="2"/>
-      <c r="B286" s="2"/>
+      <c r="A286" s="2">
+        <v>330000</v>
+      </c>
+      <c r="B286" s="2">
+        <v>98.65</v>
+      </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="2"/>
-      <c r="B287" s="2"/>
+      <c r="A287" s="2">
+        <v>4254.6000000000004</v>
+      </c>
+      <c r="B287" s="2">
+        <v>97.3</v>
+      </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="2"/>
-      <c r="B288" s="2"/>
+      <c r="A288" s="2">
+        <v>1021.24</v>
+      </c>
+      <c r="B288" s="2">
+        <v>97.5</v>
+      </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="2"/>
-      <c r="B289" s="2"/>
+      <c r="A289" s="2">
+        <v>1689.44</v>
+      </c>
+      <c r="B289" s="2">
+        <v>97.5</v>
+      </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="2"/>
-      <c r="B290" s="2"/>
+      <c r="A290" s="2">
+        <v>43989.95</v>
+      </c>
+      <c r="B290" s="2">
+        <v>98</v>
+      </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="2"/>
-      <c r="B291" s="2"/>
+      <c r="A291" s="2">
+        <v>3308.97</v>
+      </c>
+      <c r="B291" s="2">
+        <v>97.35</v>
+      </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="2"/>
-      <c r="B292" s="2"/>
+      <c r="A292" s="2">
+        <v>8212.26</v>
+      </c>
+      <c r="B292" s="2">
+        <v>97.7</v>
+      </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="2"/>
-      <c r="B293" s="2"/>
+      <c r="A293" s="2">
+        <v>2814.19</v>
+      </c>
+      <c r="B293" s="2">
+        <v>97.25</v>
+      </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="2"/>
-      <c r="B294" s="2"/>
+      <c r="A294" s="2">
+        <v>28000</v>
+      </c>
+      <c r="B294" s="2">
+        <v>98.6</v>
+      </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="2"/>
-      <c r="B295" s="2"/>
+      <c r="A295" s="2">
+        <v>215.36</v>
+      </c>
+      <c r="B295" s="2">
+        <v>93.1</v>
+      </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" s="2"/>
-      <c r="B296" s="2"/>
+      <c r="A296" s="2">
+        <v>366.53</v>
+      </c>
+      <c r="B296" s="2">
+        <v>95</v>
+      </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" s="2"/>
-      <c r="B297" s="2"/>
+      <c r="A297" s="2">
+        <v>131.9</v>
+      </c>
+      <c r="B297" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="2"/>
-      <c r="B298" s="2"/>
+      <c r="A298" s="2">
+        <v>850</v>
+      </c>
+      <c r="B298" s="2">
+        <v>97</v>
+      </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" s="2"/>
-      <c r="B299" s="2"/>
+      <c r="A299" s="2">
+        <v>886.46</v>
+      </c>
+      <c r="B299" s="2">
+        <v>97</v>
+      </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" s="2"/>
-      <c r="B300" s="2"/>
+      <c r="A300" s="2">
+        <v>1222.57</v>
+      </c>
+      <c r="B300" s="2">
+        <v>97.25</v>
+      </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" s="2"/>
-      <c r="B301" s="2"/>
+      <c r="A301" s="2">
+        <v>2066.96</v>
+      </c>
+      <c r="B301" s="2">
+        <v>97.3</v>
+      </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" s="2"/>
-      <c r="B302" s="2"/>
+      <c r="A302" s="2">
+        <v>1775.87</v>
+      </c>
+      <c r="B302" s="2">
+        <v>97.5</v>
+      </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" s="2"/>
-      <c r="B303" s="2"/>
+      <c r="A303" s="2">
+        <v>6390.79</v>
+      </c>
+      <c r="B303" s="2">
+        <v>97.7</v>
+      </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" s="2"/>
-      <c r="B304" s="2"/>
+      <c r="A304" s="2">
+        <v>5091.38</v>
+      </c>
+      <c r="B304" s="2">
+        <v>97.7</v>
+      </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="2"/>
-      <c r="B305" s="2"/>
+      <c r="A305" s="2">
+        <v>1200.78</v>
+      </c>
+      <c r="B305" s="3">
+        <v>97.25</v>
+      </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="2"/>

</xml_diff>

<commit_message>
actualizacion de notas de credito semanal
</commit_message>
<xml_diff>
--- a/data/NC_semanal.xlsx
+++ b/data/NC_semanal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Desktop\MetrovaloresApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2DEABC-990F-482F-BD2C-4D4391026D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71379220-900D-4084-9D19-B4AA16B749A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{9E78C8B1-ED59-4A81-8FF9-F1A88ED1C1A0}"/>
   </bookViews>
@@ -943,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077B50AF-9C9F-4CF5-BB56-A27ACF5565DE}">
-  <dimension ref="A1:B285"/>
+  <dimension ref="A1:B329"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2:B329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,87 +964,87 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>23907.73</v>
+        <v>550.38</v>
       </c>
       <c r="B2" s="2">
-        <v>98.5</v>
+        <v>97.35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>12252.84</v>
+        <v>508423.79</v>
       </c>
       <c r="B3" s="2">
-        <v>98.3</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>6417.05</v>
+        <v>1047.0899999999999</v>
       </c>
       <c r="B4" s="2">
-        <v>98.15</v>
+        <v>97.75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>25120.99</v>
+        <v>5851.64</v>
       </c>
       <c r="B5" s="2">
-        <v>98.55</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>67141.600000000006</v>
+        <v>8897.4599999999991</v>
       </c>
       <c r="B6" s="2">
-        <v>98.55</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>175637.71</v>
+        <v>14135.48</v>
       </c>
       <c r="B7" s="2">
-        <v>98.7</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>36977.42</v>
+        <v>3070.84</v>
       </c>
       <c r="B8" s="2">
-        <v>98.5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>999.31</v>
+        <v>249661.49</v>
       </c>
       <c r="B9" s="2">
-        <v>97.15</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>1656.77</v>
+        <v>1131.3399999999999</v>
       </c>
       <c r="B10" s="2">
-        <v>97.5</v>
+        <v>97.55</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>2271.37</v>
+        <v>35000</v>
       </c>
       <c r="B11" s="2">
-        <v>97.7</v>
+        <v>98.730699999999999</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>2539.23</v>
+        <v>9073.49</v>
       </c>
       <c r="B12" s="2">
         <v>98</v>
@@ -1052,151 +1052,151 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>3207.71</v>
+        <v>118280.34</v>
       </c>
       <c r="B13" s="2">
-        <v>97.8</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>312.48</v>
+        <v>30821.62</v>
       </c>
       <c r="B14" s="2">
-        <v>94</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>8457.41</v>
+        <v>32549.32</v>
       </c>
       <c r="B15" s="2">
-        <v>98.3</v>
+        <v>98.48</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>7699.29</v>
+        <v>310000</v>
       </c>
       <c r="B16" s="2">
-        <v>98.250500000000002</v>
+        <v>98.8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>1545.2</v>
+        <v>114046.39</v>
       </c>
       <c r="B17" s="2">
-        <v>97.55</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>33514.89</v>
+        <v>140397.67000000001</v>
       </c>
       <c r="B18" s="2">
-        <v>98.4</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>113738</v>
+        <v>18748.72</v>
       </c>
       <c r="B19" s="2">
-        <v>98.65</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>2738.8</v>
+        <v>601.86</v>
       </c>
       <c r="B20" s="2">
-        <v>97.8</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>8109.96</v>
+        <v>15732.39</v>
       </c>
       <c r="B21" s="2">
-        <v>98</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>11979.42</v>
+        <v>7998.06</v>
       </c>
       <c r="B22" s="2">
-        <v>98.3</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>29195.22</v>
+        <v>2039.22</v>
       </c>
       <c r="B23" s="2">
-        <v>98.5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>6326.31</v>
+        <v>1235.99</v>
       </c>
       <c r="B24" s="2">
-        <v>97.7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>1102.18</v>
+        <v>24364.92</v>
       </c>
       <c r="B25" s="2">
-        <v>97.5</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>2294.1</v>
+        <v>8695.99</v>
       </c>
       <c r="B26" s="2">
-        <v>98</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>32817.24</v>
+        <v>4514.5600000000004</v>
       </c>
       <c r="B27" s="2">
-        <v>98.55</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>7143.43</v>
+        <v>338.98</v>
       </c>
       <c r="B28" s="2">
-        <v>97.85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>105166.05</v>
+        <v>5422.06</v>
       </c>
       <c r="B29" s="2">
-        <v>98.62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>41975.32</v>
+        <v>15000</v>
       </c>
       <c r="B30" s="2">
-        <v>98.55</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>9895.34</v>
+        <v>11341.42</v>
       </c>
       <c r="B31" s="2">
         <v>98.2</v>
@@ -1204,151 +1204,151 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>69203.34</v>
+        <v>11418.04</v>
       </c>
       <c r="B32" s="2">
-        <v>98.7</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>1495.23</v>
+        <v>17436.48</v>
       </c>
       <c r="B33" s="2">
-        <v>97.5</v>
+        <v>98.25</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>116329.75</v>
+        <v>75000</v>
       </c>
       <c r="B34" s="2">
-        <v>98.68</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>50540.12</v>
+        <v>94213.99</v>
       </c>
       <c r="B35" s="2">
-        <v>98.6</v>
+        <v>98.58</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>2441.5500000000002</v>
+        <v>6673.17</v>
       </c>
       <c r="B36" s="2">
-        <v>97.55</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>1721.29</v>
+        <v>34800.370000000003</v>
       </c>
       <c r="B37" s="2">
-        <v>97.25</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>791.03</v>
+        <v>17511.29</v>
       </c>
       <c r="B38" s="2">
-        <v>97</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>119543.07</v>
+        <v>7985.97</v>
       </c>
       <c r="B39" s="2">
-        <v>98.7</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>155370.54999999999</v>
+        <v>356.02</v>
       </c>
       <c r="B40" s="2">
-        <v>98.7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>91871.95</v>
+        <v>3708.93</v>
       </c>
       <c r="B41" s="2">
-        <v>99</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>274352.2</v>
+        <v>13147.47</v>
       </c>
       <c r="B42" s="2">
-        <v>98.7</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>11365.56</v>
+        <v>384.86</v>
       </c>
       <c r="B43" s="2">
-        <v>98.3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>9962.2800000000007</v>
+        <v>849</v>
       </c>
       <c r="B44" s="2">
-        <v>98.27</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>12203.68</v>
+        <v>1582.28</v>
       </c>
       <c r="B45" s="2">
-        <v>98.350499999999997</v>
+        <v>97.65</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>133857.72</v>
+        <v>23790.13</v>
       </c>
       <c r="B46" s="2">
-        <v>98.7</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>546.34</v>
+        <v>27227.93</v>
       </c>
       <c r="B47" s="2">
-        <v>97</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>13871.1</v>
+        <v>668.53</v>
       </c>
       <c r="B48" s="2">
-        <v>98.4</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>18250.7</v>
+        <v>1768.31</v>
       </c>
       <c r="B49" s="2">
-        <v>98.5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>2066.0100000000002</v>
+        <v>1499.72</v>
       </c>
       <c r="B50" s="2">
         <v>98</v>
@@ -1356,71 +1356,71 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>7768.28</v>
+        <v>60270.93</v>
       </c>
       <c r="B51" s="2">
-        <v>98.1</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>9893.6299999999992</v>
+        <v>269.16000000000003</v>
       </c>
       <c r="B52" s="2">
-        <v>98.1</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>2644.91</v>
+        <v>4018.08</v>
       </c>
       <c r="B53" s="2">
-        <v>98</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>1110.98</v>
+        <v>4405.8100000000004</v>
       </c>
       <c r="B54" s="2">
-        <v>97.65</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>26601.29</v>
+        <v>873.03</v>
       </c>
       <c r="B55" s="2">
-        <v>98.5</v>
+        <v>97.4</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>311.39</v>
+        <v>27806.21</v>
       </c>
       <c r="B56" s="2">
-        <v>94.75</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>47279.81</v>
+        <v>126117.97</v>
       </c>
       <c r="B57" s="2">
-        <v>98.6</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>789.44</v>
+        <v>1140.0899999999999</v>
       </c>
       <c r="B58" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>32053.23</v>
+        <v>70177.97</v>
       </c>
       <c r="B59" s="2">
         <v>98.5</v>
@@ -1428,311 +1428,311 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>1022.83</v>
+        <v>55684.69</v>
       </c>
       <c r="B60" s="2">
-        <v>97.65</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>11431.42</v>
+        <v>129341.51</v>
       </c>
       <c r="B61" s="2">
-        <v>98.27</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>7882.68</v>
+        <v>19621.28</v>
       </c>
       <c r="B62" s="2">
-        <v>98.27</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>7603.3</v>
+        <v>42675.6</v>
       </c>
       <c r="B63" s="2">
-        <v>98.25</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>1539.7</v>
+        <v>85348.93</v>
       </c>
       <c r="B64" s="2">
-        <v>98</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>7404.5</v>
+        <v>933000</v>
       </c>
       <c r="B65" s="2">
-        <v>98.2</v>
+        <v>98.72</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>1725.77</v>
+        <v>17137.8</v>
       </c>
       <c r="B66" s="2">
-        <v>97.75</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>4235.47</v>
+        <v>25411.75</v>
       </c>
       <c r="B67" s="2">
-        <v>98.25</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>2145</v>
+        <v>341340.42</v>
       </c>
       <c r="B68" s="2">
-        <v>98.05</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>114783.56</v>
+        <v>2723.1</v>
       </c>
       <c r="B69" s="2">
-        <v>98.75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>11390.1</v>
+        <v>17412.560000000001</v>
       </c>
       <c r="B70" s="2">
-        <v>98.4</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>983.01</v>
+        <v>2356.27</v>
       </c>
       <c r="B71" s="2">
-        <v>97.15</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>701.41</v>
+        <v>20116.87</v>
       </c>
       <c r="B72" s="2">
-        <v>97</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>297981.95</v>
+        <v>73497.31</v>
       </c>
       <c r="B73" s="2">
-        <v>99.1</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>106646.02</v>
+        <v>40000</v>
       </c>
       <c r="B74" s="2">
-        <v>98.75</v>
+        <v>98.56</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>50341.02</v>
+        <v>35000</v>
       </c>
       <c r="B75" s="2">
-        <v>98.5</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>204973.81</v>
+        <v>49572.959999999999</v>
       </c>
       <c r="B76" s="2">
-        <v>98.7</v>
+        <v>98.57</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>14589.42</v>
+        <v>21608.67</v>
       </c>
       <c r="B77" s="2">
-        <v>98</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>1354.36</v>
+        <v>4099.6499999999996</v>
       </c>
       <c r="B78" s="2">
-        <v>97.85</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>314.32</v>
+        <v>29008.17</v>
       </c>
       <c r="B79" s="2">
-        <v>94</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>1467.8</v>
+        <v>2166.94</v>
       </c>
       <c r="B80" s="2">
-        <v>97.5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>1667.12</v>
+        <v>556.38</v>
       </c>
       <c r="B81" s="2">
-        <v>97.8</v>
+        <v>97.25</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>1956.96</v>
+        <v>71784.490000000005</v>
       </c>
       <c r="B82" s="2">
-        <v>97.5</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>1999.69</v>
+        <v>22633.279999999999</v>
       </c>
       <c r="B83" s="2">
-        <v>97.5</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>3724.13</v>
+        <v>50970.06</v>
       </c>
       <c r="B84" s="2">
-        <v>97.8</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>1500</v>
+        <v>485000</v>
       </c>
       <c r="B85" s="2">
-        <v>97.65</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>4869.6899999999996</v>
+        <v>14768.64</v>
       </c>
       <c r="B86" s="2">
-        <v>98.2</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>686647.66</v>
+        <v>5016.7700000000004</v>
       </c>
       <c r="B87" s="2">
-        <v>98.73</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>21311.95</v>
+        <v>5652.76</v>
       </c>
       <c r="B88" s="2">
-        <v>98.6</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>26779.32</v>
+        <v>54400.78</v>
       </c>
       <c r="B89" s="2">
-        <v>98.5</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>3502.5</v>
+        <v>3516.54</v>
       </c>
       <c r="B90" s="2">
-        <v>98</v>
+        <v>98.05</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>72724.460000000006</v>
+        <v>42620.36</v>
       </c>
       <c r="B91" s="2">
-        <v>98.6</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>1727.17</v>
+        <v>60913.919999999998</v>
       </c>
       <c r="B92" s="2">
-        <v>97.8</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>297.52999999999997</v>
+        <v>15251.38</v>
       </c>
       <c r="B93" s="2">
-        <v>94.15</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>38572</v>
+        <v>828144.74</v>
       </c>
       <c r="B94" s="2">
-        <v>98.5</v>
+        <v>98.74</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>95244.51</v>
+        <v>2820.34</v>
       </c>
       <c r="B95" s="2">
-        <v>98.66</v>
+        <v>98.05</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>44082.03</v>
+        <v>2875790.28</v>
       </c>
       <c r="B96" s="2">
-        <v>98.6</v>
+        <v>98.826499999999996</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>20454.509999999998</v>
+        <v>1087.3399999999999</v>
       </c>
       <c r="B97" s="2">
-        <v>98.55</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>1592.56</v>
+        <v>1964.25</v>
       </c>
       <c r="B98" s="2">
         <v>98</v>
@@ -1740,287 +1740,287 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>4544.07</v>
+        <v>1520.21</v>
       </c>
       <c r="B99" s="2">
-        <v>98.2</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>1800</v>
+        <v>20506.02</v>
       </c>
       <c r="B100" s="2">
-        <v>97.7</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>12749</v>
+        <v>836393.82</v>
       </c>
       <c r="B101" s="2">
-        <v>98.3</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>15072.39</v>
+        <v>117091.76</v>
       </c>
       <c r="B102" s="2">
-        <v>98.5</v>
+        <v>98.65</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>1998.16</v>
+        <v>436.47</v>
       </c>
       <c r="B103" s="2">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>3480084.11</v>
+        <v>23653.06</v>
       </c>
       <c r="B104" s="2">
-        <v>98.92</v>
+        <v>98.46</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>1411.99</v>
+        <v>282365</v>
       </c>
       <c r="B105" s="2">
-        <v>97.7</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>191923.84</v>
+        <v>47341.21</v>
       </c>
       <c r="B106" s="2">
-        <v>98.75</v>
+        <v>98.63</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>36424.61</v>
+        <v>81551.960000000006</v>
       </c>
       <c r="B107" s="2">
-        <v>98.5</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>17972.28</v>
+        <v>20117.45</v>
       </c>
       <c r="B108" s="2">
-        <v>98.4</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>11053.91</v>
+        <v>286069.40999999997</v>
       </c>
       <c r="B109" s="2">
-        <v>98.5</v>
+        <v>98.63</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>1019.43</v>
+        <v>160000</v>
       </c>
       <c r="B110" s="2">
-        <v>98</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>785660.17</v>
+        <v>1841</v>
       </c>
       <c r="B111" s="2">
-        <v>98.82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>6001.16</v>
+        <v>1445.23</v>
       </c>
       <c r="B112" s="2">
-        <v>98.35</v>
+        <v>97.75</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>43800.31</v>
+        <v>4154.0600000000004</v>
       </c>
       <c r="B113" s="2">
-        <v>98.65</v>
+        <v>98</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>126320.71</v>
+        <v>4564.74</v>
       </c>
       <c r="B114" s="2">
-        <v>98.76</v>
+        <v>98</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>1944.69</v>
+        <v>475522.59</v>
       </c>
       <c r="B115" s="2">
-        <v>98.25</v>
+        <v>98.67</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>2109.7199999999998</v>
+        <v>17537.8</v>
       </c>
       <c r="B116" s="2">
-        <v>98</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>1823670.57</v>
+        <v>17200</v>
       </c>
       <c r="B117" s="2">
-        <v>98.85</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>1981.88</v>
+        <v>10990.42</v>
       </c>
       <c r="B118" s="2">
-        <v>98</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>3500</v>
+        <v>104011.57</v>
       </c>
       <c r="B119" s="2">
-        <v>98.15</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>11660.94</v>
+        <v>74179.87</v>
       </c>
       <c r="B120" s="2">
-        <v>98.35</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>579.37</v>
+        <v>7359.44</v>
       </c>
       <c r="B121" s="2">
-        <v>97</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>4211.59</v>
+        <v>8415.01</v>
       </c>
       <c r="B122" s="2">
-        <v>98</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>3184.65</v>
+        <v>1620.12</v>
       </c>
       <c r="B123" s="2">
-        <v>98</v>
+        <v>97.75</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>7749.75</v>
+        <v>4348.41</v>
       </c>
       <c r="B124" s="2">
-        <v>98.3</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>700.88</v>
+        <v>686.04</v>
       </c>
       <c r="B125" s="2">
-        <v>97.15</v>
+        <v>97</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>674.67</v>
+        <v>1740</v>
       </c>
       <c r="B126" s="2">
-        <v>97.15</v>
+        <v>97.75</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>57606.19</v>
+        <v>1474.23</v>
       </c>
       <c r="B127" s="2">
-        <v>98.6</v>
+        <v>98</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>114.05</v>
+        <v>18362.310000000001</v>
       </c>
       <c r="B128" s="2">
-        <v>92</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>180248.8</v>
+        <v>1003.28</v>
       </c>
       <c r="B129" s="2">
-        <v>98.75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>30380.37</v>
+        <v>1174.94</v>
       </c>
       <c r="B130" s="2">
-        <v>98.6</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>3326.78</v>
+        <v>5167.2</v>
       </c>
       <c r="B131" s="2">
-        <v>98.15</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>763.37</v>
+        <v>2623.13</v>
       </c>
       <c r="B132" s="2">
-        <v>97.25</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>1066.78</v>
+        <v>139597.66</v>
       </c>
       <c r="B133" s="2">
-        <v>98</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>1042.3699999999999</v>
+        <v>2215.6799999999998</v>
       </c>
       <c r="B134" s="2">
         <v>98</v>
@@ -2028,135 +2028,135 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>740.48</v>
+        <v>331034.51</v>
       </c>
       <c r="B135" s="2">
-        <v>97.15</v>
+        <v>98.67</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>41064.370000000003</v>
+        <v>20453.95</v>
       </c>
       <c r="B136" s="2">
-        <v>98.65</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>316081.23</v>
+        <v>598.75</v>
       </c>
       <c r="B137" s="2">
-        <v>98.8</v>
+        <v>97</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>2358.5500000000002</v>
+        <v>604.69000000000005</v>
       </c>
       <c r="B138" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>3505.96</v>
+        <v>61882.39</v>
       </c>
       <c r="B139" s="2">
-        <v>98.27</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>2268.19</v>
+        <v>2111.19</v>
       </c>
       <c r="B140" s="2">
-        <v>98.15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>9662</v>
+        <v>33088.33</v>
       </c>
       <c r="B141" s="2">
-        <v>98.45</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>47840.23</v>
+        <v>93813.59</v>
       </c>
       <c r="B142" s="2">
-        <v>98.5</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>3775.96</v>
+        <v>8306.8799999999992</v>
       </c>
       <c r="B143" s="2">
-        <v>97.7</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>295499.40000000002</v>
+        <v>9151.61</v>
       </c>
       <c r="B144" s="2">
-        <v>98.78</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>106446.86</v>
+        <v>9083.27</v>
       </c>
       <c r="B145" s="2">
-        <v>98.7</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>30369.9</v>
+        <v>331107.3</v>
       </c>
       <c r="B146" s="2">
-        <v>98.45</v>
+        <v>98.67</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>10791.06</v>
+        <v>2422.64</v>
       </c>
       <c r="B147" s="2">
-        <v>98.5</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>79605.55</v>
+        <v>114019.22</v>
       </c>
       <c r="B148" s="2">
-        <v>98.75</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>10694.37</v>
+        <v>3267.09</v>
       </c>
       <c r="B149" s="2">
-        <v>98.3</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>2214.6999999999998</v>
+        <v>186405.22</v>
       </c>
       <c r="B150" s="2">
-        <v>98.05</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>1806.39</v>
+        <v>2528.23</v>
       </c>
       <c r="B151" s="2">
         <v>98</v>
@@ -2164,167 +2164,167 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>10307.74</v>
+        <v>71561.94</v>
       </c>
       <c r="B152" s="2">
-        <v>98</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>9950.1200000000008</v>
+        <v>13756.25</v>
       </c>
       <c r="B153" s="2">
-        <v>98.1</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>53898.36</v>
+        <v>17190.7</v>
       </c>
       <c r="B154" s="2">
-        <v>98.65</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>1455.76</v>
+        <v>100320.01</v>
       </c>
       <c r="B155" s="2">
-        <v>98.1</v>
+        <v>98.62</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>1001.17</v>
+        <v>5058.2</v>
       </c>
       <c r="B156" s="2">
-        <v>98.1</v>
+        <v>98</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>14717.68</v>
+        <v>21420.9</v>
       </c>
       <c r="B157" s="2">
-        <v>98.45</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>17769.16</v>
+        <v>29457.32</v>
       </c>
       <c r="B158" s="2">
-        <v>98.4</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>717.96</v>
+        <v>575714.4</v>
       </c>
       <c r="B159" s="2">
-        <v>97</v>
+        <v>98.72</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>653526.97</v>
+        <v>22000</v>
       </c>
       <c r="B160" s="2">
-        <v>98.8</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>827.14</v>
+        <v>12971.42</v>
       </c>
       <c r="B161" s="2">
-        <v>97</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>26368.83</v>
+        <v>6127.65</v>
       </c>
       <c r="B162" s="2">
-        <v>98.55</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>323354.38</v>
+        <v>23609.38</v>
       </c>
       <c r="B163" s="2">
-        <v>98.8</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>17454.68</v>
+        <v>502248.04</v>
       </c>
       <c r="B164" s="2">
-        <v>98.4</v>
+        <v>98.67</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>59075.040000000001</v>
+        <v>21073.23</v>
       </c>
       <c r="B165" s="2">
-        <v>98.65</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>3355.47</v>
+        <v>82815.520000000004</v>
       </c>
       <c r="B166" s="2">
-        <v>98.1</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>128504.55</v>
+        <v>52933.78</v>
       </c>
       <c r="B167" s="2">
-        <v>98.63</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>30529.97</v>
+        <v>13565.3</v>
       </c>
       <c r="B168" s="2">
-        <v>98.5</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>1028.5</v>
+        <v>1755.86</v>
       </c>
       <c r="B169" s="2">
-        <v>97.75</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>8621.58</v>
+        <v>3438.65</v>
       </c>
       <c r="B170" s="2">
-        <v>98.35</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>526.67999999999995</v>
+        <v>250000</v>
       </c>
       <c r="B171" s="2">
-        <v>97</v>
+        <v>98.63</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>56991.95</v>
+        <v>18354.62</v>
       </c>
       <c r="B172" s="2">
         <v>98.5</v>
@@ -2332,127 +2332,127 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>3835.8</v>
+        <v>11387.1</v>
       </c>
       <c r="B173" s="2">
-        <v>98.15</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>2304.89</v>
+        <v>1914.94</v>
       </c>
       <c r="B174" s="2">
-        <v>98.15</v>
+        <v>97.65</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>218837.26</v>
+        <v>142163.5</v>
       </c>
       <c r="B175" s="2">
-        <v>98.8</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>659118.28</v>
+        <v>2000</v>
       </c>
       <c r="B176" s="2">
-        <v>98.805000000000007</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>3940</v>
+        <v>273103.59000000003</v>
       </c>
       <c r="B177" s="2">
-        <v>98.35</v>
+        <v>98.53</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>313711.71999999997</v>
+        <v>66777.210000000006</v>
       </c>
       <c r="B178" s="2">
-        <v>98.8</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>1677.87</v>
+        <v>51380.62</v>
       </c>
       <c r="B179" s="2">
-        <v>97.8</v>
+        <v>98.52</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>14248.66</v>
+        <v>85761.68</v>
       </c>
       <c r="B180" s="2">
-        <v>98.2</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>338.38</v>
+        <v>36139.24</v>
       </c>
       <c r="B181" s="2">
-        <v>96</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>250000</v>
+        <v>692356.32</v>
       </c>
       <c r="B182" s="2">
-        <v>98.87</v>
+        <v>98.68</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>331235.27</v>
+        <v>82519.509999999995</v>
       </c>
       <c r="B183" s="2">
-        <v>98.8</v>
+        <v>98.52</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>104688.22</v>
+        <v>542.64</v>
       </c>
       <c r="B184" s="2">
-        <v>98.73</v>
+        <v>96</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>206710.86</v>
+        <v>152610.57999999999</v>
       </c>
       <c r="B185" s="2">
-        <v>98.724999999999994</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>132844.78</v>
+        <v>1337.96</v>
       </c>
       <c r="B186" s="2">
-        <v>98.73</v>
+        <v>98</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>424.24</v>
+        <v>25165.97</v>
       </c>
       <c r="B187" s="2">
-        <v>95</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>1216.55</v>
+        <v>1291.23</v>
       </c>
       <c r="B188" s="2">
         <v>98</v>
@@ -2460,23 +2460,23 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>1268.47</v>
+        <v>1331.99</v>
       </c>
       <c r="B189" s="2">
-        <v>97.65</v>
+        <v>98</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>1992.79</v>
+        <v>8040.41</v>
       </c>
       <c r="B190" s="2">
-        <v>97.65</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>2247.52</v>
+        <v>3221.54</v>
       </c>
       <c r="B191" s="2">
         <v>98.1</v>
@@ -2484,753 +2484,1105 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
-        <v>24090.13</v>
+        <v>1644.39</v>
       </c>
       <c r="B192" s="2">
-        <v>98.55</v>
+        <v>98.05</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
-        <v>413796.88</v>
+        <v>12925.03</v>
       </c>
       <c r="B193" s="2">
-        <v>98.75</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>16481.919999999998</v>
+        <v>191.27</v>
       </c>
       <c r="B194" s="2">
-        <v>98.7</v>
+        <v>92</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>14899.97</v>
+        <v>25203.3</v>
       </c>
       <c r="B195" s="2">
-        <v>98.6</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
-        <v>867.45</v>
+        <v>18710.77</v>
       </c>
       <c r="B196" s="2">
-        <v>97.05</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
-        <v>7321.67</v>
+        <v>20814.03</v>
       </c>
       <c r="B197" s="2">
-        <v>98.3</v>
+        <v>98.43</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
-        <v>724.94</v>
+        <v>15132.36</v>
       </c>
       <c r="B198" s="2">
-        <v>97</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
-        <v>18611.02</v>
+        <v>28003.58</v>
       </c>
       <c r="B199" s="2">
-        <v>98.4</v>
+        <v>98.47</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
-        <v>16238.92</v>
+        <v>50836.17</v>
       </c>
       <c r="B200" s="2">
-        <v>98.5</v>
+        <v>98.48</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
-        <v>37715.69</v>
+        <v>165977.35</v>
       </c>
       <c r="B201" s="2">
-        <v>98.59</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
-        <v>32908.879999999997</v>
+        <v>2396.31</v>
       </c>
       <c r="B202" s="2">
-        <v>98.59</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
-        <v>19638.93</v>
+        <v>2258.96</v>
       </c>
       <c r="B203" s="2">
-        <v>98.6</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
-        <v>21124.28</v>
+        <v>553723.56999999995</v>
       </c>
       <c r="B204" s="2">
-        <v>98.5</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
-        <v>3157.07</v>
+        <v>5047.7700000000004</v>
       </c>
       <c r="B205" s="2">
-        <v>98.15</v>
+        <v>98.25</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
-        <v>39148.42</v>
+        <v>9944.44</v>
       </c>
       <c r="B206" s="2">
-        <v>98.6</v>
+        <v>98.25</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
-        <v>35582.720000000001</v>
+        <v>157950.94</v>
       </c>
       <c r="B207" s="2">
-        <v>98.6</v>
+        <v>98.52</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
-        <v>170581.05</v>
+        <v>907759.63</v>
       </c>
       <c r="B208" s="2">
-        <v>98.8</v>
+        <v>98.72</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
-        <v>165274.68</v>
+        <v>1798.06</v>
       </c>
       <c r="B209" s="2">
-        <v>98.75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
-        <v>46813.52</v>
+        <v>19226.36</v>
       </c>
       <c r="B210" s="2">
-        <v>98.6</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
-        <v>15129.12</v>
+        <v>52265.1</v>
       </c>
       <c r="B211" s="2">
-        <v>98.2</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
-        <v>30325.33</v>
+        <v>1387.28</v>
       </c>
       <c r="B212" s="2">
-        <v>98.59</v>
+        <v>98</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
-        <v>20303.07</v>
+        <v>1332.69</v>
       </c>
       <c r="B213" s="2">
-        <v>98.5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
-        <v>36885.08</v>
+        <v>775.1</v>
       </c>
       <c r="B214" s="2">
-        <v>98.5</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
-        <v>25395.360000000001</v>
+        <v>21372.15</v>
       </c>
       <c r="B215" s="2">
-        <v>98.55</v>
+        <v>98.65</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
-        <v>11459.96</v>
+        <v>36683.43</v>
       </c>
       <c r="B216" s="2">
-        <v>98.25</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
-        <v>2044.06</v>
+        <v>646539.82999999996</v>
       </c>
       <c r="B217" s="2">
-        <v>98.1</v>
+        <v>98.63</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
-        <v>1116.24</v>
+        <v>2903.44</v>
       </c>
       <c r="B218" s="2">
-        <v>98.15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
-        <v>4083.26</v>
+        <v>10363.700000000001</v>
       </c>
       <c r="B219" s="2">
-        <v>98.15</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
-        <v>23507.32</v>
+        <v>99367</v>
       </c>
       <c r="B220" s="2">
-        <v>98.4</v>
+        <v>98.58</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
-        <v>1607.27</v>
+        <v>28691.72</v>
       </c>
       <c r="B221" s="2">
-        <v>98</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
-        <v>865.89</v>
+        <v>43778.48</v>
       </c>
       <c r="B222" s="2">
-        <v>97.5</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
-        <v>115253.22</v>
+        <v>276103.73</v>
       </c>
       <c r="B223" s="2">
-        <v>98</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
-        <v>765587.33</v>
+        <v>1651152.05</v>
       </c>
       <c r="B224" s="2">
-        <v>98.8</v>
+        <v>98.81</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
-        <v>96379.91</v>
+        <v>2939.06</v>
       </c>
       <c r="B225" s="2">
-        <v>98.65</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
-        <v>21547.21</v>
+        <v>13804.59</v>
       </c>
       <c r="B226" s="2">
-        <v>98.5</v>
+        <v>98.32</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
-        <v>26960.21</v>
+        <v>28568.33</v>
       </c>
       <c r="B227" s="2">
-        <v>98.5</v>
+        <v>98.43</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
-        <v>915.75</v>
+        <v>9288.49</v>
       </c>
       <c r="B228" s="2">
-        <v>97.5</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
-        <v>1292.99</v>
+        <v>5152.57</v>
       </c>
       <c r="B229" s="2">
-        <v>97.8</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
-        <v>51519.46</v>
+        <v>2129.5300000000002</v>
       </c>
       <c r="B230" s="2">
-        <v>98.5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
-        <v>1339.26</v>
+        <v>16422.23</v>
       </c>
       <c r="B231" s="2">
-        <v>97.8</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
-        <v>115253.22</v>
+        <v>440.39</v>
       </c>
       <c r="B232" s="2">
-        <v>98.7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
-        <v>698071.3</v>
+        <v>668.92</v>
       </c>
       <c r="B233" s="2">
-        <v>98.8</v>
+        <v>97</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
-        <v>466799.42</v>
+        <v>13928.57</v>
       </c>
       <c r="B234" s="2">
-        <v>98.75</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
-        <v>130580.83</v>
+        <v>367733.43</v>
       </c>
       <c r="B235" s="2">
-        <v>98.5</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
-        <v>61283.4</v>
+        <v>2533.13</v>
       </c>
       <c r="B236" s="2">
-        <v>98.5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
-        <v>161947.10999999999</v>
+        <v>20169.89</v>
       </c>
       <c r="B237" s="2">
-        <v>98.65</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
-        <v>53756.2</v>
+        <v>825.84</v>
       </c>
       <c r="B238" s="2">
-        <v>98.5</v>
+        <v>97.1</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
-        <v>16266.37</v>
+        <v>70241.119999999995</v>
       </c>
       <c r="B239" s="2">
-        <v>98.4</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
-        <v>70.37</v>
+        <v>114805.73</v>
       </c>
       <c r="B240" s="2">
-        <v>92</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
-        <v>19000</v>
+        <v>110063.41</v>
       </c>
       <c r="B241" s="2">
-        <v>98.5</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
-        <v>61699.49</v>
+        <v>3029.85</v>
       </c>
       <c r="B242" s="2">
-        <v>98.75</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
-        <v>4794.3</v>
+        <v>4475.72</v>
       </c>
       <c r="B243" s="2">
-        <v>98</v>
+        <v>98.18</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
-        <v>1099.44</v>
+        <v>84099.05</v>
       </c>
       <c r="B244" s="2">
-        <v>98.1</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
-        <v>30656.42</v>
+        <v>2059.54</v>
       </c>
       <c r="B245" s="2">
-        <v>98.6</v>
+        <v>98.25</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
-        <v>144140.88</v>
+        <v>31633.1</v>
       </c>
       <c r="B246" s="2">
-        <v>98.75</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
-        <v>2123.6</v>
+        <v>83288.09</v>
       </c>
       <c r="B247" s="2">
-        <v>98</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
-        <v>244520.9</v>
+        <v>5057.08</v>
       </c>
       <c r="B248" s="2">
-        <v>98.75</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
-        <v>903.49</v>
+        <v>50527.81</v>
       </c>
       <c r="B249" s="2">
-        <v>97.1</v>
+        <v>98.51</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
-        <v>93175.57</v>
+        <v>251551.15</v>
       </c>
       <c r="B250" s="2">
-        <v>98.75</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
-        <v>730845.89</v>
+        <v>656643.14</v>
       </c>
       <c r="B251" s="2">
-        <v>98.8</v>
+        <v>98.68</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
-        <v>425.63</v>
+        <v>235261.27</v>
       </c>
       <c r="B252" s="2">
-        <v>97.05</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
-        <v>1063.25</v>
+        <v>3345.28</v>
       </c>
       <c r="B253" s="2">
-        <v>98.17</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
-        <v>8637.1</v>
+        <v>23100.58</v>
       </c>
       <c r="B254" s="2">
-        <v>98.3</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
-        <v>357734.82</v>
+        <v>6166.97</v>
       </c>
       <c r="B255" s="2">
-        <v>98.8</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
-        <v>12749.58</v>
+        <v>18597.45</v>
       </c>
       <c r="B256" s="2">
-        <v>98.25</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
-        <v>14141.41</v>
+        <v>3901.77</v>
       </c>
       <c r="B257" s="2">
-        <v>98.35</v>
+        <v>98</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
-        <v>18991.900000000001</v>
+        <v>6192.15</v>
       </c>
       <c r="B258" s="2">
-        <v>98.4</v>
+        <v>98</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
-        <v>15415.54</v>
+        <v>7801.72</v>
       </c>
       <c r="B259" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" s="2">
+        <v>15709.84</v>
+      </c>
+      <c r="B260" s="3">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" s="2">
+        <v>645.76</v>
+      </c>
+      <c r="B261" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" s="2">
+        <v>990.33</v>
+      </c>
+      <c r="B262" s="1">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" s="2">
+        <v>1310.03</v>
+      </c>
+      <c r="B263" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" s="2">
+        <v>7680.09</v>
+      </c>
+      <c r="B264" s="1">
+        <v>98.1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" s="2">
+        <v>1117.26</v>
+      </c>
+      <c r="B265" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" s="2">
+        <v>12154.7</v>
+      </c>
+      <c r="B266" s="1">
+        <v>98.2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" s="2">
+        <v>5608.06</v>
+      </c>
+      <c r="B267" s="1">
+        <v>98.25</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" s="2">
+        <v>5786.55</v>
+      </c>
+      <c r="B268" s="1">
+        <v>98.25</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" s="2">
+        <v>1162.24</v>
+      </c>
+      <c r="B269" s="1">
+        <v>98.15</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" s="2">
+        <v>27075.67</v>
+      </c>
+      <c r="B270" s="1">
+        <v>98.65</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" s="2">
+        <v>111742.79</v>
+      </c>
+      <c r="B271" s="1">
         <v>98.5</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="3">
-        <v>23497.18</v>
-      </c>
-      <c r="B260" s="3">
-        <v>98.45</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="1">
-        <v>8812.0400000000009</v>
-      </c>
-      <c r="B261" s="1">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" s="2">
+        <v>58394.28</v>
+      </c>
+      <c r="B272" s="1">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" s="2">
+        <v>4539.8599999999997</v>
+      </c>
+      <c r="B273" s="1">
+        <v>98.25</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" s="2">
+        <v>1315.05</v>
+      </c>
+      <c r="B274" s="1">
+        <v>98.05</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" s="2">
+        <v>272141.78000000003</v>
+      </c>
+      <c r="B275" s="1">
+        <v>98.63</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" s="2">
+        <v>482821.74</v>
+      </c>
+      <c r="B276" s="1">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" s="2">
+        <v>116629.11</v>
+      </c>
+      <c r="B277" s="1">
+        <v>98.55</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" s="2">
+        <v>507923.18</v>
+      </c>
+      <c r="B278" s="1">
+        <v>98.7</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="2">
+        <v>23355.759999999998</v>
+      </c>
+      <c r="B279" s="1">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="2">
+        <v>4742.29</v>
+      </c>
+      <c r="B280" s="1">
+        <v>98.1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="2">
+        <v>3879.07</v>
+      </c>
+      <c r="B281" s="1">
+        <v>98.15</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="2">
+        <v>2162.4</v>
+      </c>
+      <c r="B282" s="1">
+        <v>98.15</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" s="2">
+        <v>13627.52</v>
+      </c>
+      <c r="B283" s="1">
         <v>98.3</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="1">
-        <v>4915.54</v>
-      </c>
-      <c r="B262" s="1">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" s="2">
+        <v>1502.43</v>
+      </c>
+      <c r="B284" s="1">
+        <v>98.15</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" s="2">
+        <v>31531.56</v>
+      </c>
+      <c r="B285" s="1">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" s="2">
+        <v>723.22</v>
+      </c>
+      <c r="B286" s="1">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" s="2">
+        <v>72106.5</v>
+      </c>
+      <c r="B287" s="1">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" s="2">
+        <v>23585.5</v>
+      </c>
+      <c r="B288" s="1">
+        <v>98.43</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" s="2">
+        <v>165843.82999999999</v>
+      </c>
+      <c r="B289" s="1">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" s="2">
+        <v>1333.91</v>
+      </c>
+      <c r="B290" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" s="2">
+        <v>18685.34</v>
+      </c>
+      <c r="B291" s="1">
         <v>98.3</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="1">
-        <v>59798.29</v>
-      </c>
-      <c r="B263" s="1">
-        <v>98.6</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="1">
-        <v>300000</v>
-      </c>
-      <c r="B264" s="1">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" s="2">
+        <v>607.08000000000004</v>
+      </c>
+      <c r="B292" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" s="2">
+        <v>2051.17</v>
+      </c>
+      <c r="B293" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" s="2">
+        <v>145184.98000000001</v>
+      </c>
+      <c r="B294" s="1">
+        <v>98.62</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" s="2">
+        <v>11808.84</v>
+      </c>
+      <c r="B295" s="1">
+        <v>98.2</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" s="2">
+        <v>1884.24</v>
+      </c>
+      <c r="B296" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" s="2">
+        <v>44666.39</v>
+      </c>
+      <c r="B297" s="1">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" s="2">
+        <v>107241.81</v>
+      </c>
+      <c r="B298" s="1">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" s="2">
+        <v>2264.77</v>
+      </c>
+      <c r="B299" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" s="2">
+        <v>4629.92</v>
+      </c>
+      <c r="B300" s="1">
+        <v>98.2</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" s="2">
+        <v>447.24</v>
+      </c>
+      <c r="B301" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" s="2">
+        <v>934.37</v>
+      </c>
+      <c r="B302" s="1">
+        <v>97.75</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" s="2">
+        <v>15841.61</v>
+      </c>
+      <c r="B303" s="1">
+        <v>98.2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" s="2">
+        <v>807.37</v>
+      </c>
+      <c r="B304" s="1">
+        <v>97.4</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" s="2">
+        <v>2682.08</v>
+      </c>
+      <c r="B305" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" s="2">
+        <v>29503.99</v>
+      </c>
+      <c r="B306" s="1">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" s="2">
+        <v>29055.66</v>
+      </c>
+      <c r="B307" s="1">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308" s="2">
+        <v>2674.53</v>
+      </c>
+      <c r="B308" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309" s="2">
+        <v>530.58000000000004</v>
+      </c>
+      <c r="B309" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310" s="2">
+        <v>587613.76</v>
+      </c>
+      <c r="B310" s="1">
         <v>98.7</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="1">
-        <v>126357.57</v>
-      </c>
-      <c r="B265" s="1">
-        <v>98.7</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="1">
-        <v>1843.11</v>
-      </c>
-      <c r="B266" s="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="1">
-        <v>13689.06</v>
-      </c>
-      <c r="B267" s="1">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311" s="2">
+        <v>7126.75</v>
+      </c>
+      <c r="B311" s="1">
+        <v>98.25</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" s="2">
+        <v>4094.79</v>
+      </c>
+      <c r="B312" s="1">
+        <v>98.25</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313" s="2">
+        <v>2591.4899999999998</v>
+      </c>
+      <c r="B313" s="1">
+        <v>98.1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" s="2">
+        <v>1315881.7</v>
+      </c>
+      <c r="B314" s="1">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" s="2">
+        <v>3543.86</v>
+      </c>
+      <c r="B315" s="1">
+        <v>98.2</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" s="2">
+        <v>64784.54</v>
+      </c>
+      <c r="B316" s="1">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" s="2">
+        <v>21646.83</v>
+      </c>
+      <c r="B317" s="1">
         <v>98.35</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="1">
-        <v>235859.12</v>
-      </c>
-      <c r="B268" s="1">
-        <v>98.81</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="1">
-        <v>138948.44</v>
-      </c>
-      <c r="B269" s="1">
-        <v>98.6</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="1">
-        <v>76694.509999999995</v>
-      </c>
-      <c r="B270" s="1">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318" s="2">
+        <v>69707.210000000006</v>
+      </c>
+      <c r="B318" s="1">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319" s="2">
+        <v>22043.200000000001</v>
+      </c>
+      <c r="B319" s="1">
+        <v>98.43</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" s="2">
+        <v>25000</v>
+      </c>
+      <c r="B320" s="1">
+        <v>98.43</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" s="2">
+        <v>76338.09</v>
+      </c>
+      <c r="B321" s="1">
         <v>98.75</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="1">
-        <v>5175.0600000000004</v>
-      </c>
-      <c r="B271" s="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="1">
-        <v>334956.75</v>
-      </c>
-      <c r="B272" s="1">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" s="2">
+        <v>1649.42</v>
+      </c>
+      <c r="B322" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" s="2">
+        <v>76338.09</v>
+      </c>
+      <c r="B323" s="1">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" s="2">
+        <v>7848.06</v>
+      </c>
+      <c r="B324" s="1">
+        <v>98.3</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" s="2">
+        <v>20987.46</v>
+      </c>
+      <c r="B325" s="1">
+        <v>98.43</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" s="2">
+        <v>8050.28</v>
+      </c>
+      <c r="B326" s="1">
         <v>98.25</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="1">
-        <v>7627.95</v>
-      </c>
-      <c r="B273" s="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="1">
-        <v>26892.05</v>
-      </c>
-      <c r="B274" s="1">
-        <v>98.5</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="1">
-        <v>127850.95</v>
-      </c>
-      <c r="B275" s="1">
-        <v>98.6</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="1">
-        <v>316.41000000000003</v>
-      </c>
-      <c r="B276" s="1">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="1">
-        <v>1287.21</v>
-      </c>
-      <c r="B277" s="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="1">
-        <v>1966.37</v>
-      </c>
-      <c r="B278" s="1">
-        <v>97.65</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="1">
-        <v>8390.92</v>
-      </c>
-      <c r="B279" s="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="1">
-        <v>11909.69</v>
-      </c>
-      <c r="B280" s="1">
-        <v>98.3</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="1">
-        <v>1033.3</v>
-      </c>
-      <c r="B281" s="1">
-        <v>97.65</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="1">
-        <v>2508.64</v>
-      </c>
-      <c r="B282" s="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="1">
-        <v>21838.799999999999</v>
-      </c>
-      <c r="B283" s="1">
-        <v>98.4</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="1">
-        <v>9658.0499999999993</v>
-      </c>
-      <c r="B284" s="1">
-        <v>98.1</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="1">
-        <v>7929.12</v>
-      </c>
-      <c r="B285" s="1">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" s="2">
+        <v>54324.06</v>
+      </c>
+      <c r="B327" s="1">
+        <v>98.55</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" s="2">
+        <v>140000</v>
+      </c>
+      <c r="B328" s="1">
+        <v>98.57</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" s="2">
+        <v>3788.27</v>
+      </c>
+      <c r="B329" s="1">
         <v>98.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nc semanal 23 - 27 de febrero
</commit_message>
<xml_diff>
--- a/data/NC_semanal.xlsx
+++ b/data/NC_semanal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Desktop\MetrovaloresApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348FCA56-4248-41D6-BEA5-74C1E596E38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1521EB4-368B-44C0-90B6-CB9A77B3B502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{9E78C8B1-ED59-4A81-8FF9-F1A88ED1C1A0}"/>
   </bookViews>
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077B50AF-9C9F-4CF5-BB56-A27ACF5565DE}">
   <dimension ref="A1:B329"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A189"/>
+    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
+      <selection activeCell="D263" sqref="D263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,55 +964,55 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>50040.27</v>
+        <v>26689.62</v>
       </c>
       <c r="B2" s="2">
-        <v>98.55</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>18800.02</v>
+        <v>20016.41</v>
       </c>
       <c r="B3" s="2">
-        <v>98.35</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>111083.85</v>
+        <v>24155.49</v>
       </c>
       <c r="B4" s="2">
-        <v>98.65</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>233619.05</v>
+        <v>4816.92</v>
       </c>
       <c r="B5" s="2">
-        <v>98.65</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>743916.91</v>
+        <v>762.49</v>
       </c>
       <c r="B6" s="2">
-        <v>98.78</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>4933.3500000000004</v>
+        <v>35270.269999999997</v>
       </c>
       <c r="B7" s="2">
-        <v>98.2</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>35270.06</v>
+        <v>20706.03</v>
       </c>
       <c r="B8" s="2">
         <v>98.45</v>
@@ -1020,255 +1020,255 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>27487.279999999999</v>
+        <v>1155398.49</v>
       </c>
       <c r="B9" s="2">
-        <v>98.4</v>
+        <v>98.844999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>18719.32</v>
+        <v>135163.28</v>
       </c>
       <c r="B10" s="2">
-        <v>98.3</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>14500</v>
+        <v>3138.86</v>
       </c>
       <c r="B11" s="2">
-        <v>98.4</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>36263.39</v>
+        <v>44941.45</v>
       </c>
       <c r="B12" s="2">
-        <v>98.48</v>
+        <v>98.56</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>1643787.51</v>
+        <v>2166.9499999999998</v>
       </c>
       <c r="B13" s="2">
-        <v>98.8</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>13216.28</v>
+        <v>5896</v>
       </c>
       <c r="B14" s="2">
-        <v>98.4</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>92981.8</v>
+        <v>15115.26</v>
       </c>
       <c r="B15" s="2">
-        <v>98.56</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>1117.97</v>
+        <v>6226.89</v>
       </c>
       <c r="B16" s="2">
-        <v>98</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>28166.43</v>
+        <v>267835.90000000002</v>
       </c>
       <c r="B17" s="2">
-        <v>98.4</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>1038.21</v>
+        <v>2843</v>
       </c>
       <c r="B18" s="2">
-        <v>98</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>7305.13</v>
+        <v>6188.45</v>
       </c>
       <c r="B19" s="2">
-        <v>98.15</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>2266.19</v>
+        <v>1036.33</v>
       </c>
       <c r="B20" s="2">
-        <v>98</v>
+        <v>98.05</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>747.12</v>
+        <v>38382.75</v>
       </c>
       <c r="B21" s="2">
-        <v>97</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>432000.83</v>
+        <v>20958.439999999999</v>
       </c>
       <c r="B22" s="2">
-        <v>98.69</v>
+        <v>98.43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>90338.91</v>
+        <v>1564.7</v>
       </c>
       <c r="B23" s="2">
-        <v>98.55</v>
+        <v>98.25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>85104.66</v>
+        <v>124427.23</v>
       </c>
       <c r="B24" s="2">
-        <v>98.5</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>38604.17</v>
+        <v>243301.58</v>
       </c>
       <c r="B25" s="2">
-        <v>98.5</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>629.19000000000005</v>
+        <v>251499.76</v>
       </c>
       <c r="B26" s="2">
-        <v>97</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>13694.34</v>
+        <v>31113.48</v>
       </c>
       <c r="B27" s="2">
-        <v>98.45</v>
+        <v>98.65</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>5308.17</v>
+        <v>285522.5</v>
       </c>
       <c r="B28" s="2">
-        <v>98.15</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>8449.59</v>
+        <v>663052.13</v>
       </c>
       <c r="B29" s="2">
-        <v>98</v>
+        <v>98.82</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>26583.93</v>
+        <v>25269.17</v>
       </c>
       <c r="B30" s="2">
-        <v>98.4</v>
+        <v>98.65</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>148274.16</v>
+        <v>2119.61</v>
       </c>
       <c r="B31" s="2">
-        <v>98.65</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>16089.23</v>
+        <v>345.26</v>
       </c>
       <c r="B32" s="2">
-        <v>98.2</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>59318.91</v>
+        <v>3803.13</v>
       </c>
       <c r="B33" s="2">
-        <v>98.5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>21812.75</v>
+        <v>20624.91</v>
       </c>
       <c r="B34" s="2">
-        <v>98.35</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>5133.01</v>
+        <v>52558.8</v>
       </c>
       <c r="B35" s="2">
-        <v>98.2</v>
+        <v>98.65</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>5000</v>
+        <v>21757.42</v>
       </c>
       <c r="B36" s="2">
-        <v>98.2</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>4502.66</v>
+        <v>1074.97</v>
       </c>
       <c r="B37" s="2">
-        <v>98.15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>1022.36</v>
+        <v>1384.49</v>
       </c>
       <c r="B38" s="2">
-        <v>97.5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>436193.36</v>
+        <v>2046.68</v>
       </c>
       <c r="B39" s="2">
-        <v>98.69</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>58292.26</v>
+        <v>36106.49</v>
       </c>
       <c r="B40" s="2">
         <v>98.5</v>
@@ -1276,247 +1276,247 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>26406.959999999999</v>
+        <v>52643.97</v>
       </c>
       <c r="B41" s="2">
-        <v>98.35</v>
+        <v>98.67</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>5314.67</v>
+        <v>1181.6400000000001</v>
       </c>
       <c r="B42" s="2">
-        <v>98.1</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>3383.54</v>
+        <v>95891.24</v>
       </c>
       <c r="B43" s="2">
-        <v>97.5</v>
+        <v>98.65</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>10383.94</v>
+        <v>1650</v>
       </c>
       <c r="B44" s="2">
-        <v>98.5</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>1847.62</v>
+        <v>17414.89</v>
       </c>
       <c r="B45" s="2">
-        <v>98</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>133191.81</v>
+        <v>1503.98</v>
       </c>
       <c r="B46" s="2">
-        <v>98.5</v>
+        <v>98.05</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>30034.94</v>
+        <v>7204</v>
       </c>
       <c r="B47" s="2">
-        <v>98.45</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>7700.57</v>
+        <v>16302.3</v>
       </c>
       <c r="B48" s="2">
-        <v>98.2</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>3870.5</v>
+        <v>1082436.73</v>
       </c>
       <c r="B49" s="2">
-        <v>98</v>
+        <v>98.827500000000001</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>3468.84</v>
+        <v>2953.45</v>
       </c>
       <c r="B50" s="2">
-        <v>98</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>322.64</v>
+        <v>70301.820000000007</v>
       </c>
       <c r="B51" s="2">
-        <v>94</v>
+        <v>98.65</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>1706.55</v>
+        <v>511235.21</v>
       </c>
       <c r="B52" s="2">
-        <v>98</v>
+        <v>98.77</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>181158.95</v>
+        <v>665.69</v>
       </c>
       <c r="B53" s="2">
-        <v>98.65</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>20756.64</v>
+        <v>2059.54</v>
       </c>
       <c r="B54" s="2">
-        <v>98.43</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>6035.28</v>
+        <v>231.77</v>
       </c>
       <c r="B55" s="2">
-        <v>98.2</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>54365.88</v>
+        <v>1234.6500000000001</v>
       </c>
       <c r="B56" s="2">
-        <v>98.5</v>
+        <v>98.25</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>1826.07</v>
+        <v>21800.9</v>
       </c>
       <c r="B57" s="2">
-        <v>98</v>
+        <v>98.65</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>1408.55</v>
+        <v>2600</v>
       </c>
       <c r="B58" s="2">
-        <v>98</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>17430.88</v>
+        <v>1938.99</v>
       </c>
       <c r="B59" s="2">
-        <v>98.35</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>50903.58</v>
+        <v>25171.46</v>
       </c>
       <c r="B60" s="2">
-        <v>98.55</v>
+        <v>98.65</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>176000</v>
+        <v>5019.67</v>
       </c>
       <c r="B61" s="2">
-        <v>98.57</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>6887.04</v>
+        <v>2158.42</v>
       </c>
       <c r="B62" s="2">
-        <v>98.15</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>10612.74</v>
+        <v>3859837.33</v>
       </c>
       <c r="B63" s="2">
-        <v>98.4</v>
+        <v>99.037099999999995</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>642</v>
+        <v>4569.1499999999996</v>
       </c>
       <c r="B64" s="2">
-        <v>96</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>831.5</v>
+        <v>24588.6</v>
       </c>
       <c r="B65" s="2">
-        <v>97</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>476613.07</v>
+        <v>179219.07</v>
       </c>
       <c r="B66" s="2">
-        <v>98.72</v>
+        <v>98.77</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>5540.49</v>
+        <v>90839.44</v>
       </c>
       <c r="B67" s="2">
-        <v>98.3</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>2124.85</v>
+        <v>200893.45</v>
       </c>
       <c r="B68" s="2">
-        <v>98</v>
+        <v>98.8</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>358.86</v>
+        <v>288884.49</v>
       </c>
       <c r="B69" s="2">
-        <v>94</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>26091.439999999999</v>
+        <v>1135028.31</v>
       </c>
       <c r="B70" s="2">
-        <v>98.45</v>
+        <v>98.85</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>3404.41</v>
+        <v>2813.11</v>
       </c>
       <c r="B71" s="2">
         <v>98.15</v>
@@ -1524,183 +1524,183 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>21387.32</v>
+        <v>1306.54</v>
       </c>
       <c r="B72" s="2">
-        <v>98.45</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>196989.94</v>
+        <v>7785.93</v>
       </c>
       <c r="B73" s="2">
-        <v>98.65</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>16476.400000000001</v>
+        <v>2285.7800000000002</v>
       </c>
       <c r="B74" s="2">
-        <v>98.4</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>1594.26</v>
+        <v>4807.04</v>
       </c>
       <c r="B75" s="2">
-        <v>98.2</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>9841.57</v>
+        <v>43495.96</v>
       </c>
       <c r="B76" s="2">
-        <v>98.2</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>311033.36</v>
+        <v>3202.29</v>
       </c>
       <c r="B77" s="2">
-        <v>98.7</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>40902.699999999997</v>
+        <v>20724.939999999999</v>
       </c>
       <c r="B78" s="2">
-        <v>98.55</v>
+        <v>98.65</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>68989.95</v>
+        <v>200704.77</v>
       </c>
       <c r="B79" s="2">
-        <v>98.600099999999998</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>19164.150000000001</v>
+        <v>17066.36</v>
       </c>
       <c r="B80" s="2">
-        <v>98.25</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>315.14</v>
+        <v>13174.87</v>
       </c>
       <c r="B81" s="2">
-        <v>93</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>33365.120000000003</v>
+        <v>39102.800000000003</v>
       </c>
       <c r="B82" s="2">
-        <v>98.5501</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>41285.760000000002</v>
+        <v>8912.41</v>
       </c>
       <c r="B83" s="2">
-        <v>98.55</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>174858.79</v>
+        <v>15986.85</v>
       </c>
       <c r="B84" s="2">
-        <v>98.6</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>184980.58</v>
+        <v>94643.45</v>
       </c>
       <c r="B85" s="2">
-        <v>98.65</v>
+        <v>98.750100000000003</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>53659.05</v>
+        <v>1705645.17</v>
       </c>
       <c r="B86" s="2">
-        <v>98.6</v>
+        <v>98.87</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>2107.9499999999998</v>
+        <v>2377</v>
       </c>
       <c r="B87" s="2">
-        <v>98.2</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>125259.02</v>
+        <v>88028.65</v>
       </c>
       <c r="B88" s="2">
-        <v>98.65</v>
+        <v>98.81</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>6815.08</v>
+        <v>7000</v>
       </c>
       <c r="B89" s="2">
-        <v>98.35</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>81803.009999999995</v>
+        <v>26503.56</v>
       </c>
       <c r="B90" s="2">
-        <v>98.55</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>136887.4</v>
+        <v>22451.13</v>
       </c>
       <c r="B91" s="2">
-        <v>98.6</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>93111.360000000001</v>
+        <v>5590.92</v>
       </c>
       <c r="B92" s="2">
-        <v>98.6</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>38815.57</v>
+        <v>90866.89</v>
       </c>
       <c r="B93" s="2">
-        <v>98.55</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>46820.99</v>
+        <v>1945.49</v>
       </c>
       <c r="B94" s="2">
         <v>98.5</v>
@@ -1708,327 +1708,327 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>204692.27</v>
+        <v>83790.02</v>
       </c>
       <c r="B95" s="2">
-        <v>98.65</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>76588.5</v>
+        <v>926.48</v>
       </c>
       <c r="B96" s="2">
-        <v>98.7</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>3091.63</v>
+        <v>10088.51</v>
       </c>
       <c r="B97" s="2">
-        <v>98.25</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>3469.51</v>
+        <v>2888.86</v>
       </c>
       <c r="B98" s="2">
-        <v>98.15</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>924118.95</v>
+        <v>1664845.78</v>
       </c>
       <c r="B99" s="2">
-        <v>98.78</v>
+        <v>98.97</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>1379.74</v>
+        <v>704339.53</v>
       </c>
       <c r="B100" s="2">
-        <v>98.1</v>
+        <v>98.82</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>4065.56</v>
+        <v>4601.41</v>
       </c>
       <c r="B101" s="2">
-        <v>98.1</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>6438.45</v>
+        <v>9571.2199999999993</v>
       </c>
       <c r="B102" s="2">
-        <v>98.3</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>2694.29</v>
+        <v>41222.68</v>
       </c>
       <c r="B103" s="2">
-        <v>98.1</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>22670.18</v>
+        <v>28670.86</v>
       </c>
       <c r="B104" s="2">
-        <v>98.45</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>12469.34</v>
+        <v>3848.38</v>
       </c>
       <c r="B105" s="2">
-        <v>98.5</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>1190.05</v>
+        <v>363091.73</v>
       </c>
       <c r="B106" s="2">
-        <v>98</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>3394.46</v>
+        <v>2478.75</v>
       </c>
       <c r="B107" s="2">
-        <v>98.1</v>
+        <v>98</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>37246.870000000003</v>
+        <v>1403.85</v>
       </c>
       <c r="B108" s="2">
-        <v>98.52</v>
+        <v>98</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>17521.7</v>
+        <v>44424.84</v>
       </c>
       <c r="B109" s="2">
-        <v>98.5</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>640771.71</v>
+        <v>525.21</v>
       </c>
       <c r="B110" s="2">
-        <v>98.72</v>
+        <v>98.061000000000007</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>16706.48</v>
+        <v>2246.09</v>
       </c>
       <c r="B111" s="2">
-        <v>98.45</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>2392.81</v>
+        <v>296801.64</v>
       </c>
       <c r="B112" s="2">
-        <v>98</v>
+        <v>98.8</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>14293.68</v>
+        <v>590.94000000000005</v>
       </c>
       <c r="B113" s="2">
-        <v>98.4</v>
+        <v>98</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>27005.599999999999</v>
+        <v>1038</v>
       </c>
       <c r="B114" s="2">
-        <v>98.45</v>
+        <v>97.15</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>1305.76</v>
+        <v>2835.75</v>
       </c>
       <c r="B115" s="2">
-        <v>98</v>
+        <v>98.15</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>65496.480000000003</v>
+        <v>25974.78</v>
       </c>
       <c r="B116" s="2">
-        <v>98.6</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>30870.080000000002</v>
+        <v>63893.47</v>
       </c>
       <c r="B117" s="2">
-        <v>98.6</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>4244.4799999999996</v>
+        <v>2323.06</v>
       </c>
       <c r="B118" s="2">
-        <v>98.2</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>2163.81</v>
+        <v>71812.25</v>
       </c>
       <c r="B119" s="2">
-        <v>98.1</v>
+        <v>98.68</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>7000</v>
+        <v>925.59</v>
       </c>
       <c r="B120" s="2">
-        <v>98.2</v>
+        <v>98.26</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>10520.54</v>
+        <v>3520.13</v>
       </c>
       <c r="B121" s="2">
-        <v>98.4</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>193870.58</v>
+        <v>1287.21</v>
       </c>
       <c r="B122" s="2">
-        <v>98.57</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>10876.82</v>
+        <v>2819.6</v>
       </c>
       <c r="B123" s="2">
-        <v>98.5</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>45000</v>
+        <v>1415.58</v>
       </c>
       <c r="B124" s="2">
-        <v>98.55</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>9123.89</v>
+        <v>2045.35</v>
       </c>
       <c r="B125" s="2">
-        <v>98.4</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>9617.68</v>
+        <v>137195.79999999999</v>
       </c>
       <c r="B126" s="2">
-        <v>98.4</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>24384.95</v>
+        <v>404727.63</v>
       </c>
       <c r="B127" s="2">
-        <v>98.75</v>
+        <v>98.8</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>5443.52</v>
+        <v>2000</v>
       </c>
       <c r="B128" s="2">
-        <v>98.25</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>24384.95</v>
+        <v>925.96</v>
       </c>
       <c r="B129" s="2">
-        <v>98.6</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>4872.55</v>
+        <v>1270.51</v>
       </c>
       <c r="B130" s="2">
-        <v>98.2</v>
+        <v>98</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>549928.94999999995</v>
+        <v>2103.46</v>
       </c>
       <c r="B131" s="2">
-        <v>98.8</v>
+        <v>98</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>11910.16</v>
+        <v>2306.11</v>
       </c>
       <c r="B132" s="2">
-        <v>98.3</v>
+        <v>98</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>406.02</v>
+        <v>2258.6799999999998</v>
       </c>
       <c r="B133" s="2">
-        <v>97</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>9705.68</v>
+        <v>7812.75</v>
       </c>
       <c r="B134" s="2">
-        <v>98.25</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>3471.29</v>
+        <v>5448.32</v>
       </c>
       <c r="B135" s="2">
         <v>98.3</v>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>1047</v>
+        <v>1907.55</v>
       </c>
       <c r="B136" s="2">
         <v>98.1</v>
@@ -2044,47 +2044,47 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>54094.97</v>
+        <v>20571.79</v>
       </c>
       <c r="B137" s="2">
-        <v>98.6</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>3213.65</v>
+        <v>1640.19</v>
       </c>
       <c r="B138" s="2">
-        <v>98.2</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>3078.31</v>
+        <v>45196.84</v>
       </c>
       <c r="B139" s="2">
-        <v>98.3</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>10134.01</v>
+        <v>186497.62</v>
       </c>
       <c r="B140" s="2">
-        <v>98.4</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>104793.96</v>
+        <v>1619.23</v>
       </c>
       <c r="B141" s="2">
-        <v>98.67</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>82114.23</v>
+        <v>43011.14</v>
       </c>
       <c r="B142" s="2">
         <v>98.6</v>
@@ -2092,79 +2092,79 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>5998.42</v>
+        <v>4253.2299999999996</v>
       </c>
       <c r="B143" s="2">
-        <v>98.35</v>
+        <v>98.25</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>878755.24</v>
+        <v>4231.8599999999997</v>
       </c>
       <c r="B144" s="2">
-        <v>98.8</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>5254.14</v>
+        <v>61064.23</v>
       </c>
       <c r="B145" s="2">
-        <v>98.35</v>
+        <v>98.65</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>667.27</v>
+        <v>1500</v>
       </c>
       <c r="B146" s="2">
-        <v>97.5</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>3695.98</v>
+        <v>10746.62</v>
       </c>
       <c r="B147" s="2">
-        <v>98.1</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>3156.78</v>
+        <v>152840.21</v>
       </c>
       <c r="B148" s="2">
-        <v>98.3</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>31561.31</v>
+        <v>8397.85</v>
       </c>
       <c r="B149" s="2">
-        <v>98.55</v>
+        <v>98.45</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>2972.23</v>
+        <v>31500</v>
       </c>
       <c r="B150" s="2">
-        <v>98.2</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>17850.09</v>
+        <v>563.65</v>
       </c>
       <c r="B151" s="2">
-        <v>98.45</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>1158313.6200000001</v>
+        <v>770000</v>
       </c>
       <c r="B152" s="2">
         <v>98.85</v>
@@ -2172,47 +2172,47 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>2193.81</v>
+        <v>112163.36</v>
       </c>
       <c r="B153" s="2">
-        <v>98</v>
+        <v>98.87</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>105955.86</v>
+        <v>71571.789999999994</v>
       </c>
       <c r="B154" s="2">
-        <v>98.67</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>53154.35</v>
+        <v>450000</v>
       </c>
       <c r="B155" s="2">
-        <v>98.55</v>
+        <v>98.85</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>8623.1200000000008</v>
+        <v>7814025.6799999997</v>
       </c>
       <c r="B156" s="2">
-        <v>98.15</v>
+        <v>99.077500000000001</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>21211.38</v>
+        <v>309219.08</v>
       </c>
       <c r="B157" s="2">
-        <v>98.45</v>
+        <v>98.8</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>51902.04</v>
+        <v>14800.07</v>
       </c>
       <c r="B158" s="2">
         <v>98.6</v>
@@ -2220,39 +2220,39 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>2075.54</v>
+        <v>28706.45</v>
       </c>
       <c r="B159" s="2">
-        <v>98.2</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>42282.05</v>
+        <v>16355.37</v>
       </c>
       <c r="B160" s="2">
-        <v>98.5</v>
+        <v>99.6</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>29612.09</v>
+        <v>16355.37</v>
       </c>
       <c r="B161" s="2">
-        <v>98.5</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>112948.36</v>
+        <v>5413.77</v>
       </c>
       <c r="B162" s="2">
-        <v>98.6</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>70975.009999999995</v>
+        <v>12625.17</v>
       </c>
       <c r="B163" s="2">
         <v>98.6</v>
@@ -2260,79 +2260,79 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>543406.77</v>
+        <v>2346.65</v>
       </c>
       <c r="B164" s="2">
-        <v>98.67</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>168048.51</v>
+        <v>47223.09</v>
       </c>
       <c r="B165" s="2">
-        <v>98.65</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>611.04999999999995</v>
+        <v>20718.060000000001</v>
       </c>
       <c r="B166" s="2">
-        <v>97</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>12927.52</v>
+        <v>5079.47</v>
       </c>
       <c r="B167" s="2">
-        <v>98.5</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>115046.58</v>
+        <v>18211.95</v>
       </c>
       <c r="B168" s="2">
-        <v>98.7</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>403.1</v>
+        <v>1832.53</v>
       </c>
       <c r="B169" s="2">
-        <v>98</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>106081.73</v>
+        <v>353858.67</v>
       </c>
       <c r="B170" s="2">
-        <v>98.65</v>
+        <v>98.8</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>634.02</v>
+        <v>3429.58</v>
       </c>
       <c r="B171" s="2">
-        <v>97.15</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>567.12</v>
+        <v>24269.54</v>
       </c>
       <c r="B172" s="2">
-        <v>97.15</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>54654.75</v>
+        <v>37128.67</v>
       </c>
       <c r="B173" s="2">
         <v>98.5</v>
@@ -2340,15 +2340,15 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>10239.200000000001</v>
+        <v>14854.7</v>
       </c>
       <c r="B174" s="2">
-        <v>98.4</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>44012.18</v>
+        <v>26745.67</v>
       </c>
       <c r="B175" s="2">
         <v>98.5</v>
@@ -2356,7 +2356,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>54645.93</v>
+        <v>22174.91</v>
       </c>
       <c r="B176" s="2">
         <v>98.5</v>
@@ -2364,31 +2364,31 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>570.26</v>
+        <v>14750.87</v>
       </c>
       <c r="B177" s="2">
-        <v>97.5</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>51954.78</v>
+        <v>4232.8599999999997</v>
       </c>
       <c r="B178" s="2">
-        <v>98.5</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>872.02</v>
+        <v>1108.45</v>
       </c>
       <c r="B179" s="2">
-        <v>97.5</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>73786.720000000001</v>
+        <v>15000</v>
       </c>
       <c r="B180" s="2">
         <v>98.5</v>
@@ -2396,380 +2396,699 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>11083.73</v>
+        <v>4377.83</v>
       </c>
       <c r="B181" s="2">
-        <v>98.35</v>
+        <v>98</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>2892.13</v>
+        <v>3586.66</v>
       </c>
       <c r="B182" s="2">
-        <v>98</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>22603.79</v>
+        <v>24084.15</v>
       </c>
       <c r="B183" s="2">
-        <v>98.55</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>1873.02</v>
+        <v>5142.71</v>
       </c>
       <c r="B184" s="2">
-        <v>98</v>
+        <v>98.35</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>2814.13</v>
+        <v>1663.79</v>
       </c>
       <c r="B185" s="2">
-        <v>98</v>
+        <v>98.3</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>26157.119999999999</v>
+        <v>23256.92</v>
       </c>
       <c r="B186" s="2">
-        <v>98.5</v>
+        <v>98.67</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>22490</v>
+        <v>80000</v>
       </c>
       <c r="B187" s="2">
-        <v>98.55</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>38278.15</v>
+        <v>69698.509999999995</v>
       </c>
       <c r="B188" s="2">
-        <v>98.67</v>
+        <v>98.8</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>2000</v>
+        <v>15758.51</v>
       </c>
       <c r="B189" s="2">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>163950.1</v>
+      </c>
+      <c r="B190" s="2">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
+        <v>25500.51</v>
+      </c>
+      <c r="B191" s="2">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
+        <v>14612.18</v>
+      </c>
+      <c r="B192" s="2">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
+        <v>61311.1</v>
+      </c>
+      <c r="B193" s="2">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
+        <v>16522.150000000001</v>
+      </c>
+      <c r="B194" s="2">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
+        <v>40338.76</v>
+      </c>
+      <c r="B195" s="2">
+        <v>98.73</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
+        <v>37022.86</v>
+      </c>
+      <c r="B196" s="2">
+        <v>98.7</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <v>1419.63</v>
+      </c>
+      <c r="B197" s="2">
+        <v>98.25</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
+        <v>9023.66</v>
+      </c>
+      <c r="B198" s="2">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
+        <v>10245.16</v>
+      </c>
+      <c r="B199" s="2">
+        <v>98.55</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
+        <v>70929.53</v>
+      </c>
+      <c r="B200" s="2">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
+        <v>298334.96999999997</v>
+      </c>
+      <c r="B201" s="2">
+        <v>98.82</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
+        <v>59764.85</v>
+      </c>
+      <c r="B202" s="2">
+        <v>98.75</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
+        <v>4213.6899999999996</v>
+      </c>
+      <c r="B203" s="2">
+        <v>98.2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
+        <v>205343.35999999999</v>
+      </c>
+      <c r="B204" s="2">
+        <v>98.9</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
+        <v>1305.8599999999999</v>
+      </c>
+      <c r="B205" s="2">
+        <v>98.25</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
+        <v>427.85</v>
+      </c>
+      <c r="B206" s="2">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
+        <v>1637.21</v>
+      </c>
+      <c r="B207" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
+        <v>14335.62</v>
+      </c>
+      <c r="B208" s="2">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="2">
+        <v>12257.06</v>
+      </c>
+      <c r="B209" s="2">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="2">
+        <v>287464.84999999998</v>
+      </c>
+      <c r="B210" s="2">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
+        <v>709.37</v>
+      </c>
+      <c r="B211" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
+        <v>21914</v>
+      </c>
+      <c r="B212" s="2">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="2">
+        <v>7524.79</v>
+      </c>
+      <c r="B213" s="2">
+        <v>98.2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="2">
+        <v>18801.96</v>
+      </c>
+      <c r="B214" s="2">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="2">
+        <v>127016.36</v>
+      </c>
+      <c r="B215" s="2">
+        <v>98.9</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" s="2">
+        <v>2553.02</v>
+      </c>
+      <c r="B216" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="2">
+        <v>1389.9</v>
+      </c>
+      <c r="B217" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="2">
+        <v>1236.31</v>
+      </c>
+      <c r="B218" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" s="2">
+        <v>38797.410000000003</v>
+      </c>
+      <c r="B219" s="2">
+        <v>98.55</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="2">
+        <v>1864.75</v>
+      </c>
+      <c r="B220" s="2">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
+        <v>2064.9499999999998</v>
+      </c>
+      <c r="B221" s="2">
+        <v>98.3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" s="2">
+        <v>258317.09</v>
+      </c>
+      <c r="B222" s="2">
+        <v>98.75</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="2">
+        <v>1635.31</v>
+      </c>
+      <c r="B223" s="2">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
+        <v>18948.990000000002</v>
+      </c>
+      <c r="B224" s="2">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" s="2">
+        <v>5500</v>
+      </c>
+      <c r="B225" s="2">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" s="2">
+        <v>51685.31</v>
+      </c>
+      <c r="B226" s="2">
+        <v>98.65</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" s="2">
+        <v>5112.18</v>
+      </c>
+      <c r="B227" s="2">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" s="2">
+        <v>725.41</v>
+      </c>
+      <c r="B228" s="2">
+        <v>97.6</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" s="2">
+        <v>8457.14</v>
+      </c>
+      <c r="B229" s="2">
+        <v>98.62</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" s="2">
+        <v>6393.55</v>
+      </c>
+      <c r="B230" s="2">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" s="2">
+        <v>101413.65</v>
+      </c>
+      <c r="B231" s="2">
+        <v>98.7</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" s="2">
+        <v>47119.44</v>
+      </c>
+      <c r="B232" s="2">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" s="2">
+        <v>2410.44</v>
+      </c>
+      <c r="B233" s="2">
+        <v>98.3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" s="2">
+        <v>125.22</v>
+      </c>
+      <c r="B234" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="2">
+        <v>2347.98</v>
+      </c>
+      <c r="B235" s="2">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" s="2">
+        <v>433.85</v>
+      </c>
+      <c r="B236" s="2">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" s="2">
+        <v>869.13</v>
+      </c>
+      <c r="B237" s="2">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" s="2">
+        <v>51682.44</v>
+      </c>
+      <c r="B238" s="2">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" s="2">
+        <v>3000</v>
+      </c>
+      <c r="B239" s="2">
+        <v>98.45</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" s="2">
+        <v>663.12</v>
+      </c>
+      <c r="B240" s="2">
+        <v>98.2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" s="2">
+        <v>2798.58</v>
+      </c>
+      <c r="B241" s="2">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" s="2">
+        <v>2558339.85</v>
+      </c>
+      <c r="B242" s="2">
+        <v>99.02</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" s="2">
+        <v>360.14</v>
+      </c>
+      <c r="B243" s="2">
+        <v>97.05</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" s="2">
+        <v>15728.85</v>
+      </c>
+      <c r="B244" s="2">
+        <v>98.7</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" s="2">
+        <v>1358.01</v>
+      </c>
+      <c r="B245" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" s="2">
+        <v>126588.06</v>
+      </c>
+      <c r="B246" s="2">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" s="2">
+        <v>169450.53</v>
+      </c>
+      <c r="B247" s="2">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" s="2">
+        <v>163.05000000000001</v>
+      </c>
+      <c r="B248" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" s="2">
+        <v>15148.57</v>
+      </c>
+      <c r="B249" s="2">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="2">
+        <v>39938.300000000003</v>
+      </c>
+      <c r="B250" s="2">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="2">
+        <v>26802.15</v>
+      </c>
+      <c r="B251" s="2">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="2">
+        <v>603.38</v>
+      </c>
+      <c r="B252" s="2">
+        <v>97.75</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="2">
+        <v>23493.85</v>
+      </c>
+      <c r="B253" s="2">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" s="2">
+        <v>143496.5</v>
+      </c>
+      <c r="B254" s="2">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" s="2">
+        <v>381526.73</v>
+      </c>
+      <c r="B255" s="2">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" s="2">
+        <v>957881</v>
+      </c>
+      <c r="B256" s="2">
+        <v>98.93</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" s="2">
+        <v>501534.03</v>
+      </c>
+      <c r="B257" s="2">
+        <v>98.83</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" s="2">
+        <v>142870.43</v>
+      </c>
+      <c r="B258" s="2">
+        <v>98.82</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" s="2">
+        <v>167699.91</v>
+      </c>
+      <c r="B259" s="2">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" s="2">
+        <v>34954.300000000003</v>
+      </c>
+      <c r="B260" s="3">
+        <v>98.65</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" s="2">
+        <v>4567.87</v>
+      </c>
+      <c r="B261" s="1">
+        <v>98.55</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" s="2">
+        <v>14950.12</v>
+      </c>
+      <c r="B262" s="1">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" s="2">
+        <v>252852.9</v>
+      </c>
+      <c r="B263" s="1">
+        <v>98.75</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B264" s="1">
+        <v>98.45</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" s="2">
+        <v>507</v>
+      </c>
+      <c r="B265" s="1">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" s="2">
+        <v>1239.55</v>
+      </c>
+      <c r="B266" s="1">
         <v>98.1</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="2"/>
-      <c r="B190" s="2"/>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="2"/>
-      <c r="B191" s="2"/>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="2"/>
-      <c r="B192" s="2"/>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="2"/>
-      <c r="B193" s="2"/>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="2"/>
-      <c r="B194" s="2"/>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="2"/>
-      <c r="B195" s="2"/>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="2"/>
-      <c r="B196" s="2"/>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="2"/>
-      <c r="B197" s="2"/>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="2"/>
-      <c r="B198" s="2"/>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="2"/>
-      <c r="B199" s="2"/>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="2"/>
-      <c r="B200" s="2"/>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="2"/>
-      <c r="B201" s="2"/>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="2"/>
-      <c r="B202" s="2"/>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="2"/>
-      <c r="B203" s="2"/>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="2"/>
-      <c r="B204" s="2"/>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="2"/>
-      <c r="B205" s="2"/>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="2"/>
-      <c r="B206" s="2"/>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="2"/>
-      <c r="B207" s="2"/>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="2"/>
-      <c r="B208" s="2"/>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="2"/>
-      <c r="B209" s="2"/>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="2"/>
-      <c r="B210" s="2"/>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="2"/>
-      <c r="B211" s="2"/>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="2"/>
-      <c r="B212" s="2"/>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="2"/>
-      <c r="B213" s="2"/>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="2"/>
-      <c r="B214" s="2"/>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="2"/>
-      <c r="B215" s="2"/>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="2"/>
-      <c r="B216" s="2"/>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="2"/>
-      <c r="B217" s="2"/>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="2"/>
-      <c r="B218" s="2"/>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="2"/>
-      <c r="B219" s="2"/>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="2"/>
-      <c r="B220" s="2"/>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="2"/>
-      <c r="B221" s="2"/>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="2"/>
-      <c r="B222" s="2"/>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="2"/>
-      <c r="B223" s="2"/>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="2"/>
-      <c r="B224" s="2"/>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="2"/>
-      <c r="B225" s="2"/>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="2"/>
-      <c r="B226" s="2"/>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="2"/>
-      <c r="B227" s="2"/>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="2"/>
-      <c r="B228" s="2"/>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" s="2"/>
-      <c r="B229" s="2"/>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" s="2"/>
-      <c r="B230" s="2"/>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="2"/>
-      <c r="B231" s="2"/>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="2"/>
-      <c r="B232" s="2"/>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="2"/>
-      <c r="B233" s="2"/>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="2"/>
-      <c r="B234" s="2"/>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="2"/>
-      <c r="B235" s="2"/>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="2"/>
-      <c r="B236" s="2"/>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="2"/>
-      <c r="B237" s="2"/>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="2"/>
-      <c r="B238" s="2"/>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="2"/>
-      <c r="B239" s="2"/>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="2"/>
-      <c r="B240" s="2"/>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="2"/>
-      <c r="B241" s="2"/>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="2"/>
-      <c r="B242" s="2"/>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="2"/>
-      <c r="B243" s="2"/>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="2"/>
-      <c r="B244" s="2"/>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="2"/>
-      <c r="B245" s="2"/>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="2"/>
-      <c r="B246" s="2"/>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="2"/>
-      <c r="B247" s="2"/>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="2"/>
-      <c r="B248" s="2"/>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="2"/>
-      <c r="B249" s="2"/>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="2"/>
-      <c r="B250" s="2"/>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="2"/>
-      <c r="B251" s="2"/>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="2"/>
-      <c r="B252" s="2"/>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="2"/>
-      <c r="B253" s="2"/>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="2"/>
-      <c r="B254" s="2"/>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="2"/>
-      <c r="B255" s="2"/>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="2"/>
-      <c r="B256" s="2"/>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="2"/>
-      <c r="B257" s="2"/>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="2"/>
-      <c r="B258" s="2"/>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="2"/>
-      <c r="B259" s="2"/>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="2"/>
-      <c r="B260" s="3"/>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="2"/>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="2"/>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="2"/>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="2"/>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="2"/>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="2"/>
-    </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="2"/>
+      <c r="A267" s="2">
+        <v>1903.61</v>
+      </c>
+      <c r="B267" s="1">
+        <v>98.3</v>
+      </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="2"/>

</xml_diff>